<commit_message>
update MC02 substitutions file
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -88,7 +88,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.15
+          <t>vert = -4.65
 pitch = 3.5
 lateral = -1
 yaw = 0.150</t>
@@ -104,7 +104,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -8.276
+          <t>vert = -6.583
 pitch = -5.0</t>
         </r>
       </text>
@@ -11146,11 +11146,11 @@
   <dimension ref="1:60"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="J47" activeCellId="0" sqref="J47"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="H58" activeCellId="0" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -12770,10 +12770,10 @@
         <v>-57542</v>
       </c>
       <c r="G37" s="39" t="n">
-        <v>-6.4041</v>
+        <v>-6.9038</v>
       </c>
       <c r="H37" s="19" t="n">
-        <v>-57542</v>
+        <v>-62538</v>
       </c>
       <c r="I37" s="39" t="n">
         <v>-6.4041</v>
@@ -12832,10 +12832,10 @@
         <v>-27846</v>
       </c>
       <c r="G38" s="30" t="n">
-        <v>-1.8946</v>
+        <v>-2.3945</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>-27846</v>
+        <v>-32846</v>
       </c>
       <c r="I38" s="30" t="n">
         <v>-1.8946</v>
@@ -12880,10 +12880,10 @@
         <v>-21956</v>
       </c>
       <c r="G39" s="30" t="n">
-        <v>-1.8955</v>
+        <v>-2.3951</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>-21956</v>
+        <v>-26950</v>
       </c>
       <c r="I39" s="30" t="n">
         <v>-1.8955</v>
@@ -13088,10 +13088,10 @@
         <v>3208</v>
       </c>
       <c r="G43" s="40" t="n">
-        <v>-6.608</v>
+        <v>-4.9154</v>
       </c>
       <c r="H43" s="24" t="n">
-        <v>-47880</v>
+        <v>-30953</v>
       </c>
       <c r="I43" s="0" t="n">
         <v>-6.08242</v>
@@ -13150,10 +13150,10 @@
         <v>-11313</v>
       </c>
       <c r="G44" s="28" t="n">
-        <v>-9.943</v>
+        <v>-8.2511</v>
       </c>
       <c r="H44" s="29" t="n">
-        <v>-95730</v>
+        <v>-78810</v>
       </c>
       <c r="I44" s="0" t="n">
         <v>-8.41762</v>
@@ -13198,10 +13198,10 @@
         <v>-12617</v>
       </c>
       <c r="G45" s="28" t="n">
-        <v>-9.943</v>
+        <v>-8.2512</v>
       </c>
       <c r="H45" s="29" t="n">
-        <v>-97030</v>
+        <v>-80111</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>-8.41752</v>
@@ -13358,10 +13358,10 @@
         <v>288431</v>
       </c>
       <c r="G48" s="50" t="n">
-        <v>-59.0037</v>
+        <v>-66.743</v>
       </c>
       <c r="H48" s="51" t="n">
-        <v>-631605</v>
+        <v>-708892</v>
       </c>
       <c r="I48" s="49" t="n">
         <v>-48.1824</v>
@@ -13706,10 +13706,10 @@
         <v>459199</v>
       </c>
       <c r="G54" s="53" t="n">
-        <v>-42.6</v>
+        <v>-59.5913</v>
       </c>
       <c r="H54" s="54" t="n">
-        <v>-461870</v>
+        <v>-631720</v>
       </c>
       <c r="I54" s="52" t="n">
         <v>-17.25</v>
@@ -13832,16 +13832,16 @@
         <v>9990244</v>
       </c>
       <c r="G56" s="55" t="n">
-        <v>30.5</v>
+        <v>24.4104</v>
       </c>
       <c r="H56" s="22" t="n">
-        <v>4917073</v>
+        <v>4600216</v>
       </c>
       <c r="I56" s="55" t="n">
-        <v>59.25</v>
+        <v>50.9301</v>
       </c>
       <c r="J56" s="24" t="n">
-        <v>6432521</v>
+        <v>5980102</v>
       </c>
       <c r="K56" s="55" t="n">
         <v>126</v>
@@ -13880,16 +13880,16 @@
         <v>7544716</v>
       </c>
       <c r="G57" s="56" t="n">
-        <v>21</v>
+        <v>12.81</v>
       </c>
       <c r="H57" s="29" t="n">
-        <v>780488</v>
+        <v>1551088</v>
       </c>
       <c r="I57" s="56" t="n">
-        <v>51.5</v>
+        <v>42.81</v>
       </c>
       <c r="J57" s="29" t="n">
-        <v>2367480</v>
+        <v>3112063</v>
       </c>
       <c r="K57" s="56" t="n">
         <v>126</v>
@@ -13928,16 +13928,16 @@
         <v>6347968</v>
       </c>
       <c r="G58" s="56" t="n">
-        <v>21</v>
+        <v>12.81</v>
       </c>
       <c r="H58" s="29" t="n">
-        <v>1977236</v>
+        <v>354340</v>
       </c>
       <c r="I58" s="56" t="n">
-        <v>51.5</v>
+        <v>42.81</v>
       </c>
       <c r="J58" s="54" t="n">
-        <v>3564228</v>
+        <v>1915315</v>
       </c>
       <c r="K58" s="56" t="n">
         <v>126</v>

</xml_diff>

<commit_message>
look up table update
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,8 +48,8 @@
           </rPr>
           <t>vert = -4.15
 pitch = 3.225
-lateral = -0.4
-yaw = 0.124</t>
+lateral = 0.0
+yaw = 0.053</t>
         </r>
       </text>
     </comment>
@@ -90,8 +90,8 @@
           </rPr>
           <t>vert = -4.15
 pitch = 3.225
-lateral = -0.4
-yaw = 0.124</t>
+lateral = 0.0
+yaw = 0.053</t>
         </r>
       </text>
     </comment>
@@ -133,8 +133,8 @@
           </rPr>
           <t>vert = -4.15
 pitch = 3.225
-lateral = -0.4
-yaw = 0.124</t>
+lateral = 0.0
+yaw = 0.053</t>
         </r>
       </text>
     </comment>
@@ -11142,12 +11142,12 @@
   </sheetPr>
   <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
-      <selection pane="bottomRight" activeCell="I42" activeCellId="0" sqref="I42"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="I37" activeCellId="0" sqref="I37:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -12919,22 +12919,22 @@
         <v>134</v>
       </c>
       <c r="E40" s="30" t="n">
-        <v>-0.415799999</v>
+        <v>-0.034</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-16348</v>
+        <v>-12534</v>
       </c>
       <c r="G40" s="30" t="n">
-        <v>-0.415799999</v>
+        <v>-0.034</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>-16348</v>
+        <v>-12534</v>
       </c>
       <c r="I40" s="30" t="n">
-        <v>-0.415799999</v>
+        <v>-0.034</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>-16348</v>
+        <v>-12534</v>
       </c>
       <c r="K40" s="30" t="n">
         <v>-0.415799999</v>
@@ -12967,22 +12967,22 @@
         <v>137</v>
       </c>
       <c r="E41" s="30" t="n">
-        <v>-0.3847</v>
+        <v>0.034</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-31347</v>
+        <v>-27156</v>
       </c>
       <c r="G41" s="30" t="n">
-        <v>-0.3847</v>
+        <v>0.034</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>-31347</v>
+        <v>-27156</v>
       </c>
       <c r="I41" s="30" t="n">
-        <v>-0.3847</v>
+        <v>0.034</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>-31347</v>
+        <v>-27156</v>
       </c>
       <c r="K41" s="30" t="n">
         <v>-0.3847</v>
@@ -14093,8 +14093,8 @@
   </sheetPr>
   <dimension ref="1:30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I37:J41 C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15643,7 +15643,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="1" sqref="I37:J41 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15784,7 +15784,7 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I37:J41 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21856,7 +21856,7 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I37:J41 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
slit positions ofr modes D and E
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11143,11 +11143,11 @@
   <dimension ref="1:60"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="I37" activeCellId="0" sqref="I37:J41"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="N52" activeCellId="0" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13431,16 +13431,16 @@
         <v>-86672</v>
       </c>
       <c r="K49" s="40" t="n">
-        <v>-2.6001</v>
+        <v>-4.6002</v>
       </c>
       <c r="L49" s="24" t="n">
-        <v>-34670</v>
+        <v>-54671</v>
       </c>
       <c r="M49" s="40" t="n">
-        <v>-2.6001</v>
+        <v>-4.6002</v>
       </c>
       <c r="N49" s="24" t="n">
-        <v>-34670</v>
+        <v>-54671</v>
       </c>
       <c r="O49" s="40" t="n">
         <v>-2.6001</v>
@@ -13493,16 +13493,16 @@
         <v>40742</v>
       </c>
       <c r="K50" s="28" t="n">
-        <v>-2.4001</v>
+        <v>-0.4001</v>
       </c>
       <c r="L50" s="29" t="n">
-        <v>15751</v>
+        <v>35751</v>
       </c>
       <c r="M50" s="28" t="n">
-        <v>-2.4001</v>
+        <v>-0.4001</v>
       </c>
       <c r="N50" s="29" t="n">
-        <v>15751</v>
+        <v>35751</v>
       </c>
       <c r="O50" s="28" t="n">
         <v>-2.4001</v>
@@ -13541,16 +13541,16 @@
         <v>58500</v>
       </c>
       <c r="K51" s="30" t="n">
-        <v>3.3045</v>
+        <v>4.4571</v>
       </c>
       <c r="L51" s="29" t="n">
-        <v>23505</v>
+        <v>35030</v>
       </c>
       <c r="M51" s="30" t="n">
-        <v>3.3045</v>
+        <v>4.4571</v>
       </c>
       <c r="N51" s="29" t="n">
-        <v>23505</v>
+        <v>35030</v>
       </c>
       <c r="O51" s="30" t="n">
         <v>3.3045</v>
@@ -13589,16 +13589,16 @@
         <v>-34835</v>
       </c>
       <c r="K52" s="34" t="n">
-        <v>-2.5001</v>
+        <v>0.6004</v>
       </c>
       <c r="L52" s="42" t="n">
-        <v>1166</v>
+        <v>32171</v>
       </c>
       <c r="M52" s="34" t="n">
-        <v>-2.5001</v>
+        <v>0.6004</v>
       </c>
       <c r="N52" s="42" t="n">
-        <v>1166</v>
+        <v>32171</v>
       </c>
       <c r="O52" s="34" t="n">
         <v>-1.7001</v>
@@ -14094,7 +14094,7 @@
   <dimension ref="1:30"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="1" sqref="I37:J41 C17"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15643,7 +15643,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E4" activeCellId="1" sqref="I37:J41 E4"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15784,7 +15784,7 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="I37:J41 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -21856,7 +21856,7 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="I37:J41 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
achieved energy in scan, work on dm3 slits
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11143,11 +11143,11 @@
   <dimension ref="1:60"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
-      <selection pane="bottomRight" activeCell="N52" activeCellId="0" sqref="N52"/>
+      <selection pane="bottomRight" activeCell="J49" activeCellId="0" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13413,40 +13413,40 @@
         <v>164</v>
       </c>
       <c r="E49" s="39" t="n">
-        <v>-8.2496</v>
+        <v>5</v>
       </c>
       <c r="F49" s="19" t="n">
-        <v>-91165</v>
+        <v>-49670</v>
       </c>
       <c r="G49" s="40" t="n">
-        <v>-7.7001</v>
+        <v>5</v>
       </c>
       <c r="H49" s="24" t="n">
-        <v>-85670</v>
+        <v>-49670</v>
       </c>
       <c r="I49" s="39" t="n">
-        <v>-7.8003</v>
+        <v>5</v>
       </c>
       <c r="J49" s="19" t="n">
-        <v>-86672</v>
+        <v>-49670</v>
       </c>
       <c r="K49" s="40" t="n">
-        <v>-4.6002</v>
+        <v>5</v>
       </c>
       <c r="L49" s="24" t="n">
-        <v>-54671</v>
+        <v>-49670</v>
       </c>
       <c r="M49" s="40" t="n">
-        <v>-4.6002</v>
+        <v>5</v>
       </c>
       <c r="N49" s="24" t="n">
-        <v>-54671</v>
+        <v>-49670</v>
       </c>
       <c r="O49" s="40" t="n">
-        <v>-2.6001</v>
+        <v>5</v>
       </c>
       <c r="P49" s="24" t="n">
-        <v>-34670</v>
+        <v>-49670</v>
       </c>
       <c r="ALW49" s="0"/>
       <c r="ALX49" s="0"/>
@@ -13475,40 +13475,40 @@
         <v>167</v>
       </c>
       <c r="E50" s="30" t="n">
-        <v>0.2395</v>
+        <v>-5</v>
       </c>
       <c r="F50" s="0" t="n">
-        <v>42146</v>
+        <v>30752</v>
       </c>
       <c r="G50" s="28" t="n">
-        <v>0.0908</v>
+        <v>-5</v>
       </c>
       <c r="H50" s="29" t="n">
-        <v>40660</v>
+        <v>30752</v>
       </c>
       <c r="I50" s="30" t="n">
-        <v>0.099</v>
+        <v>-5</v>
       </c>
       <c r="J50" s="0" t="n">
-        <v>40742</v>
+        <v>30752</v>
       </c>
       <c r="K50" s="28" t="n">
-        <v>-0.4001</v>
+        <v>-5</v>
       </c>
       <c r="L50" s="29" t="n">
-        <v>35751</v>
+        <v>30752</v>
       </c>
       <c r="M50" s="28" t="n">
-        <v>-0.4001</v>
+        <v>-5</v>
       </c>
       <c r="N50" s="29" t="n">
-        <v>35751</v>
+        <v>30752</v>
       </c>
       <c r="O50" s="28" t="n">
-        <v>-2.4001</v>
+        <v>-5</v>
       </c>
       <c r="P50" s="29" t="n">
-        <v>15751</v>
+        <v>30752</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13523,40 +13523,40 @@
         <v>170</v>
       </c>
       <c r="E51" s="30" t="n">
-        <v>6.8</v>
+        <v>1</v>
       </c>
       <c r="F51" s="0" t="n">
-        <v>58500</v>
+        <v>26041</v>
       </c>
       <c r="G51" s="30" t="n">
-        <v>6.8</v>
+        <v>1</v>
       </c>
       <c r="H51" s="0" t="n">
-        <v>58500</v>
+        <v>26041</v>
       </c>
       <c r="I51" s="30" t="n">
-        <v>6.8</v>
+        <v>1</v>
       </c>
       <c r="J51" s="0" t="n">
-        <v>58500</v>
+        <v>26041</v>
       </c>
       <c r="K51" s="30" t="n">
-        <v>4.4571</v>
+        <v>1</v>
       </c>
       <c r="L51" s="29" t="n">
-        <v>35030</v>
+        <v>26041</v>
       </c>
       <c r="M51" s="30" t="n">
-        <v>4.4571</v>
+        <v>1</v>
       </c>
       <c r="N51" s="29" t="n">
-        <v>35030</v>
+        <v>26041</v>
       </c>
       <c r="O51" s="30" t="n">
-        <v>3.3045</v>
+        <v>1</v>
       </c>
       <c r="P51" s="29" t="n">
-        <v>23505</v>
+        <v>26041</v>
       </c>
     </row>
     <row r="52" s="32" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13571,40 +13571,40 @@
         <v>173</v>
       </c>
       <c r="E52" s="34" t="n">
-        <v>-6.1003</v>
+        <v>-1</v>
       </c>
       <c r="F52" s="32" t="n">
-        <v>-34835</v>
+        <v>-1342</v>
       </c>
       <c r="G52" s="34" t="n">
-        <v>-6.1003</v>
+        <v>-1</v>
       </c>
       <c r="H52" s="32" t="n">
-        <v>-34835</v>
+        <v>-1342</v>
       </c>
       <c r="I52" s="34" t="n">
-        <v>-6.1003</v>
+        <v>-1</v>
       </c>
       <c r="J52" s="32" t="n">
-        <v>-34835</v>
+        <v>-1342</v>
       </c>
       <c r="K52" s="34" t="n">
-        <v>0.6004</v>
+        <v>-1</v>
       </c>
       <c r="L52" s="42" t="n">
-        <v>32171</v>
+        <v>-1342</v>
       </c>
       <c r="M52" s="34" t="n">
-        <v>0.6004</v>
+        <v>-1</v>
       </c>
       <c r="N52" s="42" t="n">
-        <v>32171</v>
+        <v>-1342</v>
       </c>
       <c r="O52" s="34" t="n">
-        <v>-1.7001</v>
+        <v>-1</v>
       </c>
       <c r="P52" s="32" t="n">
-        <v>9165</v>
+        <v>-1342</v>
       </c>
       <c r="ALW52" s="0"/>
       <c r="ALX52" s="0"/>

</xml_diff>

<commit_message>
cheatsheet + mirror config
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -10438,7 +10438,7 @@
     <numFmt numFmtId="169" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="170" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -10564,11 +10564,6 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -10813,7 +10808,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11042,10 +11037,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11134,7 +11125,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11162,7 +11153,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11290,7 +11281,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11298,7 +11289,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="22" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11397,12 +11388,12 @@
   </sheetPr>
   <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="I31" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E31" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="O55" activeCellId="0" sqref="O55"/>
+      <selection pane="bottomRight" activeCell="F39" activeCellId="0" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13016,10 +13007,10 @@
         <v>125</v>
       </c>
       <c r="E37" s="39" t="n">
-        <v>-6.2262</v>
+        <v>-6.60298</v>
       </c>
       <c r="F37" s="19" t="n">
-        <v>-55761</v>
+        <v>-59529</v>
       </c>
       <c r="G37" s="39" t="n">
         <v>-6.2262</v>
@@ -13078,10 +13069,10 @@
         <v>128</v>
       </c>
       <c r="E38" s="30" t="n">
-        <v>-2.0722</v>
+        <v>-2.09497</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>-29624</v>
+        <v>-29850</v>
       </c>
       <c r="G38" s="30" t="n">
         <v>-2.0722</v>
@@ -13126,10 +13117,10 @@
         <v>131</v>
       </c>
       <c r="E39" s="30" t="n">
-        <v>-2.0722</v>
+        <v>-2.09497</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>-23721</v>
+        <v>-23949</v>
       </c>
       <c r="G39" s="30" t="n">
         <v>-2.0722</v>
@@ -13952,10 +13943,10 @@
         <v>180</v>
       </c>
       <c r="E54" s="52" t="n">
-        <v>44.5433</v>
+        <v>51.32</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>409617</v>
+        <v>477354</v>
       </c>
       <c r="G54" s="53" t="n">
         <v>-52.1921</v>
@@ -14078,10 +14069,10 @@
         <v>187</v>
       </c>
       <c r="E56" s="55" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F56" s="24" t="n">
-        <v>9990244</v>
+        <v>10406504</v>
       </c>
       <c r="G56" s="55" t="n">
         <v>24.4104</v>
@@ -14126,10 +14117,10 @@
         <v>190</v>
       </c>
       <c r="E57" s="56" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F57" s="29" t="n">
-        <v>7544716</v>
+        <v>7960975</v>
       </c>
       <c r="G57" s="56" t="n">
         <v>12.81</v>
@@ -14174,10 +14165,10 @@
         <v>193</v>
       </c>
       <c r="E58" s="56" t="n">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="F58" s="54" t="n">
-        <v>6347968</v>
+        <v>6764228</v>
       </c>
       <c r="G58" s="56" t="n">
         <v>12.81</v>
@@ -14206,7 +14197,7 @@
       <c r="O58" s="56" t="n">
         <v>100.43</v>
       </c>
-      <c r="P58" s="57" t="n">
+      <c r="P58" s="27" t="n">
         <v>4913439</v>
       </c>
     </row>
@@ -14269,37 +14260,37 @@
       <c r="D60" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="E60" s="58" t="n">
+      <c r="E60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="F60" s="44" t="n">
         <v>130000</v>
       </c>
-      <c r="G60" s="58" t="n">
+      <c r="G60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="H60" s="44" t="n">
         <v>130000</v>
       </c>
-      <c r="I60" s="58" t="n">
+      <c r="I60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="J60" s="44" t="n">
         <v>130000</v>
       </c>
-      <c r="K60" s="58" t="n">
+      <c r="K60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="L60" s="44" t="n">
         <v>130000</v>
       </c>
-      <c r="M60" s="58" t="n">
+      <c r="M60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="N60" s="44" t="n">
         <v>130000</v>
       </c>
-      <c r="O60" s="58" t="n">
+      <c r="O60" s="57" t="n">
         <v>16.9</v>
       </c>
       <c r="P60" s="44" t="n">
@@ -14357,34 +14348,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="59" width="3.0969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="59" width="13.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="59" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="58" width="3.0969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="58" width="13.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="58" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59"/>
+    <row r="1" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="58"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="AMJ1" s="59"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="AMJ1" s="58"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="60" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -15405,168 +15396,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="66" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="62"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="64" t="s">
+    <row r="3" s="65" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>203</v>
       </c>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="AMJ3" s="62"/>
-    </row>
-    <row r="4" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="59"/>
-      <c r="B4" s="63" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="AMJ3" s="61"/>
+    </row>
+    <row r="4" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="58"/>
+      <c r="B4" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59" t="n">
+      <c r="C4" s="58"/>
+      <c r="D4" s="58" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="67" t="n">
+      <c r="E4" s="66" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="AMJ4" s="59"/>
-    </row>
-    <row r="5" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="59"/>
-      <c r="B5" s="63" t="s">
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="AMJ4" s="58"/>
+    </row>
+    <row r="5" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="58"/>
+      <c r="B5" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="58" t="s">
         <v>206</v>
       </c>
-      <c r="D5" s="59" t="n">
+      <c r="D5" s="58" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="AMJ5" s="59"/>
-    </row>
-    <row r="6" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="59"/>
-      <c r="B6" s="63" t="s">
+      <c r="E5" s="66"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="AMJ5" s="58"/>
+    </row>
+    <row r="6" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="58"/>
+      <c r="B6" s="62" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="D6" s="59" t="n">
+      <c r="D6" s="58" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="67"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="AMJ6" s="59"/>
-    </row>
-    <row r="7" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="59"/>
-      <c r="B7" s="63" t="s">
+      <c r="E6" s="66"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="58"/>
+      <c r="AMJ6" s="58"/>
+    </row>
+    <row r="7" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="58"/>
+      <c r="B7" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D7" s="59" t="n">
+      <c r="D7" s="58" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="AMJ7" s="59"/>
-    </row>
-    <row r="8" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="59"/>
-      <c r="B8" s="63" t="s">
+      <c r="E7" s="66"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="AMJ7" s="58"/>
+    </row>
+    <row r="8" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="58"/>
+      <c r="B8" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="C8" s="59" t="s">
+      <c r="C8" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="D8" s="59" t="n">
+      <c r="D8" s="58" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="67"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="AMJ8" s="59"/>
-    </row>
-    <row r="9" s="60" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="59"/>
-      <c r="B9" s="63" t="s">
+      <c r="E8" s="66"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="AMJ8" s="58"/>
+    </row>
+    <row r="9" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="58"/>
+      <c r="B9" s="62" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59" t="n">
+      <c r="C9" s="58"/>
+      <c r="D9" s="58" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="67"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="AMJ9" s="59"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
+      <c r="L9" s="58"/>
+      <c r="AMJ9" s="58"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="67" t="s">
         <v>214</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69" t="n">
+      <c r="C10" s="68"/>
+      <c r="D10" s="68" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="70"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="71"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -15575,8 +15566,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -15585,82 +15576,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="72" t="s">
         <v>215</v>
       </c>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="74" t="s">
+      <c r="B14" s="73" t="s">
         <v>216</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="74" t="s">
         <v>217</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="67"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="62" t="s">
         <v>204</v>
       </c>
-      <c r="C15" s="59" t="n">
+      <c r="C15" s="58" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="67"/>
+      <c r="E15" s="66"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="62" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="76" t="n">
+      <c r="C16" s="75" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="67"/>
+      <c r="E16" s="66"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="62" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="59" t="n">
+      <c r="C17" s="58" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="67"/>
+      <c r="E17" s="66"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="67" t="s">
         <v>220</v>
       </c>
-      <c r="C18" s="69" t="n">
+      <c r="C18" s="68" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="69"/>
-      <c r="E18" s="70"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="69"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -15687,188 +15678,188 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="73" t="s">
+      <c r="B21" s="72" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
-      <c r="H21" s="73"/>
-      <c r="I21" s="73"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="77" t="s">
+      <c r="B22" s="76" t="s">
         <v>221</v>
       </c>
-      <c r="C22" s="77"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="71" t="s">
+      <c r="C22" s="76"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="70" t="s">
         <v>222</v>
       </c>
-      <c r="F22" s="71"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="78" t="s">
+      <c r="F22" s="70"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="77" t="s">
         <v>223</v>
       </c>
-      <c r="I22" s="78"/>
+      <c r="I22" s="77"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="73" t="s">
         <v>224</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="74" t="s">
         <v>217</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="59" t="s">
         <v>224</v>
       </c>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="74" t="s">
         <v>217</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="60" t="s">
+      <c r="H23" s="59" t="s">
         <v>225</v>
       </c>
-      <c r="I23" s="79" t="s">
+      <c r="I23" s="78" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="63" t="s">
+      <c r="B24" s="62" t="s">
         <v>226</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="58" t="s">
         <v>226</v>
       </c>
-      <c r="F24" s="59" t="n">
+      <c r="F24" s="58" t="n">
         <v>25.5</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="59" t="s">
+      <c r="H24" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="I24" s="67" t="n">
+      <c r="I24" s="66" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="63" t="s">
+      <c r="B25" s="62" t="s">
         <v>228</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="59" t="s">
+      <c r="E25" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="F25" s="59" t="n">
+      <c r="F25" s="58" t="n">
         <v>-42.6</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="I25" s="67" t="n">
+      <c r="I25" s="66" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="63" t="s">
+      <c r="B26" s="62" t="s">
         <v>230</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="F26" s="59" t="n">
+      <c r="F26" s="58" t="n">
         <v>-17.25</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="59" t="s">
+      <c r="H26" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="I26" s="67" t="n">
+      <c r="I26" s="66" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="62" t="s">
         <v>232</v>
       </c>
-      <c r="C27" s="59" t="n">
+      <c r="C27" s="58" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="F27" s="59" t="n">
+      <c r="F27" s="58" t="n">
         <v>46.1092</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="67"/>
+      <c r="I27" s="66"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="63" t="s">
+      <c r="B28" s="62" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="59" t="n">
+      <c r="C28" s="58" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="59" t="s">
+      <c r="E28" s="58" t="s">
         <v>233</v>
       </c>
-      <c r="F28" s="59" t="n">
+      <c r="F28" s="58" t="n">
         <v>46.1092</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="67"/>
+      <c r="I28" s="66"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="63" t="s">
+      <c r="B29" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C29" s="59" t="n">
+      <c r="C29" s="58" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="59" t="s">
+      <c r="E29" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="F29" s="59" t="n">
+      <c r="F29" s="58" t="n">
         <v>19.5956</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="67"/>
+      <c r="I29" s="66"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="67" t="s">
         <v>227</v>
       </c>
-      <c r="C30" s="69" t="n">
+      <c r="C30" s="68" t="n">
         <v>55</v>
       </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="70"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -15926,14 +15917,14 @@
       <c r="D1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="79" t="s">
         <v>235</v>
       </c>
-      <c r="F1" s="80"/>
-      <c r="G1" s="81" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="80" t="s">
         <v>236</v>
       </c>
-      <c r="H1" s="81"/>
+      <c r="H1" s="80"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
@@ -15951,7 +15942,7 @@
       <c r="F2" s="0" t="n">
         <v>-5276</v>
       </c>
-      <c r="G2" s="82" t="n">
+      <c r="G2" s="81" t="n">
         <v>2.33113</v>
       </c>
       <c r="H2" s="29" t="n">
@@ -15959,25 +15950,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="83" t="s">
         <v>237</v>
       </c>
-      <c r="E3" s="84" t="n">
+      <c r="E3" s="83" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="84" t="n">
+      <c r="F3" s="83" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="85" t="n">
+      <c r="G3" s="84" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="86" t="n">
+      <c r="H3" s="85" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -15997,7 +15988,7 @@
       <c r="F4" s="0" t="n">
         <v>-38578</v>
       </c>
-      <c r="G4" s="82" t="n">
+      <c r="G4" s="81" t="n">
         <v>-23.8594</v>
       </c>
       <c r="H4" s="29" t="n">
@@ -16020,7 +16011,7 @@
       <c r="F5" s="0" t="n">
         <v>-354999</v>
       </c>
-      <c r="G5" s="82" t="n">
+      <c r="G5" s="81" t="n">
         <v>29</v>
       </c>
       <c r="H5" s="29" t="n">
@@ -16040,11 +16031,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="87" t="s">
+      <c r="I6" s="86" t="s">
         <v>240</v>
       </c>
-      <c r="J6" s="87"/>
-      <c r="K6" s="87"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -16056,9 +16047,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16084,8 +16075,8 @@
   </sheetPr>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -16100,26 +16091,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="88"/>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="90" t="s">
+      <c r="A1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="89" t="s">
         <v>242</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="91" t="s">
+      <c r="G1" s="90" t="s">
         <v>243</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="91" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="93"/>
-      <c r="D2" s="94" t="s">
+      <c r="A2" s="92"/>
+      <c r="D2" s="93" t="s">
         <v>245</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -16128,93 +16119,93 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="95"/>
+      <c r="G2" s="94"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>246</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="94" t="s">
+      <c r="D3" s="93" t="s">
         <v>247</v>
       </c>
-      <c r="E3" s="97" t="n">
+      <c r="E3" s="96" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="98" t="n">
+      <c r="F3" s="97" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="99" t="n">
+      <c r="G3" s="98" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>19.89</v>
       </c>
-      <c r="H3" s="100" t="n">
+      <c r="H3" s="99" t="n">
         <f aca="false">G3-F3</f>
         <v>0.786881018291666</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="95" t="s">
         <v>248</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="E4" s="98" t="n">
+      <c r="E4" s="97" t="n">
         <f aca="false">'Modes A-F'!K56</f>
         <v>132</v>
       </c>
-      <c r="F4" s="98" t="n">
+      <c r="F4" s="97" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
         <v>103.088913266688</v>
       </c>
-      <c r="G4" s="99" t="n">
+      <c r="G4" s="98" t="n">
         <f aca="false">'Modes A-F'!O56</f>
         <v>103.91</v>
       </c>
-      <c r="H4" s="100" t="n">
+      <c r="H4" s="99" t="n">
         <f aca="false">G4-F4</f>
         <v>0.821086733312242</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="102" t="n">
+      <c r="B5" s="101" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="102"/>
-      <c r="D5" s="103" t="s">
+      <c r="C5" s="101"/>
+      <c r="D5" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="E5" s="104" t="n">
+      <c r="E5" s="103" t="n">
         <f aca="false">'Modes A-F'!K57</f>
         <v>132</v>
       </c>
-      <c r="F5" s="104" t="n">
+      <c r="F5" s="103" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
         <v>99.6239028716503</v>
       </c>
-      <c r="G5" s="105" t="n">
+      <c r="G5" s="104" t="n">
         <f aca="false">'Modes A-F'!O57</f>
         <v>100.43</v>
       </c>
-      <c r="H5" s="100" t="n">
+      <c r="H5" s="99" t="n">
         <f aca="false">G5-F5</f>
         <v>0.806097128349677</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="100" t="n">
+      <c r="H6" s="99" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
         <v>0.804688293317862</v>
       </c>
@@ -16223,416 +16214,419 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="106" t="s">
+      <c r="A8" s="105" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="106"/>
-      <c r="C8" s="106"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="107" t="s">
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="G8" s="108" t="n">
-        <v>0.275</v>
+      <c r="G8" s="107" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="93"/>
-      <c r="D9" s="94" t="s">
+      <c r="A9" s="92"/>
+      <c r="D9" s="93" t="s">
         <v>245</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>3.225</v>
-      </c>
-      <c r="G9" s="95" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G9" s="94" t="n">
         <f aca="false">E9+G8</f>
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="96" t="s">
+      <c r="A10" s="95" t="s">
         <v>254</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="93" t="s">
         <v>247</v>
       </c>
-      <c r="E10" s="52" t="n">
-        <v>44.5433</v>
-      </c>
-      <c r="F10" s="100"/>
-      <c r="G10" s="109" t="n">
+      <c r="E10" s="99" t="n">
+        <f aca="false">'Modes A-F'!E54</f>
+        <v>51.32</v>
+      </c>
+      <c r="F10" s="99"/>
+      <c r="G10" s="108" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>38.5444493951159</v>
+        <v>53.5014000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="95" t="s">
         <v>255</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="94" t="s">
+      <c r="D11" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="E11" s="0" t="n">
-        <v>128</v>
-      </c>
-      <c r="F11" s="100"/>
-      <c r="G11" s="109" t="n">
+      <c r="E11" s="99" t="n">
+        <f aca="false">'Modes A-F'!E57</f>
+        <v>136</v>
+      </c>
+      <c r="F11" s="99"/>
+      <c r="G11" s="108" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>121.6518993599</v>
+        <v>138.308400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="100" t="s">
         <v>256</v>
       </c>
-      <c r="B12" s="102" t="n">
+      <c r="B12" s="101" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="102"/>
-      <c r="D12" s="103" t="s">
+      <c r="C12" s="101"/>
+      <c r="D12" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="E12" s="102" t="n">
-        <v>128</v>
-      </c>
-      <c r="F12" s="110"/>
-      <c r="G12" s="111" t="n">
+      <c r="E12" s="109" t="n">
+        <f aca="false">'Modes A-F'!E58</f>
+        <v>136</v>
+      </c>
+      <c r="F12" s="109"/>
+      <c r="G12" s="110" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>121.016649295845</v>
+        <v>138.539400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="106"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="107" t="s">
+      <c r="B16" s="105"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
+      <c r="F16" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="G16" s="89" t="n">
+      <c r="G16" s="88" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="89"/>
-      <c r="I16" s="108"/>
+      <c r="H16" s="88"/>
+      <c r="I16" s="107"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="93"/>
-      <c r="D17" s="94" t="s">
+      <c r="A17" s="92"/>
+      <c r="D17" s="93" t="s">
         <v>245</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="112" t="n">
+      <c r="G17" s="111" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="113" t="s">
+      <c r="H17" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="I17" s="95" t="n">
+      <c r="I17" s="94" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
-        <v>-1.04940010581451</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="96" t="s">
+      <c r="A18" s="95" t="s">
         <v>258</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="94" t="s">
+      <c r="D18" s="93" t="s">
         <v>259</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="114" t="n">
+      <c r="G18" s="113" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="95"/>
+      <c r="I18" s="94"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="93"/>
-      <c r="D19" s="94" t="s">
+      <c r="A19" s="92"/>
+      <c r="D19" s="93" t="s">
         <v>260</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="112" t="n">
+      <c r="G19" s="111" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="95"/>
+      <c r="I19" s="94"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="93"/>
-      <c r="D20" s="94"/>
-      <c r="G20" s="115" t="s">
+      <c r="A20" s="92"/>
+      <c r="D20" s="93"/>
+      <c r="G20" s="114" t="s">
         <v>261</v>
       </c>
-      <c r="I20" s="95"/>
+      <c r="I20" s="94"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="93"/>
-      <c r="F21" s="116" t="s">
+      <c r="A21" s="92"/>
+      <c r="F21" s="115" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="95"/>
+      <c r="I21" s="94"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="96" t="s">
+      <c r="A22" s="95" t="s">
         <v>246</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="94" t="s">
+      <c r="D22" s="93" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="100" t="n">
+      <c r="E22" s="99" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-24.4724915287978</v>
-      </c>
-      <c r="F22" s="117" t="n">
+        <v>-16.6463914229833</v>
+      </c>
+      <c r="F22" s="116" t="n">
         <f aca="false">'Modes A-F'!I54</f>
         <v>-13.9982</v>
       </c>
-      <c r="G22" s="100" t="n">
+      <c r="G22" s="99" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-19.5211293546545</v>
-      </c>
-      <c r="I22" s="95"/>
+        <v>-11.69502924884</v>
+      </c>
+      <c r="I22" s="94"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="95" t="s">
         <v>248</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="94" t="s">
+      <c r="D23" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="E23" s="100" t="n">
+      <c r="E23" s="99" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>54.1898673743799</v>
-      </c>
-      <c r="F23" s="117" t="n">
+        <v>63.2392674801944</v>
+      </c>
+      <c r="F23" s="116" t="n">
         <f aca="false">'Modes A-F'!I56</f>
         <v>50.9301</v>
       </c>
-      <c r="G23" s="100" t="n">
+      <c r="G23" s="99" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>59.4904980422559</v>
-      </c>
-      <c r="I23" s="95"/>
+        <v>68.5398981480704</v>
+      </c>
+      <c r="I23" s="94"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="B24" s="102" t="n">
+      <c r="B24" s="101" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="103" t="s">
+      <c r="C24" s="101"/>
+      <c r="D24" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="E24" s="110" t="n">
+      <c r="E24" s="109" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>45.4694516785849</v>
-      </c>
-      <c r="F24" s="118" t="n">
+        <v>54.5188517843995</v>
+      </c>
+      <c r="F24" s="117" t="n">
         <f aca="false">'Modes A-F'!I57</f>
         <v>42.81</v>
       </c>
-      <c r="G24" s="119" t="n">
+      <c r="G24" s="118" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>51.4053659846675</v>
-      </c>
-      <c r="H24" s="102"/>
-      <c r="I24" s="120"/>
+        <v>60.454766090482</v>
+      </c>
+      <c r="H24" s="101"/>
+      <c r="I24" s="119"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="121" t="s">
+      <c r="A28" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="121"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="107" t="s">
+      <c r="B28" s="120"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="88"/>
+      <c r="E28" s="88"/>
+      <c r="F28" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="G28" s="89" t="n">
+      <c r="G28" s="88" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="89"/>
-      <c r="I28" s="108"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="107"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="93"/>
-      <c r="D29" s="94" t="s">
+      <c r="A29" s="92"/>
+      <c r="D29" s="93" t="s">
         <v>245</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="112" t="n">
+      <c r="G29" s="111" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="113" t="s">
+      <c r="H29" s="112" t="s">
         <v>257</v>
       </c>
-      <c r="I29" s="95" t="n">
+      <c r="I29" s="94" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
-        <v>-1.04940010581451</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="95" t="s">
         <v>258</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="94" t="s">
+      <c r="D30" s="93" t="s">
         <v>259</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="114" t="n">
+      <c r="G30" s="113" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="95"/>
+      <c r="I30" s="94"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="93"/>
-      <c r="D31" s="94" t="s">
+      <c r="A31" s="92"/>
+      <c r="D31" s="93" t="s">
         <v>260</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="112" t="n">
+      <c r="G31" s="111" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="95"/>
+      <c r="I31" s="94"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="93"/>
-      <c r="D32" s="94"/>
-      <c r="G32" s="115" t="s">
+      <c r="A32" s="92"/>
+      <c r="D32" s="93"/>
+      <c r="G32" s="114" t="s">
         <v>261</v>
       </c>
-      <c r="I32" s="95"/>
+      <c r="I32" s="94"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="93"/>
-      <c r="F33" s="116" t="s">
+      <c r="A33" s="92"/>
+      <c r="F33" s="115" t="s">
         <v>243</v>
       </c>
-      <c r="I33" s="95"/>
+      <c r="I33" s="94"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="95" t="s">
         <v>246</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="94" t="s">
+      <c r="D34" s="93" t="s">
         <v>247</v>
       </c>
-      <c r="E34" s="100" t="n">
+      <c r="E34" s="99" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-50.4313236638297</v>
-      </c>
-      <c r="F34" s="117" t="n">
+        <v>-43.6546236638297</v>
+      </c>
+      <c r="F34" s="116" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-52.1921</v>
       </c>
-      <c r="G34" s="100" t="n">
+      <c r="G34" s="99" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-46.5291008925127</v>
-      </c>
-      <c r="I34" s="95"/>
+        <v>-38.7030007866982</v>
+      </c>
+      <c r="I34" s="94"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="96" t="s">
+      <c r="A35" s="95" t="s">
         <v>248</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="94" t="s">
+      <c r="D35" s="93" t="s">
         <v>249</v>
       </c>
-      <c r="E35" s="100" t="n">
+      <c r="E35" s="99" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>26.3258777773465</v>
-      </c>
-      <c r="F35" s="117" t="n">
+        <v>34.3258777773465</v>
+      </c>
+      <c r="F35" s="116" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="100" t="n">
+      <c r="G35" s="99" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>30.5773874323536</v>
-      </c>
-      <c r="I35" s="95"/>
+        <v>39.6267875381681</v>
+      </c>
+      <c r="I35" s="94"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="101" t="s">
+      <c r="A36" s="100" t="s">
         <v>250</v>
       </c>
-      <c r="B36" s="102" t="n">
+      <c r="B36" s="101" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="102"/>
-      <c r="D36" s="103" t="s">
+      <c r="C36" s="101"/>
+      <c r="D36" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="E36" s="110" t="n">
+      <c r="E36" s="109" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>14.140175674289</v>
-      </c>
-      <c r="F36" s="118" t="n">
+        <v>22.140175674289</v>
+      </c>
+      <c r="F36" s="117" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="110" t="n">
+      <c r="G36" s="109" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>19.027002416953</v>
-      </c>
-      <c r="H36" s="102"/>
-      <c r="I36" s="120"/>
+        <v>28.0764025227675</v>
+      </c>
+      <c r="H36" s="101"/>
+      <c r="I36" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -16735,7 +16729,7 @@
       <c r="A9" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="B9" s="122" t="n">
+      <c r="B9" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -16759,7 +16753,7 @@
       <c r="A12" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="122" t="n">
+      <c r="B12" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -16855,7 +16849,7 @@
       <c r="A24" s="0" t="s">
         <v>285</v>
       </c>
-      <c r="B24" s="122" t="n">
+      <c r="B24" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -16879,7 +16873,7 @@
       <c r="A27" s="0" t="s">
         <v>288</v>
       </c>
-      <c r="B27" s="122" t="n">
+      <c r="B27" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -16975,7 +16969,7 @@
       <c r="A39" s="0" t="s">
         <v>300</v>
       </c>
-      <c r="B39" s="122" t="n">
+      <c r="B39" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -16999,7 +16993,7 @@
       <c r="A42" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="B42" s="122" t="n">
+      <c r="B42" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17095,7 +17089,7 @@
       <c r="A54" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="B54" s="122" t="n">
+      <c r="B54" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17119,7 +17113,7 @@
       <c r="A57" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="B57" s="122" t="n">
+      <c r="B57" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17183,7 +17177,7 @@
       <c r="A65" s="0" t="s">
         <v>326</v>
       </c>
-      <c r="B65" s="122" t="n">
+      <c r="B65" s="121" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -17191,7 +17185,7 @@
       <c r="A66" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="B66" s="122" t="n">
+      <c r="B66" s="121" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -17199,7 +17193,7 @@
       <c r="A67" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="B67" s="122" t="n">
+      <c r="B67" s="121" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -17207,7 +17201,7 @@
       <c r="A68" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="B68" s="122" t="n">
+      <c r="B68" s="121" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -17527,7 +17521,7 @@
       <c r="A108" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="B108" s="122" t="n">
+      <c r="B108" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17551,7 +17545,7 @@
       <c r="A111" s="0" t="s">
         <v>372</v>
       </c>
-      <c r="B111" s="122" t="n">
+      <c r="B111" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17647,7 +17641,7 @@
       <c r="A123" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="B123" s="122" t="n">
+      <c r="B123" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17671,7 +17665,7 @@
       <c r="A126" s="0" t="s">
         <v>387</v>
       </c>
-      <c r="B126" s="122" t="n">
+      <c r="B126" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17767,7 +17761,7 @@
       <c r="A138" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="B138" s="122" t="n">
+      <c r="B138" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17791,7 +17785,7 @@
       <c r="A141" s="0" t="s">
         <v>402</v>
       </c>
-      <c r="B141" s="122" t="n">
+      <c r="B141" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17887,7 +17881,7 @@
       <c r="A153" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="B153" s="122" t="n">
+      <c r="B153" s="121" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17911,7 +17905,7 @@
       <c r="A156" s="0" t="s">
         <v>417</v>
       </c>
-      <c r="B156" s="122" t="n">
+      <c r="B156" s="121" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17975,7 +17969,7 @@
       <c r="A164" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="B164" s="122" t="n">
+      <c r="B164" s="121" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -17983,7 +17977,7 @@
       <c r="A165" s="0" t="s">
         <v>426</v>
       </c>
-      <c r="B165" s="122" t="n">
+      <c r="B165" s="121" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -17991,7 +17985,7 @@
       <c r="A166" s="0" t="s">
         <v>427</v>
       </c>
-      <c r="B166" s="122" t="n">
+      <c r="B166" s="121" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -17999,7 +17993,7 @@
       <c r="A167" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="B167" s="122" t="n">
+      <c r="B167" s="121" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -18135,7 +18129,7 @@
       <c r="A184" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="B184" s="122" t="n">
+      <c r="B184" s="121" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -18143,7 +18137,7 @@
       <c r="A185" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="B185" s="122" t="n">
+      <c r="B185" s="121" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -18175,7 +18169,7 @@
       <c r="A189" s="0" t="s">
         <v>450</v>
       </c>
-      <c r="B189" s="122" t="n">
+      <c r="B189" s="121" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -18199,7 +18193,7 @@
       <c r="A192" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="B192" s="122" t="n">
+      <c r="B192" s="121" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -18207,7 +18201,7 @@
       <c r="A193" s="0" t="s">
         <v>454</v>
       </c>
-      <c r="B193" s="122" t="n">
+      <c r="B193" s="121" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -18215,7 +18209,7 @@
       <c r="A194" s="0" t="s">
         <v>455</v>
       </c>
-      <c r="B194" s="122" t="n">
+      <c r="B194" s="121" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -18223,7 +18217,7 @@
       <c r="A195" s="0" t="s">
         <v>456</v>
       </c>
-      <c r="B195" s="122" t="n">
+      <c r="B195" s="121" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -19647,40 +19641,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="122" t="n">
+      <c r="C337" s="121" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="122" t="n">
+      <c r="D337" s="121" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="122" t="n">
+      <c r="E337" s="121" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="122" t="n">
+      <c r="F337" s="121" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="122" t="n">
+      <c r="G337" s="121" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="122" t="n">
+      <c r="H337" s="121" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="122" t="n">
+      <c r="I337" s="121" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="122" t="n">
+      <c r="J337" s="121" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="122" t="n">
+      <c r="K337" s="121" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="122" t="n">
+      <c r="L337" s="121" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="122" t="n">
+      <c r="M337" s="121" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="122" t="n">
+      <c r="N337" s="121" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -19691,40 +19685,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="122" t="n">
+      <c r="C338" s="121" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="122" t="n">
+      <c r="D338" s="121" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="122" t="n">
+      <c r="E338" s="121" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="122" t="n">
+      <c r="F338" s="121" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="122" t="n">
+      <c r="G338" s="121" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="122" t="n">
+      <c r="H338" s="121" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="122" t="n">
+      <c r="I338" s="121" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="122" t="n">
+      <c r="J338" s="121" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="122" t="n">
+      <c r="K338" s="121" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="122" t="n">
+      <c r="L338" s="121" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="122" t="n">
+      <c r="M338" s="121" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="122" t="n">
+      <c r="N338" s="121" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -19735,40 +19729,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="122" t="n">
+      <c r="C339" s="121" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="122" t="n">
+      <c r="D339" s="121" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="122" t="n">
+      <c r="E339" s="121" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="122" t="n">
+      <c r="F339" s="121" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="122" t="n">
+      <c r="G339" s="121" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="122" t="n">
+      <c r="H339" s="121" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="122" t="n">
+      <c r="I339" s="121" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="122" t="n">
+      <c r="J339" s="121" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="122" t="n">
+      <c r="K339" s="121" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="122" t="n">
+      <c r="L339" s="121" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="122" t="n">
+      <c r="M339" s="121" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="122" t="n">
+      <c r="N339" s="121" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -19779,40 +19773,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="122" t="n">
+      <c r="C340" s="121" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="122" t="n">
+      <c r="D340" s="121" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="122" t="n">
+      <c r="E340" s="121" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="122" t="n">
+      <c r="F340" s="121" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="122" t="n">
+      <c r="G340" s="121" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="122" t="n">
+      <c r="H340" s="121" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="122" t="n">
+      <c r="I340" s="121" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="122" t="n">
+      <c r="J340" s="121" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="122" t="n">
+      <c r="K340" s="121" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="122" t="n">
+      <c r="L340" s="121" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="122" t="n">
+      <c r="M340" s="121" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="122" t="n">
+      <c r="N340" s="121" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -20527,40 +20521,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="122" t="n">
+      <c r="C357" s="121" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="122" t="n">
+      <c r="D357" s="121" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="122" t="n">
+      <c r="E357" s="121" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="122" t="n">
+      <c r="F357" s="121" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="122" t="n">
+      <c r="G357" s="121" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="122" t="n">
+      <c r="H357" s="121" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="122" t="n">
+      <c r="I357" s="121" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="122" t="n">
+      <c r="J357" s="121" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="122" t="n">
+      <c r="K357" s="121" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="122" t="n">
+      <c r="L357" s="121" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="122" t="n">
+      <c r="M357" s="121" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="122" t="n">
+      <c r="N357" s="121" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -20571,40 +20565,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="122" t="n">
+      <c r="C358" s="121" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="122" t="n">
+      <c r="D358" s="121" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="122" t="n">
+      <c r="E358" s="121" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="122" t="n">
+      <c r="F358" s="121" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="122" t="n">
+      <c r="G358" s="121" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="122" t="n">
+      <c r="H358" s="121" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="122" t="n">
+      <c r="I358" s="121" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="122" t="n">
+      <c r="J358" s="121" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="122" t="n">
+      <c r="K358" s="121" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="122" t="n">
+      <c r="L358" s="121" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="122" t="n">
+      <c r="M358" s="121" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="122" t="n">
+      <c r="N358" s="121" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -20615,40 +20609,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="122" t="n">
+      <c r="C359" s="121" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="122" t="n">
+      <c r="D359" s="121" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="122" t="n">
+      <c r="E359" s="121" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="122" t="n">
+      <c r="F359" s="121" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="122" t="n">
+      <c r="G359" s="121" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="122" t="n">
+      <c r="H359" s="121" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="122" t="n">
+      <c r="I359" s="121" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="122" t="n">
+      <c r="J359" s="121" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="122" t="n">
+      <c r="K359" s="121" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="122" t="n">
+      <c r="L359" s="121" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="122" t="n">
+      <c r="M359" s="121" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="122" t="n">
+      <c r="N359" s="121" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -20659,40 +20653,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="122" t="n">
+      <c r="C360" s="121" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="122" t="n">
+      <c r="D360" s="121" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="122" t="n">
+      <c r="E360" s="121" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="122" t="n">
+      <c r="F360" s="121" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="122" t="n">
+      <c r="G360" s="121" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="122" t="n">
+      <c r="H360" s="121" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="122" t="n">
+      <c r="I360" s="121" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="122" t="n">
+      <c r="J360" s="121" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="122" t="n">
+      <c r="K360" s="121" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="122" t="n">
+      <c r="L360" s="121" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="122" t="n">
+      <c r="M360" s="121" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="122" t="n">
+      <c r="N360" s="121" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -20835,7 +20829,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="122" t="n">
+      <c r="C364" s="121" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -20879,7 +20873,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="122" t="n">
+      <c r="C365" s="121" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -20923,7 +20917,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="122" t="n">
+      <c r="C366" s="121" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -20967,7 +20961,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="122" t="n">
+      <c r="C367" s="121" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -22744,13 +22738,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="122" t="s">
         <v>792</v>
       </c>
-      <c r="C1" s="123" t="n">
+      <c r="C1" s="122" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="122" t="s">
         <v>793</v>
       </c>
     </row>
@@ -22758,10 +22752,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="122" t="s">
         <v>794</v>
       </c>
-      <c r="C2" s="123" t="n">
+      <c r="C2" s="122" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -22769,10 +22763,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="122" t="s">
         <v>795</v>
       </c>
-      <c r="C3" s="123" t="n">
+      <c r="C3" s="122" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -22876,7 +22870,7 @@
       <c r="B16" s="0" t="s">
         <v>810</v>
       </c>
-      <c r="C16" s="122" t="n">
+      <c r="C16" s="121" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -22884,7 +22878,7 @@
       <c r="B17" s="0" t="s">
         <v>811</v>
       </c>
-      <c r="C17" s="122" t="n">
+      <c r="C17" s="121" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -22892,7 +22886,7 @@
       <c r="B18" s="0" t="s">
         <v>812</v>
       </c>
-      <c r="C18" s="122" t="n">
+      <c r="C18" s="121" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -22900,7 +22894,7 @@
       <c r="B19" s="0" t="s">
         <v>813</v>
       </c>
-      <c r="C19" s="122" t="n">
+      <c r="C19" s="121" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -23388,7 +23382,7 @@
       <c r="B80" s="0" t="s">
         <v>881</v>
       </c>
-      <c r="C80" s="122" t="n">
+      <c r="C80" s="121" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -23436,7 +23430,7 @@
       <c r="B86" s="0" t="s">
         <v>887</v>
       </c>
-      <c r="C86" s="122" t="n">
+      <c r="C86" s="121" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -23468,7 +23462,7 @@
       <c r="B90" s="0" t="s">
         <v>891</v>
       </c>
-      <c r="C90" s="122" t="n">
+      <c r="C90" s="121" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -23556,7 +23550,7 @@
       <c r="B101" s="0" t="s">
         <v>903</v>
       </c>
-      <c r="C101" s="122" t="n">
+      <c r="C101" s="121" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -23732,7 +23726,7 @@
       <c r="B123" s="0" t="s">
         <v>927</v>
       </c>
-      <c r="C123" s="122" t="n">
+      <c r="C123" s="121" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -23796,7 +23790,7 @@
       <c r="B131" s="0" t="s">
         <v>935</v>
       </c>
-      <c r="C131" s="122" t="n">
+      <c r="C131" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -23812,7 +23806,7 @@
       <c r="B133" s="0" t="s">
         <v>937</v>
       </c>
-      <c r="C133" s="122" t="n">
+      <c r="C133" s="121" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -24332,7 +24326,7 @@
       <c r="B198" s="0" t="s">
         <v>1004</v>
       </c>
-      <c r="C198" s="122" t="n">
+      <c r="C198" s="121" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -24380,7 +24374,7 @@
       <c r="B204" s="0" t="s">
         <v>1010</v>
       </c>
-      <c r="C204" s="122" t="n">
+      <c r="C204" s="121" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -24412,7 +24406,7 @@
       <c r="B208" s="0" t="s">
         <v>1014</v>
       </c>
-      <c r="C208" s="122" t="n">
+      <c r="C208" s="121" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -24500,7 +24494,7 @@
       <c r="B219" s="0" t="s">
         <v>1025</v>
       </c>
-      <c r="C219" s="122" t="n">
+      <c r="C219" s="121" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -24676,7 +24670,7 @@
       <c r="B241" s="0" t="s">
         <v>1048</v>
       </c>
-      <c r="C241" s="122" t="n">
+      <c r="C241" s="121" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -24740,7 +24734,7 @@
       <c r="B249" s="0" t="s">
         <v>1056</v>
       </c>
-      <c r="C249" s="122" t="n">
+      <c r="C249" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -24756,7 +24750,7 @@
       <c r="B251" s="0" t="s">
         <v>1058</v>
       </c>
-      <c r="C251" s="122" t="n">
+      <c r="C251" s="121" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -25276,7 +25270,7 @@
       <c r="B316" s="0" t="s">
         <v>1123</v>
       </c>
-      <c r="C316" s="122" t="n">
+      <c r="C316" s="121" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -25324,7 +25318,7 @@
       <c r="B322" s="0" t="s">
         <v>1129</v>
       </c>
-      <c r="C322" s="122" t="n">
+      <c r="C322" s="121" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -25356,7 +25350,7 @@
       <c r="B326" s="0" t="s">
         <v>1133</v>
       </c>
-      <c r="C326" s="122" t="n">
+      <c r="C326" s="121" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -25444,7 +25438,7 @@
       <c r="B337" s="0" t="s">
         <v>1144</v>
       </c>
-      <c r="C337" s="122" t="n">
+      <c r="C337" s="121" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -25620,7 +25614,7 @@
       <c r="B359" s="0" t="s">
         <v>1167</v>
       </c>
-      <c r="C359" s="122" t="n">
+      <c r="C359" s="121" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -25684,7 +25678,7 @@
       <c r="B367" s="0" t="s">
         <v>1175</v>
       </c>
-      <c r="C367" s="122" t="n">
+      <c r="C367" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25700,7 +25694,7 @@
       <c r="B369" s="0" t="s">
         <v>1177</v>
       </c>
-      <c r="C369" s="122" t="n">
+      <c r="C369" s="121" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -26220,7 +26214,7 @@
       <c r="B434" s="0" t="s">
         <v>1242</v>
       </c>
-      <c r="C434" s="122" t="n">
+      <c r="C434" s="121" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -26268,7 +26262,7 @@
       <c r="B440" s="0" t="s">
         <v>1248</v>
       </c>
-      <c r="C440" s="122" t="n">
+      <c r="C440" s="121" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -26300,7 +26294,7 @@
       <c r="B444" s="0" t="s">
         <v>1252</v>
       </c>
-      <c r="C444" s="122" t="n">
+      <c r="C444" s="121" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -26388,7 +26382,7 @@
       <c r="B455" s="0" t="s">
         <v>1263</v>
       </c>
-      <c r="C455" s="122" t="n">
+      <c r="C455" s="121" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -26564,7 +26558,7 @@
       <c r="B477" s="0" t="s">
         <v>1286</v>
       </c>
-      <c r="C477" s="122" t="n">
+      <c r="C477" s="121" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -26628,7 +26622,7 @@
       <c r="B485" s="0" t="s">
         <v>1294</v>
       </c>
-      <c r="C485" s="122" t="n">
+      <c r="C485" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26644,7 +26638,7 @@
       <c r="B487" s="0" t="s">
         <v>1296</v>
       </c>
-      <c r="C487" s="122" t="n">
+      <c r="C487" s="121" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -26732,7 +26726,7 @@
       <c r="B498" s="0" t="s">
         <v>1307</v>
       </c>
-      <c r="C498" s="122" t="n">
+      <c r="C498" s="121" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -26740,7 +26734,7 @@
       <c r="B499" s="0" t="s">
         <v>1308</v>
       </c>
-      <c r="C499" s="122" t="n">
+      <c r="C499" s="121" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -26748,7 +26742,7 @@
       <c r="B500" s="0" t="s">
         <v>1309</v>
       </c>
-      <c r="C500" s="122" t="n">
+      <c r="C500" s="121" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -26756,7 +26750,7 @@
       <c r="B501" s="0" t="s">
         <v>1310</v>
       </c>
-      <c r="C501" s="122" t="n">
+      <c r="C501" s="121" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -27324,7 +27318,7 @@
       <c r="B572" s="0" t="s">
         <v>1381</v>
       </c>
-      <c r="C572" s="122" t="n">
+      <c r="C572" s="121" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -27372,7 +27366,7 @@
       <c r="B578" s="0" t="s">
         <v>1387</v>
       </c>
-      <c r="C578" s="122" t="n">
+      <c r="C578" s="121" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -27404,7 +27398,7 @@
       <c r="B582" s="0" t="s">
         <v>1391</v>
       </c>
-      <c r="C582" s="122" t="n">
+      <c r="C582" s="121" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -27492,7 +27486,7 @@
       <c r="B593" s="0" t="s">
         <v>1402</v>
       </c>
-      <c r="C593" s="122" t="n">
+      <c r="C593" s="121" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -27668,7 +27662,7 @@
       <c r="B615" s="0" t="s">
         <v>1425</v>
       </c>
-      <c r="C615" s="122" t="n">
+      <c r="C615" s="121" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -27732,7 +27726,7 @@
       <c r="B623" s="0" t="s">
         <v>1433</v>
       </c>
-      <c r="C623" s="122" t="n">
+      <c r="C623" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27748,7 +27742,7 @@
       <c r="B625" s="0" t="s">
         <v>1435</v>
       </c>
-      <c r="C625" s="122" t="n">
+      <c r="C625" s="121" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -28268,7 +28262,7 @@
       <c r="B690" s="0" t="s">
         <v>1500</v>
       </c>
-      <c r="C690" s="122" t="n">
+      <c r="C690" s="121" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -28316,7 +28310,7 @@
       <c r="B696" s="0" t="s">
         <v>1506</v>
       </c>
-      <c r="C696" s="122" t="n">
+      <c r="C696" s="121" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -28348,7 +28342,7 @@
       <c r="B700" s="0" t="s">
         <v>1510</v>
       </c>
-      <c r="C700" s="122" t="n">
+      <c r="C700" s="121" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -28436,7 +28430,7 @@
       <c r="B711" s="0" t="s">
         <v>1521</v>
       </c>
-      <c r="C711" s="122" t="n">
+      <c r="C711" s="121" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -28612,7 +28606,7 @@
       <c r="B733" s="0" t="s">
         <v>1544</v>
       </c>
-      <c r="C733" s="122" t="n">
+      <c r="C733" s="121" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -28676,7 +28670,7 @@
       <c r="B741" s="0" t="s">
         <v>1552</v>
       </c>
-      <c r="C741" s="122" t="n">
+      <c r="C741" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28692,7 +28686,7 @@
       <c r="B743" s="0" t="s">
         <v>1554</v>
       </c>
-      <c r="C743" s="122" t="n">
+      <c r="C743" s="121" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -29248,7 +29242,7 @@
       <c r="B811" s="0" t="s">
         <v>1630</v>
       </c>
-      <c r="C811" s="122" t="n">
+      <c r="C811" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -29764,7 +29758,7 @@
       <c r="B874" s="0" t="s">
         <v>1695</v>
       </c>
-      <c r="C874" s="122" t="n">
+      <c r="C874" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30280,7 +30274,7 @@
       <c r="B937" s="0" t="s">
         <v>1760</v>
       </c>
-      <c r="C937" s="122" t="n">
+      <c r="C937" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30796,7 +30790,7 @@
       <c r="B1000" s="0" t="s">
         <v>1825</v>
       </c>
-      <c r="C1000" s="122" t="n">
+      <c r="C1000" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31312,7 +31306,7 @@
       <c r="B1063" s="0" t="s">
         <v>1890</v>
       </c>
-      <c r="C1063" s="122" t="n">
+      <c r="C1063" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31828,7 +31822,7 @@
       <c r="B1126" s="0" t="s">
         <v>1955</v>
       </c>
-      <c r="C1126" s="122" t="n">
+      <c r="C1126" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32344,7 +32338,7 @@
       <c r="B1189" s="0" t="s">
         <v>2020</v>
       </c>
-      <c r="C1189" s="122" t="n">
+      <c r="C1189" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32860,7 +32854,7 @@
       <c r="B1252" s="0" t="s">
         <v>2085</v>
       </c>
-      <c r="C1252" s="122" t="n">
+      <c r="C1252" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33376,7 +33370,7 @@
       <c r="B1315" s="0" t="s">
         <v>2150</v>
       </c>
-      <c r="C1315" s="122" t="n">
+      <c r="C1315" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33892,7 +33886,7 @@
       <c r="B1378" s="0" t="s">
         <v>2215</v>
       </c>
-      <c r="C1378" s="122" t="n">
+      <c r="C1378" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34408,7 +34402,7 @@
       <c r="B1441" s="0" t="s">
         <v>2280</v>
       </c>
-      <c r="C1441" s="122" t="n">
+      <c r="C1441" s="121" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34856,7 +34850,7 @@
       <c r="B1497" s="0" t="s">
         <v>2339</v>
       </c>
-      <c r="C1497" s="122" t="n">
+      <c r="C1497" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -35482,7 +35476,7 @@
       <c r="B1576" s="0" t="s">
         <v>2423</v>
       </c>
-      <c r="C1576" s="122" t="n">
+      <c r="C1576" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -35651,7 +35645,7 @@
       <c r="B1596" s="0" t="s">
         <v>2445</v>
       </c>
-      <c r="C1596" s="122" t="n">
+      <c r="C1596" s="121" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -35659,7 +35653,7 @@
       <c r="B1597" s="0" t="s">
         <v>2446</v>
       </c>
-      <c r="C1597" s="122" t="n">
+      <c r="C1597" s="121" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36539,7 +36533,7 @@
       <c r="B1707" s="0" t="s">
         <v>2557</v>
       </c>
-      <c r="C1707" s="122" t="n">
+      <c r="C1707" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36555,7 +36549,7 @@
       <c r="B1709" s="0" t="s">
         <v>2559</v>
       </c>
-      <c r="C1709" s="122" t="n">
+      <c r="C1709" s="121" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -37075,7 +37069,7 @@
       <c r="B1774" s="0" t="s">
         <v>2624</v>
       </c>
-      <c r="C1774" s="122" t="n">
+      <c r="C1774" s="121" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -37155,7 +37149,7 @@
       <c r="B1784" s="0" t="s">
         <v>2634</v>
       </c>
-      <c r="C1784" s="122" t="n">
+      <c r="C1784" s="121" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -37243,7 +37237,7 @@
       <c r="B1795" s="0" t="s">
         <v>2645</v>
       </c>
-      <c r="C1795" s="122" t="n">
+      <c r="C1795" s="121" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -37419,7 +37413,7 @@
       <c r="B1817" s="0" t="s">
         <v>2668</v>
       </c>
-      <c r="C1817" s="122" t="n">
+      <c r="C1817" s="121" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -37483,7 +37477,7 @@
       <c r="B1825" s="0" t="s">
         <v>2676</v>
       </c>
-      <c r="C1825" s="122" t="n">
+      <c r="C1825" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37499,7 +37493,7 @@
       <c r="B1827" s="0" t="s">
         <v>2678</v>
       </c>
-      <c r="C1827" s="122" t="n">
+      <c r="C1827" s="121" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -38102,7 +38096,7 @@
       <c r="B1902" s="0" t="s">
         <v>2755</v>
       </c>
-      <c r="C1902" s="122" t="n">
+      <c r="C1902" s="121" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -38150,7 +38144,7 @@
       <c r="B1908" s="0" t="s">
         <v>2761</v>
       </c>
-      <c r="C1908" s="122" t="n">
+      <c r="C1908" s="121" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -38182,7 +38176,7 @@
       <c r="B1912" s="0" t="s">
         <v>2765</v>
       </c>
-      <c r="C1912" s="122" t="n">
+      <c r="C1912" s="121" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -38270,7 +38264,7 @@
       <c r="B1923" s="0" t="s">
         <v>2776</v>
       </c>
-      <c r="C1923" s="122" t="n">
+      <c r="C1923" s="121" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -38446,7 +38440,7 @@
       <c r="B1945" s="0" t="s">
         <v>2799</v>
       </c>
-      <c r="C1945" s="122" t="n">
+      <c r="C1945" s="121" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -38510,7 +38504,7 @@
       <c r="B1953" s="0" t="s">
         <v>2807</v>
       </c>
-      <c r="C1953" s="122" t="n">
+      <c r="C1953" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38526,7 +38520,7 @@
       <c r="B1955" s="0" t="s">
         <v>2809</v>
       </c>
-      <c r="C1955" s="122" t="n">
+      <c r="C1955" s="121" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -39046,7 +39040,7 @@
       <c r="B2020" s="0" t="s">
         <v>2874</v>
       </c>
-      <c r="C2020" s="122" t="n">
+      <c r="C2020" s="121" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -39094,7 +39088,7 @@
       <c r="B2026" s="0" t="s">
         <v>2880</v>
       </c>
-      <c r="C2026" s="122" t="n">
+      <c r="C2026" s="121" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -39126,7 +39120,7 @@
       <c r="B2030" s="0" t="s">
         <v>2884</v>
       </c>
-      <c r="C2030" s="122" t="n">
+      <c r="C2030" s="121" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -39214,7 +39208,7 @@
       <c r="B2041" s="0" t="s">
         <v>2895</v>
       </c>
-      <c r="C2041" s="122" t="n">
+      <c r="C2041" s="121" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -39390,7 +39384,7 @@
       <c r="B2063" s="0" t="s">
         <v>2918</v>
       </c>
-      <c r="C2063" s="122" t="n">
+      <c r="C2063" s="121" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -39454,7 +39448,7 @@
       <c r="B2071" s="0" t="s">
         <v>2926</v>
       </c>
-      <c r="C2071" s="122" t="n">
+      <c r="C2071" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39470,7 +39464,7 @@
       <c r="B2073" s="0" t="s">
         <v>2928</v>
       </c>
-      <c r="C2073" s="122" t="n">
+      <c r="C2073" s="121" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -39990,7 +39984,7 @@
       <c r="B2138" s="0" t="s">
         <v>2993</v>
       </c>
-      <c r="C2138" s="122" t="n">
+      <c r="C2138" s="121" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -40038,7 +40032,7 @@
       <c r="B2144" s="0" t="s">
         <v>2999</v>
       </c>
-      <c r="C2144" s="122" t="n">
+      <c r="C2144" s="121" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -40070,7 +40064,7 @@
       <c r="B2148" s="0" t="s">
         <v>3003</v>
       </c>
-      <c r="C2148" s="122" t="n">
+      <c r="C2148" s="121" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -40158,7 +40152,7 @@
       <c r="B2159" s="0" t="s">
         <v>3014</v>
       </c>
-      <c r="C2159" s="122" t="n">
+      <c r="C2159" s="121" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -40334,7 +40328,7 @@
       <c r="B2181" s="0" t="s">
         <v>3037</v>
       </c>
-      <c r="C2181" s="122" t="n">
+      <c r="C2181" s="121" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -40398,7 +40392,7 @@
       <c r="B2189" s="0" t="s">
         <v>3045</v>
       </c>
-      <c r="C2189" s="122" t="n">
+      <c r="C2189" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40414,7 +40408,7 @@
       <c r="B2191" s="0" t="s">
         <v>3047</v>
       </c>
-      <c r="C2191" s="122" t="n">
+      <c r="C2191" s="121" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -40990,7 +40984,7 @@
       <c r="B2263" s="0" t="s">
         <v>3122</v>
       </c>
-      <c r="C2263" s="122" t="n">
+      <c r="C2263" s="121" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41277,7 +41271,7 @@
       <c r="F2297" s="0" t="s">
         <v>3167</v>
       </c>
-      <c r="G2297" s="124" t="n">
+      <c r="G2297" s="123" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -41369,7 +41363,7 @@
       <c r="B2307" s="0" t="s">
         <v>3181</v>
       </c>
-      <c r="C2307" s="122" t="n">
+      <c r="C2307" s="121" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -41455,7 +41449,7 @@
       <c r="B2317" s="0" t="s">
         <v>3197</v>
       </c>
-      <c r="C2317" s="122" t="n">
+      <c r="C2317" s="121" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -41463,7 +41457,7 @@
       <c r="B2318" s="0" t="s">
         <v>3198</v>
       </c>
-      <c r="C2318" s="122" t="n">
+      <c r="C2318" s="121" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -41479,7 +41473,7 @@
       <c r="B2320" s="0" t="s">
         <v>3200</v>
       </c>
-      <c r="C2320" s="122" t="n">
+      <c r="C2320" s="121" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -41527,7 +41521,7 @@
       <c r="C2326" s="0" t="s">
         <v>3208</v>
       </c>
-      <c r="D2326" s="125" t="n">
+      <c r="D2326" s="124" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -41578,7 +41572,7 @@
       <c r="C2332" s="0" t="s">
         <v>3216</v>
       </c>
-      <c r="D2332" s="125" t="n">
+      <c r="D2332" s="124" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -41597,7 +41591,7 @@
       <c r="D2334" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="E2334" s="125" t="n">
+      <c r="E2334" s="124" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -41655,7 +41649,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="125" t="n">
+      <c r="F2339" s="124" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -42127,7 +42121,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="125" t="n">
+      <c r="F2380" s="124" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modes and cheatsheet tweaks
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -47,10 +47,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.15
-pitch = 3.225
+          <t>vert = -4.35
+pitch = 3.5
 lateral = 0.0
-yaw = 0.053</t>
+yaw = 0.2</t>
         </r>
       </text>
     </comment>
@@ -11393,7 +11393,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="F39" activeCellId="0" sqref="F39"/>
+      <selection pane="bottomRight" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13165,10 +13165,10 @@
         <v>134</v>
       </c>
       <c r="E40" s="30" t="n">
-        <v>-0.034</v>
+        <v>-0.1287</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-12534</v>
+        <v>-13478</v>
       </c>
       <c r="G40" s="30" t="n">
         <v>-0.034</v>
@@ -13213,10 +13213,10 @@
         <v>137</v>
       </c>
       <c r="E41" s="30" t="n">
-        <v>0.034</v>
+        <v>0.1289</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-27156</v>
+        <v>-26210</v>
       </c>
       <c r="G41" s="30" t="n">
         <v>0.034</v>

</xml_diff>

<commit_message>
update Modes doc after move to xf06bm
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -48,7 +48,7 @@
             <charset val="1"/>
           </rPr>
           <t>vert = -4.35
-pitch = 3.5
+Pitch = 2.8
 lateral = 0.0
 yaw = 0.2</t>
         </r>
@@ -89,11 +89,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.15
-pitch = 3.225
+          <t>vert = -4.35
+Pitch = 2.8
 lateral = 0.0
-yaw = 0.053
-Note: underfocused!</t>
+yaw = 0.2</t>
         </r>
       </text>
     </comment>
@@ -133,11 +132,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.15
-pitch = 3.225
+          <t>vert = -4.35
+Pitch = 2.8
 lateral = 0.0
-yaw = 0.053
-Note: underfocused!</t>
+yaw = 0.2</t>
         </r>
       </text>
     </comment>
@@ -11586,11 +11584,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="P45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="P1" activeCellId="0" sqref="P1"/>
-      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
-      <selection pane="bottomRight" activeCell="T39" activeCellId="0" sqref="T39"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="F54" activeCellId="0" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13451,22 +13449,22 @@
         <v>125</v>
       </c>
       <c r="E37" s="42" t="n">
-        <v>-6.60298</v>
+        <v>-6.1522</v>
       </c>
       <c r="F37" s="20" t="n">
-        <v>-59529</v>
+        <v>-55022</v>
       </c>
       <c r="G37" s="42" t="n">
-        <v>-6.2262</v>
+        <v>-6.1522</v>
       </c>
       <c r="H37" s="20" t="n">
-        <v>-55761</v>
+        <v>-55022</v>
       </c>
       <c r="I37" s="42" t="n">
-        <v>-6.2262</v>
+        <v>-6.1522</v>
       </c>
       <c r="J37" s="20" t="n">
-        <v>-55761</v>
+        <v>-55022</v>
       </c>
       <c r="K37" s="43" t="n">
         <v>6</v>
@@ -13527,22 +13525,22 @@
         <v>128</v>
       </c>
       <c r="E38" s="33" t="n">
-        <v>-2.09497</v>
+        <v>-2.5456</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>-29850</v>
+        <v>-34356</v>
       </c>
       <c r="G38" s="33" t="n">
-        <v>-2.0722</v>
+        <v>-2.5456</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>-29624</v>
+        <v>-34356</v>
       </c>
       <c r="I38" s="33" t="n">
-        <v>-2.0722</v>
+        <v>-2.5456</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>-29624</v>
+        <v>-34356</v>
       </c>
       <c r="K38" s="31" t="n">
         <v>6</v>
@@ -13581,22 +13579,22 @@
         <v>131</v>
       </c>
       <c r="E39" s="33" t="n">
-        <v>-2.09497</v>
+        <v>-2.5459</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>-23949</v>
+        <v>-28458</v>
       </c>
       <c r="G39" s="33" t="n">
-        <v>-2.0722</v>
+        <v>-2.5459</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>-23721</v>
+        <v>-28458</v>
       </c>
       <c r="I39" s="33" t="n">
-        <v>-2.0722</v>
+        <v>-2.5459</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>-23721</v>
+        <v>-28458</v>
       </c>
       <c r="K39" s="31" t="n">
         <v>6</v>
@@ -13635,17 +13633,22 @@
         <v>134</v>
       </c>
       <c r="E40" s="33" t="n">
-        <v>-0.1287</v>
+        <v>-0.1283</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-13478</v>
+        <v>-13473</v>
       </c>
       <c r="G40" s="33" t="n">
-        <v>-0.129</v>
-      </c>
-      <c r="H40" s="0"/>
+        <v>-0.1283</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>-13473</v>
+      </c>
       <c r="I40" s="33" t="n">
-        <v>-0.129</v>
+        <v>-0.1283</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>-13473</v>
       </c>
       <c r="K40" s="33" t="n">
         <v>-0.415799999</v>
@@ -13684,17 +13687,22 @@
         <v>137</v>
       </c>
       <c r="E41" s="33" t="n">
-        <v>0.1289</v>
+        <v>0.1291</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-26210</v>
+        <v>-26209</v>
       </c>
       <c r="G41" s="33" t="n">
-        <v>-0.129</v>
-      </c>
-      <c r="H41" s="0"/>
+        <v>0.1291</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>-26209</v>
+      </c>
       <c r="I41" s="33" t="n">
-        <v>-0.129</v>
+        <v>0.1291</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>-26209</v>
       </c>
       <c r="K41" s="33" t="n">
         <v>-0.3847</v>
@@ -13733,22 +13741,22 @@
         <v>140</v>
       </c>
       <c r="E42" s="37" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="F42" s="35" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="G42" s="37" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="H42" s="35" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="I42" s="37" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="J42" s="35" t="n">
-        <v>190000</v>
+        <v>298590</v>
       </c>
       <c r="K42" s="38" t="n">
         <v>0</v>
@@ -14543,10 +14551,10 @@
         <v>180</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>51.32</v>
+        <v>35.143</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>477354</v>
+        <v>315607</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
@@ -14557,10 +14565,10 @@
       </c>
       <c r="J54" s="28"/>
       <c r="K54" s="58" t="n">
-        <v>46.1092</v>
+        <v>44.962</v>
       </c>
       <c r="L54" s="28" t="n">
-        <v>425265</v>
+        <v>413776</v>
       </c>
       <c r="M54" s="57" t="n">
         <v>46.1094</v>
@@ -15342,8 +15350,8 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17271,12 +17279,12 @@
       </c>
       <c r="E10" s="113" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>51.32</v>
+        <v>35.143</v>
       </c>
       <c r="F10" s="113"/>
       <c r="G10" s="122" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>53.5014000290853</v>
+        <v>37.3244000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17420,7 +17428,7 @@
       </c>
       <c r="E22" s="113" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-16.6463914229833</v>
+        <v>-32.8233914229833</v>
       </c>
       <c r="F22" s="129" t="n">
         <f aca="false">'Modes A-F'!I54</f>
@@ -17428,7 +17436,7 @@
       </c>
       <c r="G22" s="113" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-11.69502924884</v>
+        <v>-27.8720292488399</v>
       </c>
       <c r="I22" s="108"/>
     </row>
@@ -17582,7 +17590,7 @@
       </c>
       <c r="E34" s="113" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-43.6546236638297</v>
+        <v>-59.8316236638297</v>
       </c>
       <c r="F34" s="129" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17590,7 +17598,7 @@
       </c>
       <c r="G34" s="113" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-38.7030007866982</v>
+        <v>-54.8800007866982</v>
       </c>
       <c r="I34" s="108"/>
     </row>

</xml_diff>

<commit_message>
update Modes at beginning of 2018-3
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -47,7 +47,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.35
+          <t>vert = -4.248
 Pitch = 2.8
 lateral = 0.0
 yaw = 0.2</t>
@@ -80,6 +80,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="E56" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vertical = 119
+Pitch = -1.8
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>These values obtained by seeing spot on phosphor screen at upstream end of I0 and downstream end of Ir</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G37" authorId="0">
       <text>
         <r>
@@ -89,7 +113,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.35
+          <t>vert = -4.248
 Pitch = 2.8
 lateral = 0.0
 yaw = 0.2</t>
@@ -132,7 +156,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.35
+          <t>vert = -4.248
 Pitch = 2.8
 lateral = 0.0
 yaw = 0.2</t>
@@ -11588,7 +11612,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="F54" activeCellId="0" sqref="F54"/>
+      <selection pane="bottomRight" activeCell="L58" activeCellId="0" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13449,19 +13473,19 @@
         <v>125</v>
       </c>
       <c r="E37" s="42" t="n">
-        <v>-6.1522</v>
+        <v>-6.0513</v>
       </c>
       <c r="F37" s="20" t="n">
         <v>-55022</v>
       </c>
       <c r="G37" s="42" t="n">
-        <v>-6.1522</v>
+        <v>-6.0513</v>
       </c>
       <c r="H37" s="20" t="n">
         <v>-55022</v>
       </c>
       <c r="I37" s="42" t="n">
-        <v>-6.1522</v>
+        <v>-6.0513</v>
       </c>
       <c r="J37" s="20" t="n">
         <v>-55022</v>
@@ -13525,19 +13549,19 @@
         <v>128</v>
       </c>
       <c r="E38" s="33" t="n">
-        <v>-2.5456</v>
+        <v>-2.4449</v>
       </c>
       <c r="F38" s="0" t="n">
         <v>-34356</v>
       </c>
       <c r="G38" s="33" t="n">
-        <v>-2.5456</v>
+        <v>-2.4449</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>-34356</v>
       </c>
       <c r="I38" s="33" t="n">
-        <v>-2.5456</v>
+        <v>-2.4449</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>-34356</v>
@@ -13579,22 +13603,22 @@
         <v>131</v>
       </c>
       <c r="E39" s="33" t="n">
-        <v>-2.5459</v>
+        <v>-2.4451</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>-28458</v>
+        <v>-54012</v>
       </c>
       <c r="G39" s="33" t="n">
-        <v>-2.5459</v>
+        <v>-2.4451</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>-28458</v>
+        <v>-54012</v>
       </c>
       <c r="I39" s="33" t="n">
-        <v>-2.5459</v>
+        <v>-2.4451</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>-28458</v>
+        <v>-54012</v>
       </c>
       <c r="K39" s="31" t="n">
         <v>6</v>
@@ -13636,7 +13660,7 @@
         <v>-0.1283</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-13473</v>
+        <v>-33350</v>
       </c>
       <c r="G40" s="33" t="n">
         <v>-0.1283</v>
@@ -13690,7 +13714,7 @@
         <v>0.1291</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-26209</v>
+        <v>-27452</v>
       </c>
       <c r="G41" s="33" t="n">
         <v>0.1291</v>
@@ -14698,10 +14722,10 @@
         <v>187</v>
       </c>
       <c r="E56" s="59" t="n">
-        <v>136</v>
+        <v>120.044</v>
       </c>
       <c r="F56" s="25" t="n">
-        <v>10406504</v>
+        <v>9576273</v>
       </c>
       <c r="G56" s="59" t="n">
         <v>24.4104</v>
@@ -14716,10 +14740,10 @@
         <v>4600216</v>
       </c>
       <c r="K56" s="59" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L56" s="23" t="n">
-        <v>10198376</v>
+        <v>10042276</v>
       </c>
       <c r="M56" s="59" t="n">
         <v>132</v>
@@ -14760,10 +14784,10 @@
         <v>190</v>
       </c>
       <c r="E57" s="60" t="n">
-        <v>136</v>
+        <v>117.956</v>
       </c>
       <c r="F57" s="32" t="n">
-        <v>7960975</v>
+        <v>7022101</v>
       </c>
       <c r="G57" s="60" t="n">
         <v>12.81</v>
@@ -14778,10 +14802,10 @@
         <v>1551088</v>
       </c>
       <c r="K57" s="60" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L57" s="32" t="n">
-        <v>7752848</v>
+        <v>7596748</v>
       </c>
       <c r="M57" s="60" t="n">
         <v>132</v>
@@ -14814,10 +14838,10 @@
         <v>193</v>
       </c>
       <c r="E58" s="60" t="n">
-        <v>136</v>
+        <v>117.956</v>
       </c>
       <c r="F58" s="28" t="n">
-        <v>6764228</v>
+        <v>5825353</v>
       </c>
       <c r="G58" s="60" t="n">
         <v>12.81</v>
@@ -14832,10 +14856,10 @@
         <v>354340</v>
       </c>
       <c r="K58" s="60" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L58" s="32" t="n">
-        <v>6556100</v>
+        <v>6400000</v>
       </c>
       <c r="M58" s="60" t="n">
         <v>132</v>
@@ -17186,11 +17210,11 @@
       </c>
       <c r="E4" s="111" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" s="111" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>103.088913266688</v>
+        <v>100.088913266688</v>
       </c>
       <c r="G4" s="112" t="n">
         <f aca="false">'Modes A-F'!O56</f>
@@ -17198,7 +17222,7 @@
       </c>
       <c r="H4" s="113" t="n">
         <f aca="false">G4-F4</f>
-        <v>0.821086733312242</v>
+        <v>3.82108673331224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17215,11 +17239,11 @@
       </c>
       <c r="E5" s="117" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F5" s="117" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>99.6239028716503</v>
+        <v>96.6239028716503</v>
       </c>
       <c r="G5" s="118" t="n">
         <f aca="false">'Modes A-F'!O57</f>
@@ -17227,13 +17251,13 @@
       </c>
       <c r="H5" s="113" t="n">
         <f aca="false">G5-F5</f>
-        <v>0.806097128349677</v>
+        <v>3.80609712834968</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="113" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>0.804688293317862</v>
+        <v>2.80468829331786</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>272</v>
@@ -17300,12 +17324,12 @@
       </c>
       <c r="E11" s="113" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>136</v>
+        <v>117.956</v>
       </c>
       <c r="F11" s="113"/>
       <c r="G11" s="122" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>138.308400030779</v>
+        <v>120.264400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17322,12 +17346,12 @@
       </c>
       <c r="E12" s="123" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>136</v>
+        <v>117.956</v>
       </c>
       <c r="F12" s="123"/>
       <c r="G12" s="124" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>138.539400033859</v>
+        <v>120.495400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17453,7 +17477,7 @@
       </c>
       <c r="E23" s="113" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>63.2392674801944</v>
+        <v>45.1952674801944</v>
       </c>
       <c r="F23" s="129" t="n">
         <f aca="false">'Modes A-F'!I56</f>
@@ -17461,7 +17485,7 @@
       </c>
       <c r="G23" s="113" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>68.5398981480704</v>
+        <v>50.4958981480704</v>
       </c>
       <c r="I23" s="108"/>
     </row>
@@ -17479,7 +17503,7 @@
       </c>
       <c r="E24" s="123" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>54.5188517843995</v>
+        <v>36.4748517843995</v>
       </c>
       <c r="F24" s="130" t="n">
         <f aca="false">'Modes A-F'!I57</f>
@@ -17487,7 +17511,7 @@
       </c>
       <c r="G24" s="131" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>60.454766090482</v>
+        <v>42.410766090482</v>
       </c>
       <c r="H24" s="115"/>
       <c r="I24" s="132"/>
@@ -17615,7 +17639,7 @@
       </c>
       <c r="E35" s="113" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>34.3258777773465</v>
+        <v>16.2818777773465</v>
       </c>
       <c r="F35" s="129" t="n">
         <f aca="false">'Modes A-F'!G56</f>
@@ -17623,7 +17647,7 @@
       </c>
       <c r="G35" s="113" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>39.6267875381681</v>
+        <v>21.5827875381681</v>
       </c>
       <c r="I35" s="108"/>
     </row>
@@ -17641,7 +17665,7 @@
       </c>
       <c r="E36" s="123" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>22.140175674289</v>
+        <v>4.09617567428903</v>
       </c>
       <c r="F36" s="130" t="n">
         <f aca="false">'Modes A-F'!G57</f>
@@ -17649,7 +17673,7 @@
       </c>
       <c r="G36" s="123" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>28.0764025227675</v>
+        <v>10.0324025227675</v>
       </c>
       <c r="H36" s="115"/>
       <c r="I36" s="132"/>

</xml_diff>

<commit_message>
update mode f positions
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -90,8 +90,7 @@
             <charset val="1"/>
           </rPr>
           <t>Vertical = 119
-Pitch = -1.8
-</t>
+Pitch = -1.8</t>
         </r>
         <r>
           <rPr>
@@ -11608,11 +11607,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
-      <selection pane="bottomRight" activeCell="L58" activeCellId="0" sqref="L58"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="P54" activeCellId="0" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14601,10 +14600,10 @@
         <v>425267</v>
       </c>
       <c r="O54" s="58" t="n">
-        <v>19.89</v>
+        <v>19.162</v>
       </c>
       <c r="P54" s="28" t="n">
-        <v>160131</v>
+        <v>155779</v>
       </c>
       <c r="T54" s="58" t="n">
         <v>33.3556</v>
@@ -17190,11 +17189,11 @@
       </c>
       <c r="G3" s="112" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>19.89</v>
+        <v>19.162</v>
       </c>
       <c r="H3" s="113" t="n">
         <f aca="false">G3-F3</f>
-        <v>0.786881018291666</v>
+        <v>0.0588810182917001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17257,7 +17256,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="113" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>2.80468829331786</v>
+        <v>2.56202162665121</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>272</v>

</xml_diff>

<commit_message>
update lookup table for good focus in XRD mode
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -25,6 +25,19 @@
     <author/>
   </authors>
   <commentList>
+    <comment ref="A48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Blocks beam around 31.5</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B48" authorId="0">
       <text>
         <r>
@@ -420,9 +433,9 @@
             <charset val="1"/>
           </rPr>
           <t>vertical = -4.349
- pitch =   2.736
+ Pitch =   3.550
  roll =   0.000
- yaw  =  0.200</t>
+ yaw  =  0.250</t>
         </r>
       </text>
     </comment>
@@ -11607,11 +11620,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="J33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="R36" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
-      <selection pane="bottomRight" activeCell="P54" activeCellId="0" sqref="P54"/>
+      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+      <selection pane="bottomRight" activeCell="C61" activeCellId="0" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13511,10 +13524,10 @@
       <c r="R37" s="26"/>
       <c r="S37" s="26"/>
       <c r="T37" s="55" t="n">
-        <v>-6.11104</v>
+        <v>-6.63518</v>
       </c>
       <c r="U37" s="25" t="n">
-        <v>-54610</v>
+        <v>-59847</v>
       </c>
       <c r="V37" s="0"/>
       <c r="W37" s="0"/>
@@ -13584,10 +13597,10 @@
         <v>51098</v>
       </c>
       <c r="T38" s="30" t="n">
-        <v>-2.58686</v>
+        <v>-2.06272</v>
       </c>
       <c r="U38" s="32" t="n">
-        <v>-34768</v>
+        <v>-29524</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13638,10 +13651,10 @@
         <v>56998</v>
       </c>
       <c r="T39" s="30" t="n">
-        <v>-2.58696</v>
+        <v>-2.06282</v>
       </c>
       <c r="U39" s="32" t="n">
-        <v>-28869</v>
+        <v>-23625</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13692,10 +13705,10 @@
         <v>-16348</v>
       </c>
       <c r="T40" s="30" t="n">
-        <v>-0.1284</v>
+        <v>-0.16105</v>
       </c>
       <c r="U40" s="32" t="n">
-        <v>-13475</v>
+        <v>-13803</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13746,10 +13759,10 @@
         <v>-31347</v>
       </c>
       <c r="T41" s="30" t="n">
-        <v>0.1289</v>
+        <v>0.16105</v>
       </c>
       <c r="U41" s="32" t="n">
-        <v>-26212</v>
+        <v>-25895</v>
       </c>
     </row>
     <row r="42" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14197,10 +14210,10 @@
       <c r="R48" s="26"/>
       <c r="S48" s="26"/>
       <c r="T48" s="53" t="n">
-        <v>33</v>
+        <v>14.4756</v>
       </c>
       <c r="U48" s="54" t="n">
-        <v>288431</v>
+        <v>103188</v>
       </c>
       <c r="V48" s="0"/>
       <c r="W48" s="0"/>
@@ -14593,11 +14606,11 @@
       <c r="L54" s="28" t="n">
         <v>413776</v>
       </c>
-      <c r="M54" s="57" t="n">
-        <v>46.1094</v>
-      </c>
-      <c r="N54" s="26" t="n">
-        <v>425267</v>
+      <c r="M54" s="58" t="n">
+        <v>44.962</v>
+      </c>
+      <c r="N54" s="28" t="n">
+        <v>413776</v>
       </c>
       <c r="O54" s="58" t="n">
         <v>19.162</v>
@@ -14606,10 +14619,10 @@
         <v>155779</v>
       </c>
       <c r="T54" s="58" t="n">
-        <v>33.3556</v>
+        <v>51.2907</v>
       </c>
       <c r="U54" s="28" t="n">
-        <v>297749</v>
+        <v>477063</v>
       </c>
       <c r="V54" s="0"/>
       <c r="W54" s="0"/>
@@ -14745,10 +14758,10 @@
         <v>10042276</v>
       </c>
       <c r="M56" s="59" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N56" s="23" t="n">
-        <v>10198376</v>
+        <v>10042276</v>
       </c>
       <c r="O56" s="59" t="n">
         <v>103.91</v>
@@ -14760,10 +14773,10 @@
       <c r="R56" s="26"/>
       <c r="S56" s="26"/>
       <c r="T56" s="55" t="n">
-        <v>117.533</v>
+        <v>136.324</v>
       </c>
       <c r="U56" s="25" t="n">
-        <v>9445608</v>
+        <v>10423373</v>
       </c>
       <c r="V56" s="0"/>
       <c r="W56" s="0"/>
@@ -14807,10 +14820,10 @@
         <v>7596748</v>
       </c>
       <c r="M57" s="60" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N57" s="32" t="n">
-        <v>7752848</v>
+        <v>7596748</v>
       </c>
       <c r="O57" s="60" t="n">
         <v>100.43</v>
@@ -14819,10 +14832,10 @@
         <v>6110187</v>
       </c>
       <c r="T57" s="30" t="n">
-        <v>115.685</v>
+        <v>136.35</v>
       </c>
       <c r="U57" s="32" t="n">
-        <v>6903924</v>
+        <v>7979171</v>
       </c>
     </row>
     <row r="58" s="26" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14861,10 +14874,10 @@
         <v>6400000</v>
       </c>
       <c r="M58" s="60" t="n">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="N58" s="32" t="n">
-        <v>6556100</v>
+        <v>6400000</v>
       </c>
       <c r="O58" s="60" t="n">
         <v>100.43</v>
@@ -14873,10 +14886,10 @@
         <v>4913439</v>
       </c>
       <c r="T58" s="27" t="n">
-        <v>115.685</v>
+        <v>136.35</v>
       </c>
       <c r="U58" s="28" t="n">
-        <v>5707176</v>
+        <v>6782423</v>
       </c>
       <c r="V58" s="0"/>
       <c r="W58" s="0"/>

</xml_diff>

<commit_message>
update modes and cheatsheet
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -60,10 +60,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.248
-Pitch = 2.8
-lateral = 0.0
-yaw = 0.2</t>
+          <t>vert = -4.148
+Pitch = 2.5
+lateral = 0.01
+yaw = 0.285</t>
         </r>
       </text>
     </comment>
@@ -102,8 +102,9 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Vertical = 119
-Pitch = -1.8</t>
+          <t>Vertical = 110.75
+Pitch = -1.465
+</t>
         </r>
         <r>
           <rPr>
@@ -125,10 +126,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.248
-Pitch = 2.8
-lateral = 0.0
-yaw = 0.2</t>
+          <t>vert = -4.148
+Pitch = 2.5
+lateral = 0.01
+yaw = 0.285</t>
         </r>
       </text>
     </comment>
@@ -168,10 +169,10 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -4.248
-Pitch = 2.8
-lateral = 0.0
-yaw = 0.2</t>
+          <t>vert = -4.148
+Pitch = 2.5
+lateral = 0.01
+yaw = 0.285</t>
         </r>
       </text>
     </comment>
@@ -184,7 +185,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>vert = -7.25
+          <t>Vert = -8.9
 pitch = -3.5</t>
         </r>
       </text>
@@ -198,7 +199,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Rh/Pt stripe</t>
+          <t>Bare Si stripe</t>
         </r>
       </text>
     </comment>
@@ -501,7 +502,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4194" uniqueCount="3307">
   <si>
-    <t>in /home/bravel/commissioning/CRS, dosh pvs.sh | xclip, then paste into appropriate column</t>
+    <t>  in /home/bravel/commissioning/CRS, do sh pvs.sh | xclip, then paste into appropriate column</t>
   </si>
   <si>
     <t>Mode A</t>
@@ -10697,7 +10698,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10718,6 +10719,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3333"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFF2DED5"/>
       </patternFill>
@@ -10729,7 +10742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="35">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -10847,6 +10860,24 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -10987,7 +11018,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11005,7 +11036,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -11216,11 +11247,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11240,23 +11275,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11264,19 +11299,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11288,7 +11323,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11296,7 +11331,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11304,7 +11339,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11312,19 +11347,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11336,11 +11371,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="24" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11352,15 +11387,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11392,19 +11427,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11412,7 +11447,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11420,11 +11455,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11436,7 +11471,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11444,39 +11479,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11484,7 +11515,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11508,19 +11543,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="30" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11528,7 +11563,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11553,7 +11588,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFCCFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000CC"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -11620,11 +11655,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="R36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="R1" activeCellId="0" sqref="R1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="C61" activeCellId="0" sqref="C61"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="bottomRight" activeCell="G33" activeCellId="0" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -13485,22 +13520,22 @@
         <v>125</v>
       </c>
       <c r="E37" s="42" t="n">
-        <v>-6.0513</v>
+        <v>-5.85828</v>
       </c>
       <c r="F37" s="20" t="n">
-        <v>-55022</v>
+        <v>-52086</v>
       </c>
       <c r="G37" s="42" t="n">
-        <v>-6.0513</v>
+        <v>-5.85828</v>
       </c>
       <c r="H37" s="20" t="n">
-        <v>-55022</v>
+        <v>-52086</v>
       </c>
       <c r="I37" s="42" t="n">
-        <v>-6.0513</v>
+        <v>-5.85828</v>
       </c>
       <c r="J37" s="20" t="n">
-        <v>-55022</v>
+        <v>-52086</v>
       </c>
       <c r="K37" s="43" t="n">
         <v>6</v>
@@ -13561,22 +13596,22 @@
         <v>128</v>
       </c>
       <c r="E38" s="33" t="n">
-        <v>-2.4449</v>
+        <v>-2.63817</v>
       </c>
       <c r="F38" s="0" t="n">
-        <v>-34356</v>
+        <v>-35283</v>
       </c>
       <c r="G38" s="33" t="n">
-        <v>-2.4449</v>
+        <v>-2.63817</v>
       </c>
       <c r="H38" s="0" t="n">
-        <v>-34356</v>
+        <v>-35283</v>
       </c>
       <c r="I38" s="33" t="n">
-        <v>-2.4449</v>
+        <v>-2.63817</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>-34356</v>
+        <v>-35283</v>
       </c>
       <c r="K38" s="31" t="n">
         <v>6</v>
@@ -13615,22 +13650,22 @@
         <v>131</v>
       </c>
       <c r="E39" s="33" t="n">
-        <v>-2.4451</v>
+        <v>-2.63837</v>
       </c>
       <c r="F39" s="0" t="n">
-        <v>-54012</v>
+        <v>-29385</v>
       </c>
       <c r="G39" s="33" t="n">
-        <v>-2.4451</v>
+        <v>-2.63837</v>
       </c>
       <c r="H39" s="0" t="n">
-        <v>-54012</v>
+        <v>-29385</v>
       </c>
       <c r="I39" s="33" t="n">
-        <v>-2.4451</v>
+        <v>-2.63837</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>-54012</v>
+        <v>-29385</v>
       </c>
       <c r="K39" s="31" t="n">
         <v>6</v>
@@ -13669,22 +13704,22 @@
         <v>134</v>
       </c>
       <c r="E40" s="33" t="n">
-        <v>-0.1283</v>
+        <v>-0.1735</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-33350</v>
+        <v>-13926</v>
       </c>
       <c r="G40" s="33" t="n">
-        <v>-0.1283</v>
+        <v>-0.1735</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>-13473</v>
+        <v>-13926</v>
       </c>
       <c r="I40" s="33" t="n">
-        <v>-0.1283</v>
+        <v>-0.1735</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>-13473</v>
+        <v>-13926</v>
       </c>
       <c r="K40" s="33" t="n">
         <v>-0.415799999</v>
@@ -13723,22 +13758,22 @@
         <v>137</v>
       </c>
       <c r="E41" s="33" t="n">
-        <v>0.1291</v>
+        <v>0.1936</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-27452</v>
+        <v>-25564</v>
       </c>
       <c r="G41" s="33" t="n">
-        <v>0.1291</v>
+        <v>0.1936</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>-26209</v>
+        <v>-25564</v>
       </c>
       <c r="I41" s="33" t="n">
-        <v>0.1291</v>
+        <v>0.1936</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>-26209</v>
+        <v>-25564</v>
       </c>
       <c r="K41" s="33" t="n">
         <v>-0.3847</v>
@@ -13777,22 +13812,22 @@
         <v>140</v>
       </c>
       <c r="E42" s="37" t="n">
-        <v>298590</v>
+        <v>209762</v>
       </c>
       <c r="F42" s="35" t="n">
-        <v>298590</v>
+        <v>209763</v>
       </c>
       <c r="G42" s="37" t="n">
-        <v>298590</v>
+        <v>209762</v>
       </c>
       <c r="H42" s="35" t="n">
-        <v>298590</v>
+        <v>209763</v>
       </c>
       <c r="I42" s="37" t="n">
-        <v>298590</v>
+        <v>209762</v>
       </c>
       <c r="J42" s="35" t="n">
-        <v>298590</v>
+        <v>209763</v>
       </c>
       <c r="K42" s="38" t="n">
         <v>0</v>
@@ -13816,10 +13851,10 @@
       <c r="R42" s="26"/>
       <c r="S42" s="26"/>
       <c r="T42" s="56" t="n">
-        <v>163788</v>
+        <v>119996</v>
       </c>
       <c r="U42" s="45" t="n">
-        <v>163789</v>
+        <v>119996</v>
       </c>
       <c r="V42" s="0"/>
       <c r="W42" s="0"/>
@@ -13867,10 +13902,10 @@
         <v>3208</v>
       </c>
       <c r="I43" s="0" t="n">
-        <v>-6.3492</v>
+        <v>-9.33327</v>
       </c>
       <c r="J43" s="20" t="n">
-        <v>-45292</v>
+        <v>-75133</v>
       </c>
       <c r="K43" s="43" t="n">
         <v>-1.1672</v>
@@ -13943,10 +13978,10 @@
         <v>-11313</v>
       </c>
       <c r="I44" s="0" t="n">
-        <v>-8.1509</v>
+        <v>-11.6676</v>
       </c>
       <c r="J44" s="0" t="n">
-        <v>-77809</v>
+        <v>-112976</v>
       </c>
       <c r="K44" s="31" t="n">
         <v>1.1673</v>
@@ -13997,10 +14032,10 @@
         <v>-12617</v>
       </c>
       <c r="I45" s="0" t="n">
-        <v>-8.1507</v>
+        <v>-11.668</v>
       </c>
       <c r="J45" s="0" t="n">
-        <v>-79107</v>
+        <v>-114280</v>
       </c>
       <c r="K45" s="31" t="n">
         <v>1.1673</v>
@@ -14051,10 +14086,10 @@
         <v>-167785</v>
       </c>
       <c r="I46" s="33" t="n">
-        <v>15.0024</v>
+        <v>-15</v>
       </c>
       <c r="J46" s="0" t="n">
-        <v>132223</v>
+        <v>-167779</v>
       </c>
       <c r="K46" s="31" t="n">
         <v>15</v>
@@ -14105,10 +14140,10 @@
         <v>-185598</v>
       </c>
       <c r="I47" s="37" t="n">
-        <v>15</v>
+        <v>-15</v>
       </c>
       <c r="J47" s="35" t="n">
-        <v>114409</v>
+        <v>-185586</v>
       </c>
       <c r="K47" s="38" t="n">
         <v>15.0002</v>
@@ -14183,10 +14218,10 @@
         <v>-708892</v>
       </c>
       <c r="I48" s="52" t="n">
-        <v>-48.1824</v>
+        <v>-35.8205</v>
       </c>
       <c r="J48" s="51" t="n">
-        <v>-523391</v>
+        <v>-399880</v>
       </c>
       <c r="K48" s="53" t="n">
         <v>27.1</v>
@@ -14587,32 +14622,34 @@
         <v>180</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>35.143</v>
+        <v>28.1862</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>315607</v>
+        <v>246016</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
       </c>
-      <c r="H54" s="28"/>
-      <c r="I54" s="58" t="n">
-        <v>-55.188</v>
-      </c>
-      <c r="J54" s="28"/>
-      <c r="K54" s="58" t="n">
+      <c r="H54" s="59"/>
+      <c r="I54" s="57" t="n">
+        <v>-20.5991</v>
+      </c>
+      <c r="J54" s="28" t="n">
+        <v>-241810</v>
+      </c>
+      <c r="K54" s="57" t="n">
         <v>44.962</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>413776</v>
       </c>
-      <c r="M54" s="58" t="n">
+      <c r="M54" s="57" t="n">
         <v>44.962</v>
       </c>
       <c r="N54" s="28" t="n">
         <v>413776</v>
       </c>
-      <c r="O54" s="58" t="n">
+      <c r="O54" s="57" t="n">
         <v>19.162</v>
       </c>
       <c r="P54" s="28" t="n">
@@ -14733,37 +14770,37 @@
       <c r="D56" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E56" s="59" t="n">
-        <v>120.044</v>
+      <c r="E56" s="60" t="n">
+        <v>111.596</v>
       </c>
       <c r="F56" s="25" t="n">
-        <v>9576273</v>
-      </c>
-      <c r="G56" s="59" t="n">
+        <v>9136682</v>
+      </c>
+      <c r="G56" s="60" t="n">
         <v>24.4104</v>
       </c>
       <c r="H56" s="23" t="n">
         <v>4600216</v>
       </c>
-      <c r="I56" s="59" t="n">
-        <v>24.4104</v>
+      <c r="I56" s="60" t="n">
+        <v>58.9099</v>
       </c>
       <c r="J56" s="23" t="n">
-        <v>4600216</v>
-      </c>
-      <c r="K56" s="59" t="n">
+        <v>6395313</v>
+      </c>
+      <c r="K56" s="60" t="n">
         <v>129</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>10042276</v>
       </c>
-      <c r="M56" s="59" t="n">
+      <c r="M56" s="60" t="n">
         <v>129</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>10042276</v>
       </c>
-      <c r="O56" s="59" t="n">
+      <c r="O56" s="60" t="n">
         <v>103.91</v>
       </c>
       <c r="P56" s="23" t="n">
@@ -14795,37 +14832,37 @@
       <c r="D57" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="E57" s="60" t="n">
-        <v>117.956</v>
+      <c r="E57" s="61" t="n">
+        <v>109.896</v>
       </c>
       <c r="F57" s="32" t="n">
-        <v>7022101</v>
-      </c>
-      <c r="G57" s="60" t="n">
+        <v>6602717</v>
+      </c>
+      <c r="G57" s="61" t="n">
         <v>12.81</v>
       </c>
       <c r="H57" s="32" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="60" t="n">
-        <v>12.81</v>
+      <c r="I57" s="61" t="n">
+        <v>50.2501</v>
       </c>
       <c r="J57" s="32" t="n">
-        <v>1551088</v>
-      </c>
-      <c r="K57" s="60" t="n">
+        <v>3499194</v>
+      </c>
+      <c r="K57" s="61" t="n">
         <v>129</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7596748</v>
       </c>
-      <c r="M57" s="60" t="n">
+      <c r="M57" s="61" t="n">
         <v>129</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7596748</v>
       </c>
-      <c r="O57" s="60" t="n">
+      <c r="O57" s="61" t="n">
         <v>100.43</v>
       </c>
       <c r="P57" s="32" t="n">
@@ -14849,37 +14886,37 @@
       <c r="D58" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E58" s="60" t="n">
-        <v>117.956</v>
+      <c r="E58" s="61" t="n">
+        <v>109.896</v>
       </c>
       <c r="F58" s="28" t="n">
-        <v>5825353</v>
-      </c>
-      <c r="G58" s="60" t="n">
+        <v>5405969</v>
+      </c>
+      <c r="G58" s="61" t="n">
         <v>12.81</v>
       </c>
       <c r="H58" s="32" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="60" t="n">
-        <v>12.81</v>
+      <c r="I58" s="61" t="n">
+        <v>50.2501</v>
       </c>
       <c r="J58" s="32" t="n">
-        <v>354340</v>
-      </c>
-      <c r="K58" s="60" t="n">
+        <v>2302446</v>
+      </c>
+      <c r="K58" s="61" t="n">
         <v>129</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6400000</v>
       </c>
-      <c r="M58" s="60" t="n">
+      <c r="M58" s="61" t="n">
         <v>129</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6400000</v>
       </c>
-      <c r="O58" s="60" t="n">
+      <c r="O58" s="61" t="n">
         <v>100.43</v>
       </c>
       <c r="P58" s="30" t="n">
@@ -14908,43 +14945,43 @@
       <c r="D59" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="E59" s="60" t="n">
+      <c r="E59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="F59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="G59" s="60" t="n">
+      <c r="G59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="H59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="I59" s="60" t="n">
+      <c r="I59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="J59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="K59" s="60" t="n">
+      <c r="K59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="L59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="M59" s="60" t="n">
+      <c r="M59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="N59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="O59" s="60" t="n">
+      <c r="O59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="P59" s="28" t="n">
         <v>-332000</v>
       </c>
-      <c r="T59" s="60" t="n">
+      <c r="T59" s="61" t="n">
         <v>-4.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -14962,46 +14999,46 @@
       <c r="D60" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="E60" s="61" t="n">
+      <c r="E60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="F60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="G60" s="61" t="n">
+      <c r="G60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="H60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="I60" s="61" t="n">
+      <c r="I60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="J60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="K60" s="61" t="n">
+      <c r="K60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="L60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="M60" s="61" t="n">
+      <c r="M60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="N60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="O60" s="61" t="n">
+      <c r="O60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="P60" s="47" t="n">
         <v>130000</v>
       </c>
-      <c r="Q60" s="62"/>
-      <c r="R60" s="62"/>
-      <c r="S60" s="62"/>
-      <c r="T60" s="61" t="n">
+      <c r="Q60" s="63"/>
+      <c r="R60" s="63"/>
+      <c r="S60" s="63"/>
+      <c r="T60" s="62" t="n">
         <v>16.9</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15014,52 +15051,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="63" t="s">
+      <c r="A61" s="64" t="s">
         <v>200</v>
       </c>
-      <c r="B61" s="64" t="s">
+      <c r="B61" s="65" t="s">
         <v>201</v>
       </c>
-      <c r="C61" s="65" t="s">
+      <c r="C61" s="66" t="s">
         <v>202</v>
       </c>
-      <c r="D61" s="65" t="s">
+      <c r="D61" s="66" t="s">
         <v>203</v>
       </c>
-      <c r="E61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="67" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="66" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="67" t="n">
+      <c r="E61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="68" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15070,8 +15107,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="63"/>
-      <c r="B62" s="68" t="s">
+      <c r="A62" s="64"/>
+      <c r="B62" s="69" t="s">
         <v>204</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15124,8 +15161,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="63"/>
-      <c r="B63" s="68" t="s">
+      <c r="A63" s="64"/>
+      <c r="B63" s="69" t="s">
         <v>207</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15178,8 +15215,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="63"/>
-      <c r="B64" s="68" t="s">
+      <c r="A64" s="64"/>
+      <c r="B64" s="69" t="s">
         <v>210</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15232,8 +15269,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="63"/>
-      <c r="B65" s="68" t="s">
+      <c r="A65" s="64"/>
+      <c r="B65" s="69" t="s">
         <v>213</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15286,53 +15323,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="63"/>
-      <c r="B66" s="69" t="s">
+      <c r="A66" s="64"/>
+      <c r="B66" s="70" t="s">
         <v>216</v>
       </c>
-      <c r="C66" s="70" t="s">
+      <c r="C66" s="71" t="s">
         <v>217</v>
       </c>
-      <c r="D66" s="70" t="s">
+      <c r="D66" s="71" t="s">
         <v>218</v>
       </c>
-      <c r="E66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="71" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="61" t="n">
+      <c r="E66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="62" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15392,34 +15429,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="73" width="3.0969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="73" width="13.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="73" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="74" width="3.0969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="74" width="13.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="74" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73"/>
+    <row r="1" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="74"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="AMJ1" s="73"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="AMJ1" s="74"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="76" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16440,168 +16477,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="80" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="76"/>
-      <c r="B3" s="77"/>
-      <c r="C3" s="78" t="s">
+    <row r="3" s="81" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="77"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="79" t="s">
         <v>221</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="80" t="s">
         <v>222</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="AMJ3" s="76"/>
-    </row>
-    <row r="4" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="73"/>
-      <c r="B4" s="77" t="s">
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="AMJ3" s="77"/>
+    </row>
+    <row r="4" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="74"/>
+      <c r="B4" s="78" t="s">
         <v>223</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73" t="n">
+      <c r="C4" s="74"/>
+      <c r="D4" s="74" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="81" t="n">
+      <c r="E4" s="82" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="AMJ4" s="73"/>
-    </row>
-    <row r="5" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="73"/>
-      <c r="B5" s="77" t="s">
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="AMJ4" s="74"/>
+    </row>
+    <row r="5" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="74"/>
+      <c r="B5" s="78" t="s">
         <v>224</v>
       </c>
-      <c r="C5" s="73" t="s">
+      <c r="C5" s="74" t="s">
         <v>225</v>
       </c>
-      <c r="D5" s="73" t="n">
+      <c r="D5" s="74" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="81"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="AMJ5" s="73"/>
-    </row>
-    <row r="6" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="73"/>
-      <c r="B6" s="77" t="s">
+      <c r="E5" s="82"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="AMJ5" s="74"/>
+    </row>
+    <row r="6" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="74"/>
+      <c r="B6" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="74" t="s">
         <v>227</v>
       </c>
-      <c r="D6" s="73" t="n">
+      <c r="D6" s="74" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="81"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="AMJ6" s="73"/>
-    </row>
-    <row r="7" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="73"/>
-      <c r="B7" s="77" t="s">
+      <c r="E6" s="82"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="74"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="74"/>
+      <c r="AMJ6" s="74"/>
+    </row>
+    <row r="7" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="74"/>
+      <c r="B7" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="C7" s="73" t="s">
+      <c r="C7" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="73" t="n">
+      <c r="D7" s="74" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="73"/>
-      <c r="L7" s="73"/>
-      <c r="AMJ7" s="73"/>
-    </row>
-    <row r="8" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="73"/>
-      <c r="B8" s="77" t="s">
+      <c r="E7" s="82"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="AMJ7" s="74"/>
+    </row>
+    <row r="8" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="74"/>
+      <c r="B8" s="78" t="s">
         <v>230</v>
       </c>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="74" t="s">
         <v>231</v>
       </c>
-      <c r="D8" s="73" t="n">
+      <c r="D8" s="74" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="81"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="73"/>
-      <c r="I8" s="73"/>
-      <c r="J8" s="73"/>
-      <c r="K8" s="73"/>
-      <c r="L8" s="73"/>
-      <c r="AMJ8" s="73"/>
-    </row>
-    <row r="9" s="74" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="73"/>
-      <c r="B9" s="77" t="s">
+      <c r="E8" s="82"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="AMJ8" s="74"/>
+    </row>
+    <row r="9" s="75" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="74"/>
+      <c r="B9" s="78" t="s">
         <v>232</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73" t="n">
+      <c r="C9" s="74"/>
+      <c r="D9" s="74" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="81"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="73"/>
-      <c r="H9" s="73"/>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="73"/>
-      <c r="AMJ9" s="73"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="AMJ9" s="74"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="82" t="s">
+      <c r="B10" s="83" t="s">
         <v>233</v>
       </c>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83" t="n">
+      <c r="C10" s="84"/>
+      <c r="D10" s="84" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="84"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="87"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16610,8 +16647,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="87"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16620,82 +16657,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="88" t="s">
         <v>234</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="88" t="s">
+      <c r="B14" s="89" t="s">
         <v>235</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="90" t="s">
         <v>236</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="81"/>
+      <c r="E14" s="82"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="78" t="s">
         <v>223</v>
       </c>
-      <c r="C15" s="73" t="n">
+      <c r="C15" s="74" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="81"/>
+      <c r="E15" s="82"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="78" t="s">
         <v>237</v>
       </c>
-      <c r="C16" s="90" t="n">
+      <c r="C16" s="91" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="81"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="78" t="s">
         <v>238</v>
       </c>
-      <c r="C17" s="73" t="n">
+      <c r="C17" s="74" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="81"/>
+      <c r="E17" s="82"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="82" t="s">
+      <c r="B18" s="83" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="83" t="n">
+      <c r="C18" s="84" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
+      <c r="D18" s="84"/>
+      <c r="E18" s="85"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16722,206 +16759,206 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="88"/>
+      <c r="E21" s="88"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="91" t="s">
+      <c r="B22" s="92" t="s">
         <v>240</v>
       </c>
-      <c r="C22" s="91"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="85" t="s">
+      <c r="C22" s="92"/>
+      <c r="D22" s="75"/>
+      <c r="E22" s="86" t="s">
         <v>241</v>
       </c>
-      <c r="F22" s="85"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="92" t="s">
+      <c r="F22" s="86"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="93" t="s">
         <v>242</v>
       </c>
-      <c r="I22" s="92"/>
+      <c r="I22" s="93"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="89" t="s">
         <v>243</v>
       </c>
-      <c r="C23" s="89" t="s">
+      <c r="C23" s="90" t="s">
         <v>236</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="74" t="s">
+      <c r="E23" s="75" t="s">
         <v>243</v>
       </c>
-      <c r="F23" s="89" t="s">
+      <c r="F23" s="90" t="s">
         <v>236</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="74" t="s">
+      <c r="H23" s="75" t="s">
         <v>244</v>
       </c>
-      <c r="I23" s="93" t="s">
+      <c r="I23" s="94" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="77" t="s">
+      <c r="B24" s="78" t="s">
         <v>245</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="73" t="s">
+      <c r="E24" s="74" t="s">
         <v>245</v>
       </c>
-      <c r="F24" s="73" t="n">
+      <c r="F24" s="74" t="n">
         <v>25.5</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="73" t="s">
+      <c r="H24" s="74" t="s">
         <v>246</v>
       </c>
-      <c r="I24" s="81" t="n">
+      <c r="I24" s="82" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="77" t="s">
+      <c r="B25" s="78" t="s">
         <v>247</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="73" t="s">
+      <c r="E25" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="73" t="n">
+      <c r="F25" s="74" t="n">
         <v>-42.6</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="73" t="s">
+      <c r="H25" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="I25" s="81" t="n">
+      <c r="I25" s="82" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="77" t="s">
+      <c r="B26" s="78" t="s">
         <v>249</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="73" t="s">
+      <c r="E26" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="F26" s="73" t="n">
+      <c r="F26" s="74" t="n">
         <v>-17.25</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="73" t="s">
+      <c r="H26" s="74" t="s">
         <v>250</v>
       </c>
-      <c r="I26" s="81" t="n">
+      <c r="I26" s="82" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="77" t="s">
+      <c r="B27" s="78" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="73" t="n">
+      <c r="C27" s="74" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="73" t="s">
+      <c r="E27" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="F27" s="73" t="n">
+      <c r="F27" s="74" t="n">
         <v>46.1092</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="81"/>
+      <c r="I27" s="82"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="77" t="s">
+      <c r="B28" s="78" t="s">
         <v>252</v>
       </c>
-      <c r="C28" s="73" t="n">
+      <c r="C28" s="74" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="73" t="s">
+      <c r="E28" s="74" t="s">
         <v>252</v>
       </c>
-      <c r="F28" s="73" t="n">
+      <c r="F28" s="74" t="n">
         <v>46.1092</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="81"/>
+      <c r="I28" s="82"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="77" t="s">
+      <c r="B29" s="78" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="73" t="n">
+      <c r="C29" s="74" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="73" t="s">
+      <c r="E29" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="F29" s="73" t="n">
+      <c r="F29" s="74" t="n">
         <v>19.5956</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="81"/>
+      <c r="I29" s="82"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="78" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="73" t="n">
+      <c r="C30" s="74" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="73" t="s">
+      <c r="E30" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="F30" s="73" t="n">
+      <c r="F30" s="74" t="n">
         <v>32.4638</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="81"/>
+      <c r="I30" s="82"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="82" t="s">
+      <c r="B31" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="83" t="n">
+      <c r="C31" s="84" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="83"/>
-      <c r="E31" s="83"/>
-      <c r="F31" s="83"/>
-      <c r="G31" s="83"/>
-      <c r="H31" s="83"/>
-      <c r="I31" s="84"/>
+      <c r="D31" s="84"/>
+      <c r="E31" s="84"/>
+      <c r="F31" s="84"/>
+      <c r="G31" s="84"/>
+      <c r="H31" s="84"/>
+      <c r="I31" s="85"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -16979,14 +17016,14 @@
       <c r="D1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="95" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="94"/>
-      <c r="G1" s="95" t="s">
+      <c r="F1" s="95"/>
+      <c r="G1" s="96" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="95"/>
+      <c r="H1" s="96"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17012,25 +17049,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="98" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="97" t="n">
+      <c r="E3" s="98" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="97" t="n">
+      <c r="F3" s="98" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="98" t="n">
+      <c r="G3" s="99" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="99" t="n">
+      <c r="H3" s="100" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17093,11 +17130,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="100" t="s">
+      <c r="I6" s="101" t="s">
         <v>260</v>
       </c>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
+      <c r="J6" s="101"/>
+      <c r="K6" s="101"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17109,9 +17146,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
+      <c r="I7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17153,26 +17190,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="101"/>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="103" t="s">
+      <c r="A1" s="102"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="104" t="s">
         <v>262</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="105" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="106" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="106"/>
-      <c r="D2" s="107" t="s">
+      <c r="A2" s="107"/>
+      <c r="D2" s="108" t="s">
         <v>265</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17181,93 +17218,93 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="108"/>
+      <c r="G2" s="109"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="108" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="110" t="n">
+      <c r="E3" s="111" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="111" t="n">
+      <c r="F3" s="112" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="112" t="n">
+      <c r="G3" s="113" t="n">
         <f aca="false">'Modes A-F'!O54</f>
         <v>19.162</v>
       </c>
-      <c r="H3" s="113" t="n">
+      <c r="H3" s="114" t="n">
         <f aca="false">G3-F3</f>
         <v>0.0588810182917001</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="110" t="s">
         <v>268</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="107" t="s">
+      <c r="D4" s="108" t="s">
         <v>269</v>
       </c>
-      <c r="E4" s="111" t="n">
+      <c r="E4" s="112" t="n">
         <f aca="false">'Modes A-F'!K56</f>
         <v>129</v>
       </c>
-      <c r="F4" s="111" t="n">
+      <c r="F4" s="112" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
         <v>100.088913266688</v>
       </c>
-      <c r="G4" s="112" t="n">
+      <c r="G4" s="113" t="n">
         <f aca="false">'Modes A-F'!O56</f>
         <v>103.91</v>
       </c>
-      <c r="H4" s="113" t="n">
+      <c r="H4" s="114" t="n">
         <f aca="false">G4-F4</f>
         <v>3.82108673331224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="114" t="s">
+      <c r="A5" s="115" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="115" t="n">
+      <c r="B5" s="116" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="115"/>
-      <c r="D5" s="116" t="s">
+      <c r="C5" s="116"/>
+      <c r="D5" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E5" s="117" t="n">
+      <c r="E5" s="118" t="n">
         <f aca="false">'Modes A-F'!K57</f>
         <v>129</v>
       </c>
-      <c r="F5" s="117" t="n">
+      <c r="F5" s="118" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
         <v>96.6239028716503</v>
       </c>
-      <c r="G5" s="118" t="n">
+      <c r="G5" s="119" t="n">
         <f aca="false">'Modes A-F'!O57</f>
         <v>100.43</v>
       </c>
-      <c r="H5" s="113" t="n">
+      <c r="H5" s="114" t="n">
         <f aca="false">G5-F5</f>
         <v>3.80609712834968</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="113" t="n">
+      <c r="H6" s="114" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
         <v>2.56202162665121</v>
       </c>
@@ -17276,419 +17313,419 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="119" t="s">
+      <c r="A8" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="119"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="120" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="121" t="s">
         <v>273</v>
       </c>
-      <c r="G8" s="121" t="n">
+      <c r="G8" s="122" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="106"/>
-      <c r="D9" s="107" t="s">
+      <c r="A9" s="107"/>
+      <c r="D9" s="108" t="s">
         <v>265</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="108" t="n">
+      <c r="G9" s="109" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="110" t="s">
         <v>274</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="107" t="s">
+      <c r="D10" s="108" t="s">
         <v>267</v>
       </c>
-      <c r="E10" s="113" t="n">
+      <c r="E10" s="114" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>35.143</v>
-      </c>
-      <c r="F10" s="113"/>
-      <c r="G10" s="122" t="n">
+        <v>28.1862</v>
+      </c>
+      <c r="F10" s="114"/>
+      <c r="G10" s="123" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>37.3244000290853</v>
+        <v>30.3676000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="110" t="s">
         <v>275</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="107" t="s">
+      <c r="D11" s="108" t="s">
         <v>269</v>
       </c>
-      <c r="E11" s="113" t="n">
+      <c r="E11" s="114" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>117.956</v>
-      </c>
-      <c r="F11" s="113"/>
-      <c r="G11" s="122" t="n">
+        <v>109.896</v>
+      </c>
+      <c r="F11" s="114"/>
+      <c r="G11" s="123" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>120.264400030779</v>
+        <v>112.204400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="114" t="s">
+      <c r="A12" s="115" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="115" t="n">
+      <c r="B12" s="116" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="115"/>
-      <c r="D12" s="116" t="s">
+      <c r="C12" s="116"/>
+      <c r="D12" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E12" s="123" t="n">
+      <c r="E12" s="124" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>117.956</v>
-      </c>
-      <c r="F12" s="123"/>
-      <c r="G12" s="124" t="n">
+        <v>109.896</v>
+      </c>
+      <c r="F12" s="124"/>
+      <c r="G12" s="125" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>120.495400033859</v>
+        <v>112.435400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="120" t="s">
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="121" t="s">
         <v>273</v>
       </c>
-      <c r="G16" s="102" t="n">
+      <c r="G16" s="103" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="102"/>
-      <c r="I16" s="121"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="122"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="106"/>
-      <c r="D17" s="107" t="s">
+      <c r="A17" s="107"/>
+      <c r="D17" s="108" t="s">
         <v>265</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="62" t="n">
+      <c r="G17" s="63" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="125" t="s">
+      <c r="H17" s="126" t="s">
         <v>277</v>
       </c>
-      <c r="I17" s="108" t="n">
+      <c r="I17" s="109" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="109" t="s">
+      <c r="A18" s="110" t="s">
         <v>278</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="107" t="s">
+      <c r="D18" s="108" t="s">
         <v>279</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="126" t="n">
+      <c r="G18" s="127" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="108"/>
+      <c r="I18" s="109"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="106"/>
-      <c r="D19" s="107" t="s">
+      <c r="A19" s="107"/>
+      <c r="D19" s="108" t="s">
         <v>280</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="62" t="n">
+      <c r="G19" s="63" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="108"/>
+      <c r="I19" s="109"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="106"/>
-      <c r="D20" s="107"/>
-      <c r="G20" s="127" t="s">
+      <c r="A20" s="107"/>
+      <c r="D20" s="108"/>
+      <c r="G20" s="128" t="s">
         <v>281</v>
       </c>
-      <c r="I20" s="108"/>
+      <c r="I20" s="109"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="106"/>
-      <c r="F21" s="128" t="s">
+      <c r="A21" s="107"/>
+      <c r="F21" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="I21" s="108"/>
+      <c r="I21" s="109"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="109" t="s">
+      <c r="A22" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="107" t="s">
+      <c r="D22" s="108" t="s">
         <v>267</v>
       </c>
-      <c r="E22" s="113" t="n">
+      <c r="E22" s="114" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-32.8233914229833</v>
-      </c>
-      <c r="F22" s="129" t="n">
+        <v>-39.7801914229833</v>
+      </c>
+      <c r="F22" s="130" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-55.188</v>
-      </c>
-      <c r="G22" s="113" t="n">
+        <v>-20.5991</v>
+      </c>
+      <c r="G22" s="114" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-27.8720292488399</v>
-      </c>
-      <c r="I22" s="108"/>
+        <v>-34.82882924884</v>
+      </c>
+      <c r="I22" s="109"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="109" t="s">
+      <c r="A23" s="110" t="s">
         <v>268</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="107" t="s">
+      <c r="D23" s="108" t="s">
         <v>269</v>
       </c>
-      <c r="E23" s="113" t="n">
+      <c r="E23" s="114" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>45.1952674801944</v>
-      </c>
-      <c r="F23" s="129" t="n">
+        <v>37.1352674801944</v>
+      </c>
+      <c r="F23" s="130" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>24.4104</v>
-      </c>
-      <c r="G23" s="113" t="n">
+        <v>58.9099</v>
+      </c>
+      <c r="G23" s="114" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>50.4958981480704</v>
-      </c>
-      <c r="I23" s="108"/>
+        <v>42.4358981480704</v>
+      </c>
+      <c r="I23" s="109"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="114" t="s">
+      <c r="A24" s="115" t="s">
         <v>270</v>
       </c>
-      <c r="B24" s="115" t="n">
+      <c r="B24" s="116" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="115"/>
-      <c r="D24" s="116" t="s">
+      <c r="C24" s="116"/>
+      <c r="D24" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E24" s="123" t="n">
+      <c r="E24" s="124" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>36.4748517843995</v>
-      </c>
-      <c r="F24" s="130" t="n">
+        <v>28.4148517843995</v>
+      </c>
+      <c r="F24" s="131" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>12.81</v>
-      </c>
-      <c r="G24" s="131" t="n">
+        <v>50.2501</v>
+      </c>
+      <c r="G24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>42.410766090482</v>
-      </c>
-      <c r="H24" s="115"/>
-      <c r="I24" s="132"/>
+        <v>34.350766090482</v>
+      </c>
+      <c r="H24" s="116"/>
+      <c r="I24" s="133"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="133" t="s">
+      <c r="A28" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="133"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="102"/>
-      <c r="E28" s="102"/>
-      <c r="F28" s="120" t="s">
+      <c r="B28" s="134"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="103"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="121" t="s">
         <v>273</v>
       </c>
-      <c r="G28" s="102" t="n">
+      <c r="G28" s="103" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="102"/>
-      <c r="I28" s="121"/>
+      <c r="H28" s="103"/>
+      <c r="I28" s="122"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="106"/>
-      <c r="D29" s="107" t="s">
+      <c r="A29" s="107"/>
+      <c r="D29" s="108" t="s">
         <v>265</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="62" t="n">
+      <c r="G29" s="63" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="125" t="s">
+      <c r="H29" s="126" t="s">
         <v>277</v>
       </c>
-      <c r="I29" s="108" t="n">
+      <c r="I29" s="109" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="109" t="s">
+      <c r="A30" s="110" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="107" t="s">
+      <c r="D30" s="108" t="s">
         <v>279</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="126" t="n">
+      <c r="G30" s="127" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="108"/>
+      <c r="I30" s="109"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="106"/>
-      <c r="D31" s="107" t="s">
+      <c r="A31" s="107"/>
+      <c r="D31" s="108" t="s">
         <v>280</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="62" t="n">
+      <c r="G31" s="63" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="108"/>
+      <c r="I31" s="109"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="106"/>
-      <c r="D32" s="107"/>
-      <c r="G32" s="127" t="s">
+      <c r="A32" s="107"/>
+      <c r="D32" s="108"/>
+      <c r="G32" s="128" t="s">
         <v>281</v>
       </c>
-      <c r="I32" s="108"/>
+      <c r="I32" s="109"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="106"/>
-      <c r="F33" s="128" t="s">
+      <c r="A33" s="107"/>
+      <c r="F33" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="I33" s="108"/>
+      <c r="I33" s="109"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="110" t="s">
         <v>266</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="107" t="s">
+      <c r="D34" s="108" t="s">
         <v>267</v>
       </c>
-      <c r="E34" s="113" t="n">
+      <c r="E34" s="114" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-59.8316236638297</v>
-      </c>
-      <c r="F34" s="129" t="n">
+        <v>-66.7884236638297</v>
+      </c>
+      <c r="F34" s="130" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="113" t="n">
+      <c r="G34" s="114" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-54.8800007866982</v>
-      </c>
-      <c r="I34" s="108"/>
+        <v>-61.8368007866982</v>
+      </c>
+      <c r="I34" s="109"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="110" t="s">
         <v>268</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="107" t="s">
+      <c r="D35" s="108" t="s">
         <v>269</v>
       </c>
-      <c r="E35" s="113" t="n">
+      <c r="E35" s="114" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>16.2818777773465</v>
-      </c>
-      <c r="F35" s="129" t="n">
+        <v>8.22187777734649</v>
+      </c>
+      <c r="F35" s="130" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="113" t="n">
+      <c r="G35" s="114" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>21.5827875381681</v>
-      </c>
-      <c r="I35" s="108"/>
+        <v>13.5227875381681</v>
+      </c>
+      <c r="I35" s="109"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="114" t="s">
+      <c r="A36" s="115" t="s">
         <v>270</v>
       </c>
-      <c r="B36" s="115" t="n">
+      <c r="B36" s="116" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="115"/>
-      <c r="D36" s="116" t="s">
+      <c r="C36" s="116"/>
+      <c r="D36" s="117" t="s">
         <v>271</v>
       </c>
-      <c r="E36" s="123" t="n">
+      <c r="E36" s="124" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>4.09617567428903</v>
-      </c>
-      <c r="F36" s="130" t="n">
+        <v>-3.96382432571097</v>
+      </c>
+      <c r="F36" s="131" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="123" t="n">
+      <c r="G36" s="124" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>10.0324025227675</v>
-      </c>
-      <c r="H36" s="115"/>
-      <c r="I36" s="132"/>
+        <v>1.9724025227675</v>
+      </c>
+      <c r="H36" s="116"/>
+      <c r="I36" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17791,7 +17828,7 @@
       <c r="A9" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="B9" s="134" t="n">
+      <c r="B9" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17815,7 +17852,7 @@
       <c r="A12" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="B12" s="134" t="n">
+      <c r="B12" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17911,7 +17948,7 @@
       <c r="A24" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="B24" s="134" t="n">
+      <c r="B24" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17935,7 +17972,7 @@
       <c r="A27" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="B27" s="134" t="n">
+      <c r="B27" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18031,7 +18068,7 @@
       <c r="A39" s="0" t="s">
         <v>320</v>
       </c>
-      <c r="B39" s="134" t="n">
+      <c r="B39" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18055,7 +18092,7 @@
       <c r="A42" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="B42" s="134" t="n">
+      <c r="B42" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18151,7 +18188,7 @@
       <c r="A54" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="B54" s="134" t="n">
+      <c r="B54" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18175,7 +18212,7 @@
       <c r="A57" s="0" t="s">
         <v>338</v>
       </c>
-      <c r="B57" s="134" t="n">
+      <c r="B57" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18239,7 +18276,7 @@
       <c r="A65" s="0" t="s">
         <v>346</v>
       </c>
-      <c r="B65" s="134" t="n">
+      <c r="B65" s="135" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18247,7 +18284,7 @@
       <c r="A66" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="B66" s="134" t="n">
+      <c r="B66" s="135" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18255,7 +18292,7 @@
       <c r="A67" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B67" s="134" t="n">
+      <c r="B67" s="135" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18263,7 +18300,7 @@
       <c r="A68" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B68" s="134" t="n">
+      <c r="B68" s="135" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18583,7 +18620,7 @@
       <c r="A108" s="0" t="s">
         <v>389</v>
       </c>
-      <c r="B108" s="134" t="n">
+      <c r="B108" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18607,7 +18644,7 @@
       <c r="A111" s="0" t="s">
         <v>392</v>
       </c>
-      <c r="B111" s="134" t="n">
+      <c r="B111" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18703,7 +18740,7 @@
       <c r="A123" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="B123" s="134" t="n">
+      <c r="B123" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18727,7 +18764,7 @@
       <c r="A126" s="0" t="s">
         <v>407</v>
       </c>
-      <c r="B126" s="134" t="n">
+      <c r="B126" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18823,7 +18860,7 @@
       <c r="A138" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="B138" s="134" t="n">
+      <c r="B138" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18847,7 +18884,7 @@
       <c r="A141" s="0" t="s">
         <v>422</v>
       </c>
-      <c r="B141" s="134" t="n">
+      <c r="B141" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18943,7 +18980,7 @@
       <c r="A153" s="0" t="s">
         <v>434</v>
       </c>
-      <c r="B153" s="134" t="n">
+      <c r="B153" s="135" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18967,7 +19004,7 @@
       <c r="A156" s="0" t="s">
         <v>437</v>
       </c>
-      <c r="B156" s="134" t="n">
+      <c r="B156" s="135" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19031,7 +19068,7 @@
       <c r="A164" s="0" t="s">
         <v>445</v>
       </c>
-      <c r="B164" s="134" t="n">
+      <c r="B164" s="135" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19039,7 +19076,7 @@
       <c r="A165" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="B165" s="134" t="n">
+      <c r="B165" s="135" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19047,7 +19084,7 @@
       <c r="A166" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B166" s="134" t="n">
+      <c r="B166" s="135" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19055,7 +19092,7 @@
       <c r="A167" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B167" s="134" t="n">
+      <c r="B167" s="135" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19191,7 +19228,7 @@
       <c r="A184" s="0" t="s">
         <v>465</v>
       </c>
-      <c r="B184" s="134" t="n">
+      <c r="B184" s="135" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19199,7 +19236,7 @@
       <c r="A185" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="B185" s="134" t="n">
+      <c r="B185" s="135" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19231,7 +19268,7 @@
       <c r="A189" s="0" t="s">
         <v>470</v>
       </c>
-      <c r="B189" s="134" t="n">
+      <c r="B189" s="135" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19255,7 +19292,7 @@
       <c r="A192" s="0" t="s">
         <v>473</v>
       </c>
-      <c r="B192" s="134" t="n">
+      <c r="B192" s="135" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19263,7 +19300,7 @@
       <c r="A193" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="B193" s="134" t="n">
+      <c r="B193" s="135" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19271,7 +19308,7 @@
       <c r="A194" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B194" s="134" t="n">
+      <c r="B194" s="135" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19279,7 +19316,7 @@
       <c r="A195" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B195" s="134" t="n">
+      <c r="B195" s="135" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20703,40 +20740,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="134" t="n">
+      <c r="C337" s="135" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="134" t="n">
+      <c r="D337" s="135" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="134" t="n">
+      <c r="E337" s="135" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="134" t="n">
+      <c r="F337" s="135" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="134" t="n">
+      <c r="G337" s="135" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="134" t="n">
+      <c r="H337" s="135" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="134" t="n">
+      <c r="I337" s="135" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="134" t="n">
+      <c r="J337" s="135" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="134" t="n">
+      <c r="K337" s="135" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="134" t="n">
+      <c r="L337" s="135" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="134" t="n">
+      <c r="M337" s="135" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="134" t="n">
+      <c r="N337" s="135" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20747,40 +20784,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="134" t="n">
+      <c r="C338" s="135" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="134" t="n">
+      <c r="D338" s="135" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="134" t="n">
+      <c r="E338" s="135" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="134" t="n">
+      <c r="F338" s="135" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="134" t="n">
+      <c r="G338" s="135" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="134" t="n">
+      <c r="H338" s="135" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="134" t="n">
+      <c r="I338" s="135" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="134" t="n">
+      <c r="J338" s="135" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="134" t="n">
+      <c r="K338" s="135" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="134" t="n">
+      <c r="L338" s="135" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="134" t="n">
+      <c r="M338" s="135" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="134" t="n">
+      <c r="N338" s="135" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20791,40 +20828,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="134" t="n">
+      <c r="C339" s="135" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="134" t="n">
+      <c r="D339" s="135" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="134" t="n">
+      <c r="E339" s="135" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="134" t="n">
+      <c r="F339" s="135" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="134" t="n">
+      <c r="G339" s="135" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="134" t="n">
+      <c r="H339" s="135" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="134" t="n">
+      <c r="I339" s="135" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="134" t="n">
+      <c r="J339" s="135" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="134" t="n">
+      <c r="K339" s="135" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="134" t="n">
+      <c r="L339" s="135" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="134" t="n">
+      <c r="M339" s="135" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="134" t="n">
+      <c r="N339" s="135" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -20835,40 +20872,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="134" t="n">
+      <c r="C340" s="135" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="134" t="n">
+      <c r="D340" s="135" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="134" t="n">
+      <c r="E340" s="135" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="134" t="n">
+      <c r="F340" s="135" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="134" t="n">
+      <c r="G340" s="135" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="134" t="n">
+      <c r="H340" s="135" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="134" t="n">
+      <c r="I340" s="135" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="134" t="n">
+      <c r="J340" s="135" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="134" t="n">
+      <c r="K340" s="135" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="134" t="n">
+      <c r="L340" s="135" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="134" t="n">
+      <c r="M340" s="135" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="134" t="n">
+      <c r="N340" s="135" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21583,40 +21620,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="134" t="n">
+      <c r="C357" s="135" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="134" t="n">
+      <c r="D357" s="135" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="134" t="n">
+      <c r="E357" s="135" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="134" t="n">
+      <c r="F357" s="135" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="134" t="n">
+      <c r="G357" s="135" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="134" t="n">
+      <c r="H357" s="135" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="134" t="n">
+      <c r="I357" s="135" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="134" t="n">
+      <c r="J357" s="135" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="134" t="n">
+      <c r="K357" s="135" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="134" t="n">
+      <c r="L357" s="135" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="134" t="n">
+      <c r="M357" s="135" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="134" t="n">
+      <c r="N357" s="135" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21627,40 +21664,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="134" t="n">
+      <c r="C358" s="135" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="134" t="n">
+      <c r="D358" s="135" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="134" t="n">
+      <c r="E358" s="135" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="134" t="n">
+      <c r="F358" s="135" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="134" t="n">
+      <c r="G358" s="135" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="134" t="n">
+      <c r="H358" s="135" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="134" t="n">
+      <c r="I358" s="135" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="134" t="n">
+      <c r="J358" s="135" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="134" t="n">
+      <c r="K358" s="135" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="134" t="n">
+      <c r="L358" s="135" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="134" t="n">
+      <c r="M358" s="135" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="134" t="n">
+      <c r="N358" s="135" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21671,40 +21708,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="134" t="n">
+      <c r="C359" s="135" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="134" t="n">
+      <c r="D359" s="135" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="134" t="n">
+      <c r="E359" s="135" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="134" t="n">
+      <c r="F359" s="135" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="134" t="n">
+      <c r="G359" s="135" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="134" t="n">
+      <c r="H359" s="135" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="134" t="n">
+      <c r="I359" s="135" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="134" t="n">
+      <c r="J359" s="135" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="134" t="n">
+      <c r="K359" s="135" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="134" t="n">
+      <c r="L359" s="135" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="134" t="n">
+      <c r="M359" s="135" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="134" t="n">
+      <c r="N359" s="135" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21715,40 +21752,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="134" t="n">
+      <c r="C360" s="135" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="134" t="n">
+      <c r="D360" s="135" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="134" t="n">
+      <c r="E360" s="135" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="134" t="n">
+      <c r="F360" s="135" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="134" t="n">
+      <c r="G360" s="135" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="134" t="n">
+      <c r="H360" s="135" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="134" t="n">
+      <c r="I360" s="135" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="134" t="n">
+      <c r="J360" s="135" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="134" t="n">
+      <c r="K360" s="135" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="134" t="n">
+      <c r="L360" s="135" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="134" t="n">
+      <c r="M360" s="135" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="134" t="n">
+      <c r="N360" s="135" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -21891,7 +21928,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="134" t="n">
+      <c r="C364" s="135" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -21935,7 +21972,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="134" t="n">
+      <c r="C365" s="135" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -21979,7 +22016,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="134" t="n">
+      <c r="C366" s="135" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22023,7 +22060,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="134" t="n">
+      <c r="C367" s="135" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23800,13 +23837,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="136" t="s">
         <v>812</v>
       </c>
-      <c r="C1" s="135" t="n">
+      <c r="C1" s="136" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="135" t="s">
+      <c r="D1" s="136" t="s">
         <v>813</v>
       </c>
     </row>
@@ -23814,10 +23851,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="135" t="s">
+      <c r="B2" s="136" t="s">
         <v>814</v>
       </c>
-      <c r="C2" s="135" t="n">
+      <c r="C2" s="136" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -23825,10 +23862,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="136" t="s">
         <v>815</v>
       </c>
-      <c r="C3" s="135" t="n">
+      <c r="C3" s="136" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -23932,7 +23969,7 @@
       <c r="B16" s="0" t="s">
         <v>830</v>
       </c>
-      <c r="C16" s="134" t="n">
+      <c r="C16" s="135" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -23940,7 +23977,7 @@
       <c r="B17" s="0" t="s">
         <v>831</v>
       </c>
-      <c r="C17" s="134" t="n">
+      <c r="C17" s="135" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -23948,7 +23985,7 @@
       <c r="B18" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C18" s="134" t="n">
+      <c r="C18" s="135" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -23956,7 +23993,7 @@
       <c r="B19" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C19" s="134" t="n">
+      <c r="C19" s="135" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24444,7 +24481,7 @@
       <c r="B80" s="0" t="s">
         <v>901</v>
       </c>
-      <c r="C80" s="134" t="n">
+      <c r="C80" s="135" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24492,7 +24529,7 @@
       <c r="B86" s="0" t="s">
         <v>907</v>
       </c>
-      <c r="C86" s="134" t="n">
+      <c r="C86" s="135" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24524,7 +24561,7 @@
       <c r="B90" s="0" t="s">
         <v>911</v>
       </c>
-      <c r="C90" s="134" t="n">
+      <c r="C90" s="135" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24612,7 +24649,7 @@
       <c r="B101" s="0" t="s">
         <v>923</v>
       </c>
-      <c r="C101" s="134" t="n">
+      <c r="C101" s="135" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24788,7 +24825,7 @@
       <c r="B123" s="0" t="s">
         <v>947</v>
       </c>
-      <c r="C123" s="134" t="n">
+      <c r="C123" s="135" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -24852,7 +24889,7 @@
       <c r="B131" s="0" t="s">
         <v>955</v>
       </c>
-      <c r="C131" s="134" t="n">
+      <c r="C131" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -24868,7 +24905,7 @@
       <c r="B133" s="0" t="s">
         <v>957</v>
       </c>
-      <c r="C133" s="134" t="n">
+      <c r="C133" s="135" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25388,7 +25425,7 @@
       <c r="B198" s="0" t="s">
         <v>1024</v>
       </c>
-      <c r="C198" s="134" t="n">
+      <c r="C198" s="135" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25436,7 +25473,7 @@
       <c r="B204" s="0" t="s">
         <v>1030</v>
       </c>
-      <c r="C204" s="134" t="n">
+      <c r="C204" s="135" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25468,7 +25505,7 @@
       <c r="B208" s="0" t="s">
         <v>1034</v>
       </c>
-      <c r="C208" s="134" t="n">
+      <c r="C208" s="135" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25556,7 +25593,7 @@
       <c r="B219" s="0" t="s">
         <v>1045</v>
       </c>
-      <c r="C219" s="134" t="n">
+      <c r="C219" s="135" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25732,7 +25769,7 @@
       <c r="B241" s="0" t="s">
         <v>1068</v>
       </c>
-      <c r="C241" s="134" t="n">
+      <c r="C241" s="135" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25796,7 +25833,7 @@
       <c r="B249" s="0" t="s">
         <v>1076</v>
       </c>
-      <c r="C249" s="134" t="n">
+      <c r="C249" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25812,7 +25849,7 @@
       <c r="B251" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="C251" s="134" t="n">
+      <c r="C251" s="135" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26332,7 +26369,7 @@
       <c r="B316" s="0" t="s">
         <v>1143</v>
       </c>
-      <c r="C316" s="134" t="n">
+      <c r="C316" s="135" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26380,7 +26417,7 @@
       <c r="B322" s="0" t="s">
         <v>1149</v>
       </c>
-      <c r="C322" s="134" t="n">
+      <c r="C322" s="135" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26412,7 +26449,7 @@
       <c r="B326" s="0" t="s">
         <v>1153</v>
       </c>
-      <c r="C326" s="134" t="n">
+      <c r="C326" s="135" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26500,7 +26537,7 @@
       <c r="B337" s="0" t="s">
         <v>1164</v>
       </c>
-      <c r="C337" s="134" t="n">
+      <c r="C337" s="135" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26676,7 +26713,7 @@
       <c r="B359" s="0" t="s">
         <v>1187</v>
       </c>
-      <c r="C359" s="134" t="n">
+      <c r="C359" s="135" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26740,7 +26777,7 @@
       <c r="B367" s="0" t="s">
         <v>1195</v>
       </c>
-      <c r="C367" s="134" t="n">
+      <c r="C367" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26756,7 +26793,7 @@
       <c r="B369" s="0" t="s">
         <v>1197</v>
       </c>
-      <c r="C369" s="134" t="n">
+      <c r="C369" s="135" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27276,7 +27313,7 @@
       <c r="B434" s="0" t="s">
         <v>1262</v>
       </c>
-      <c r="C434" s="134" t="n">
+      <c r="C434" s="135" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27324,7 +27361,7 @@
       <c r="B440" s="0" t="s">
         <v>1268</v>
       </c>
-      <c r="C440" s="134" t="n">
+      <c r="C440" s="135" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27356,7 +27393,7 @@
       <c r="B444" s="0" t="s">
         <v>1272</v>
       </c>
-      <c r="C444" s="134" t="n">
+      <c r="C444" s="135" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27444,7 +27481,7 @@
       <c r="B455" s="0" t="s">
         <v>1283</v>
       </c>
-      <c r="C455" s="134" t="n">
+      <c r="C455" s="135" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27620,7 +27657,7 @@
       <c r="B477" s="0" t="s">
         <v>1306</v>
       </c>
-      <c r="C477" s="134" t="n">
+      <c r="C477" s="135" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27684,7 +27721,7 @@
       <c r="B485" s="0" t="s">
         <v>1314</v>
       </c>
-      <c r="C485" s="134" t="n">
+      <c r="C485" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27700,7 +27737,7 @@
       <c r="B487" s="0" t="s">
         <v>1316</v>
       </c>
-      <c r="C487" s="134" t="n">
+      <c r="C487" s="135" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27788,7 +27825,7 @@
       <c r="B498" s="0" t="s">
         <v>1327</v>
       </c>
-      <c r="C498" s="134" t="n">
+      <c r="C498" s="135" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27796,7 +27833,7 @@
       <c r="B499" s="0" t="s">
         <v>1328</v>
       </c>
-      <c r="C499" s="134" t="n">
+      <c r="C499" s="135" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27804,7 +27841,7 @@
       <c r="B500" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C500" s="134" t="n">
+      <c r="C500" s="135" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27812,7 +27849,7 @@
       <c r="B501" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C501" s="134" t="n">
+      <c r="C501" s="135" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28380,7 +28417,7 @@
       <c r="B572" s="0" t="s">
         <v>1401</v>
       </c>
-      <c r="C572" s="134" t="n">
+      <c r="C572" s="135" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28428,7 +28465,7 @@
       <c r="B578" s="0" t="s">
         <v>1407</v>
       </c>
-      <c r="C578" s="134" t="n">
+      <c r="C578" s="135" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28460,7 +28497,7 @@
       <c r="B582" s="0" t="s">
         <v>1411</v>
       </c>
-      <c r="C582" s="134" t="n">
+      <c r="C582" s="135" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28548,7 +28585,7 @@
       <c r="B593" s="0" t="s">
         <v>1422</v>
       </c>
-      <c r="C593" s="134" t="n">
+      <c r="C593" s="135" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28724,7 +28761,7 @@
       <c r="B615" s="0" t="s">
         <v>1445</v>
       </c>
-      <c r="C615" s="134" t="n">
+      <c r="C615" s="135" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28788,7 +28825,7 @@
       <c r="B623" s="0" t="s">
         <v>1453</v>
       </c>
-      <c r="C623" s="134" t="n">
+      <c r="C623" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28804,7 +28841,7 @@
       <c r="B625" s="0" t="s">
         <v>1455</v>
       </c>
-      <c r="C625" s="134" t="n">
+      <c r="C625" s="135" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29324,7 +29361,7 @@
       <c r="B690" s="0" t="s">
         <v>1520</v>
       </c>
-      <c r="C690" s="134" t="n">
+      <c r="C690" s="135" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29372,7 +29409,7 @@
       <c r="B696" s="0" t="s">
         <v>1526</v>
       </c>
-      <c r="C696" s="134" t="n">
+      <c r="C696" s="135" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29404,7 +29441,7 @@
       <c r="B700" s="0" t="s">
         <v>1530</v>
       </c>
-      <c r="C700" s="134" t="n">
+      <c r="C700" s="135" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29492,7 +29529,7 @@
       <c r="B711" s="0" t="s">
         <v>1541</v>
       </c>
-      <c r="C711" s="134" t="n">
+      <c r="C711" s="135" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29668,7 +29705,7 @@
       <c r="B733" s="0" t="s">
         <v>1564</v>
       </c>
-      <c r="C733" s="134" t="n">
+      <c r="C733" s="135" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29732,7 +29769,7 @@
       <c r="B741" s="0" t="s">
         <v>1572</v>
       </c>
-      <c r="C741" s="134" t="n">
+      <c r="C741" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29748,7 +29785,7 @@
       <c r="B743" s="0" t="s">
         <v>1574</v>
       </c>
-      <c r="C743" s="134" t="n">
+      <c r="C743" s="135" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30304,7 +30341,7 @@
       <c r="B811" s="0" t="s">
         <v>1650</v>
       </c>
-      <c r="C811" s="134" t="n">
+      <c r="C811" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30820,7 +30857,7 @@
       <c r="B874" s="0" t="s">
         <v>1715</v>
       </c>
-      <c r="C874" s="134" t="n">
+      <c r="C874" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31336,7 +31373,7 @@
       <c r="B937" s="0" t="s">
         <v>1780</v>
       </c>
-      <c r="C937" s="134" t="n">
+      <c r="C937" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31852,7 +31889,7 @@
       <c r="B1000" s="0" t="s">
         <v>1845</v>
       </c>
-      <c r="C1000" s="134" t="n">
+      <c r="C1000" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32368,7 +32405,7 @@
       <c r="B1063" s="0" t="s">
         <v>1910</v>
       </c>
-      <c r="C1063" s="134" t="n">
+      <c r="C1063" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32884,7 +32921,7 @@
       <c r="B1126" s="0" t="s">
         <v>1975</v>
       </c>
-      <c r="C1126" s="134" t="n">
+      <c r="C1126" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33400,7 +33437,7 @@
       <c r="B1189" s="0" t="s">
         <v>2040</v>
       </c>
-      <c r="C1189" s="134" t="n">
+      <c r="C1189" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33916,7 +33953,7 @@
       <c r="B1252" s="0" t="s">
         <v>2105</v>
       </c>
-      <c r="C1252" s="134" t="n">
+      <c r="C1252" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34432,7 +34469,7 @@
       <c r="B1315" s="0" t="s">
         <v>2170</v>
       </c>
-      <c r="C1315" s="134" t="n">
+      <c r="C1315" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34948,7 +34985,7 @@
       <c r="B1378" s="0" t="s">
         <v>2235</v>
       </c>
-      <c r="C1378" s="134" t="n">
+      <c r="C1378" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35464,7 +35501,7 @@
       <c r="B1441" s="0" t="s">
         <v>2300</v>
       </c>
-      <c r="C1441" s="134" t="n">
+      <c r="C1441" s="135" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35912,7 +35949,7 @@
       <c r="B1497" s="0" t="s">
         <v>2359</v>
       </c>
-      <c r="C1497" s="134" t="n">
+      <c r="C1497" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36538,7 +36575,7 @@
       <c r="B1576" s="0" t="s">
         <v>2443</v>
       </c>
-      <c r="C1576" s="134" t="n">
+      <c r="C1576" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36707,7 +36744,7 @@
       <c r="B1596" s="0" t="s">
         <v>2465</v>
       </c>
-      <c r="C1596" s="134" t="n">
+      <c r="C1596" s="135" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36715,7 +36752,7 @@
       <c r="B1597" s="0" t="s">
         <v>2466</v>
       </c>
-      <c r="C1597" s="134" t="n">
+      <c r="C1597" s="135" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37595,7 +37632,7 @@
       <c r="B1707" s="0" t="s">
         <v>2577</v>
       </c>
-      <c r="C1707" s="134" t="n">
+      <c r="C1707" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37611,7 +37648,7 @@
       <c r="B1709" s="0" t="s">
         <v>2579</v>
       </c>
-      <c r="C1709" s="134" t="n">
+      <c r="C1709" s="135" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38131,7 +38168,7 @@
       <c r="B1774" s="0" t="s">
         <v>2644</v>
       </c>
-      <c r="C1774" s="134" t="n">
+      <c r="C1774" s="135" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38211,7 +38248,7 @@
       <c r="B1784" s="0" t="s">
         <v>2654</v>
       </c>
-      <c r="C1784" s="134" t="n">
+      <c r="C1784" s="135" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38299,7 +38336,7 @@
       <c r="B1795" s="0" t="s">
         <v>2665</v>
       </c>
-      <c r="C1795" s="134" t="n">
+      <c r="C1795" s="135" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38475,7 +38512,7 @@
       <c r="B1817" s="0" t="s">
         <v>2688</v>
       </c>
-      <c r="C1817" s="134" t="n">
+      <c r="C1817" s="135" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38539,7 +38576,7 @@
       <c r="B1825" s="0" t="s">
         <v>2696</v>
       </c>
-      <c r="C1825" s="134" t="n">
+      <c r="C1825" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38555,7 +38592,7 @@
       <c r="B1827" s="0" t="s">
         <v>2698</v>
       </c>
-      <c r="C1827" s="134" t="n">
+      <c r="C1827" s="135" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39158,7 +39195,7 @@
       <c r="B1902" s="0" t="s">
         <v>2775</v>
       </c>
-      <c r="C1902" s="134" t="n">
+      <c r="C1902" s="135" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39206,7 +39243,7 @@
       <c r="B1908" s="0" t="s">
         <v>2781</v>
       </c>
-      <c r="C1908" s="134" t="n">
+      <c r="C1908" s="135" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39238,7 +39275,7 @@
       <c r="B1912" s="0" t="s">
         <v>2785</v>
       </c>
-      <c r="C1912" s="134" t="n">
+      <c r="C1912" s="135" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39326,7 +39363,7 @@
       <c r="B1923" s="0" t="s">
         <v>2796</v>
       </c>
-      <c r="C1923" s="134" t="n">
+      <c r="C1923" s="135" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39502,7 +39539,7 @@
       <c r="B1945" s="0" t="s">
         <v>2819</v>
       </c>
-      <c r="C1945" s="134" t="n">
+      <c r="C1945" s="135" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39566,7 +39603,7 @@
       <c r="B1953" s="0" t="s">
         <v>2827</v>
       </c>
-      <c r="C1953" s="134" t="n">
+      <c r="C1953" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39582,7 +39619,7 @@
       <c r="B1955" s="0" t="s">
         <v>2829</v>
       </c>
-      <c r="C1955" s="134" t="n">
+      <c r="C1955" s="135" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40102,7 +40139,7 @@
       <c r="B2020" s="0" t="s">
         <v>2894</v>
       </c>
-      <c r="C2020" s="134" t="n">
+      <c r="C2020" s="135" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40150,7 +40187,7 @@
       <c r="B2026" s="0" t="s">
         <v>2900</v>
       </c>
-      <c r="C2026" s="134" t="n">
+      <c r="C2026" s="135" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40182,7 +40219,7 @@
       <c r="B2030" s="0" t="s">
         <v>2904</v>
       </c>
-      <c r="C2030" s="134" t="n">
+      <c r="C2030" s="135" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40270,7 +40307,7 @@
       <c r="B2041" s="0" t="s">
         <v>2915</v>
       </c>
-      <c r="C2041" s="134" t="n">
+      <c r="C2041" s="135" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40446,7 +40483,7 @@
       <c r="B2063" s="0" t="s">
         <v>2938</v>
       </c>
-      <c r="C2063" s="134" t="n">
+      <c r="C2063" s="135" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40510,7 +40547,7 @@
       <c r="B2071" s="0" t="s">
         <v>2946</v>
       </c>
-      <c r="C2071" s="134" t="n">
+      <c r="C2071" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40526,7 +40563,7 @@
       <c r="B2073" s="0" t="s">
         <v>2948</v>
       </c>
-      <c r="C2073" s="134" t="n">
+      <c r="C2073" s="135" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41046,7 +41083,7 @@
       <c r="B2138" s="0" t="s">
         <v>3013</v>
       </c>
-      <c r="C2138" s="134" t="n">
+      <c r="C2138" s="135" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41094,7 +41131,7 @@
       <c r="B2144" s="0" t="s">
         <v>3019</v>
       </c>
-      <c r="C2144" s="134" t="n">
+      <c r="C2144" s="135" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41126,7 +41163,7 @@
       <c r="B2148" s="0" t="s">
         <v>3023</v>
       </c>
-      <c r="C2148" s="134" t="n">
+      <c r="C2148" s="135" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41214,7 +41251,7 @@
       <c r="B2159" s="0" t="s">
         <v>3034</v>
       </c>
-      <c r="C2159" s="134" t="n">
+      <c r="C2159" s="135" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41390,7 +41427,7 @@
       <c r="B2181" s="0" t="s">
         <v>3057</v>
       </c>
-      <c r="C2181" s="134" t="n">
+      <c r="C2181" s="135" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41454,7 +41491,7 @@
       <c r="B2189" s="0" t="s">
         <v>3065</v>
       </c>
-      <c r="C2189" s="134" t="n">
+      <c r="C2189" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41470,7 +41507,7 @@
       <c r="B2191" s="0" t="s">
         <v>3067</v>
       </c>
-      <c r="C2191" s="134" t="n">
+      <c r="C2191" s="135" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42046,7 +42083,7 @@
       <c r="B2263" s="0" t="s">
         <v>3142</v>
       </c>
-      <c r="C2263" s="134" t="n">
+      <c r="C2263" s="135" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42333,7 +42370,7 @@
       <c r="F2297" s="0" t="s">
         <v>3187</v>
       </c>
-      <c r="G2297" s="136" t="n">
+      <c r="G2297" s="137" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42425,7 +42462,7 @@
       <c r="B2307" s="0" t="s">
         <v>3201</v>
       </c>
-      <c r="C2307" s="134" t="n">
+      <c r="C2307" s="135" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42511,7 +42548,7 @@
       <c r="B2317" s="0" t="s">
         <v>3217</v>
       </c>
-      <c r="C2317" s="134" t="n">
+      <c r="C2317" s="135" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42519,7 +42556,7 @@
       <c r="B2318" s="0" t="s">
         <v>3218</v>
       </c>
-      <c r="C2318" s="134" t="n">
+      <c r="C2318" s="135" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42535,7 +42572,7 @@
       <c r="B2320" s="0" t="s">
         <v>3220</v>
       </c>
-      <c r="C2320" s="134" t="n">
+      <c r="C2320" s="135" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42583,7 +42620,7 @@
       <c r="C2326" s="0" t="s">
         <v>3228</v>
       </c>
-      <c r="D2326" s="137" t="n">
+      <c r="D2326" s="138" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42634,7 +42671,7 @@
       <c r="C2332" s="0" t="s">
         <v>3236</v>
       </c>
-      <c r="D2332" s="137" t="n">
+      <c r="D2332" s="138" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42653,7 +42690,7 @@
       <c r="D2334" s="0" t="s">
         <v>3239</v>
       </c>
-      <c r="E2334" s="137" t="n">
+      <c r="E2334" s="138" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42711,7 +42748,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="137" t="n">
+      <c r="F2339" s="138" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43183,7 +43220,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="137" t="n">
+      <c r="F2380" s="138" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update Modes, add 2018-3 log
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11655,11 +11655,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="G33" activeCellId="0" sqref="G33"/>
+      <selection pane="bottomRight" activeCell="P54" activeCellId="0" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14414,46 +14414,46 @@
         <v>170</v>
       </c>
       <c r="E51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="F51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
       <c r="G51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="H51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
       <c r="I51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="J51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
       <c r="K51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="L51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
       <c r="M51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="N51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
       <c r="O51" s="33" t="n">
-        <v>0.675</v>
+        <v>0.5</v>
       </c>
       <c r="P51" s="32" t="n">
-        <v>38245</v>
-      </c>
-      <c r="T51" s="31" t="n">
-        <v>0.675</v>
+        <v>36496</v>
+      </c>
+      <c r="T51" s="33" t="n">
+        <v>0.5</v>
       </c>
       <c r="U51" s="32" t="n">
-        <v>38245</v>
+        <v>36496</v>
       </c>
     </row>
     <row r="52" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14468,49 +14468,49 @@
         <v>173</v>
       </c>
       <c r="E52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="F52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="G52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="H52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="I52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="J52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="K52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="L52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="M52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="N52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="O52" s="37" t="n">
-        <v>-0.675</v>
+        <v>-0.5</v>
       </c>
       <c r="P52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="Q52" s="26"/>
       <c r="R52" s="26"/>
       <c r="S52" s="26"/>
-      <c r="T52" s="38" t="n">
-        <v>-0.675</v>
+      <c r="T52" s="37" t="n">
+        <v>-0.5</v>
       </c>
       <c r="U52" s="45" t="n">
-        <v>27858</v>
+        <v>29606</v>
       </c>
       <c r="V52" s="0"/>
       <c r="W52" s="0"/>
@@ -14622,10 +14622,10 @@
         <v>180</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>28.1862</v>
+        <v>29.573</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>246016</v>
+        <v>259915</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
@@ -14638,10 +14638,10 @@
         <v>-241810</v>
       </c>
       <c r="K54" s="57" t="n">
-        <v>44.962</v>
+        <v>45.575</v>
       </c>
       <c r="L54" s="28" t="n">
-        <v>413776</v>
+        <v>419898</v>
       </c>
       <c r="M54" s="57" t="n">
         <v>44.962</v>
@@ -14650,10 +14650,10 @@
         <v>413776</v>
       </c>
       <c r="O54" s="57" t="n">
-        <v>19.162</v>
+        <v>19.847</v>
       </c>
       <c r="P54" s="28" t="n">
-        <v>155779</v>
+        <v>162643</v>
       </c>
       <c r="T54" s="58" t="n">
         <v>51.2907</v>
@@ -17239,11 +17239,11 @@
       </c>
       <c r="G3" s="113" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>19.162</v>
+        <v>19.847</v>
       </c>
       <c r="H3" s="114" t="n">
         <f aca="false">G3-F3</f>
-        <v>0.0588810182917001</v>
+        <v>0.743881018291702</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17306,7 +17306,7 @@
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="114" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>2.56202162665121</v>
+        <v>2.79035495998454</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>272</v>
@@ -17352,12 +17352,12 @@
       </c>
       <c r="E10" s="114" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>28.1862</v>
+        <v>29.573</v>
       </c>
       <c r="F10" s="114"/>
       <c r="G10" s="123" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>30.3676000290853</v>
+        <v>31.7544000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17501,7 +17501,7 @@
       </c>
       <c r="E22" s="114" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-39.7801914229833</v>
+        <v>-38.3933914229833</v>
       </c>
       <c r="F22" s="130" t="n">
         <f aca="false">'Modes A-F'!I54</f>
@@ -17509,7 +17509,7 @@
       </c>
       <c r="G22" s="114" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-34.82882924884</v>
+        <v>-33.44202924884</v>
       </c>
       <c r="I22" s="109"/>
     </row>
@@ -17663,7 +17663,7 @@
       </c>
       <c r="E34" s="114" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-66.7884236638297</v>
+        <v>-65.4016236638297</v>
       </c>
       <c r="F34" s="130" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17671,7 +17671,7 @@
       </c>
       <c r="G34" s="114" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-61.8368007866982</v>
+        <v>-60.4500007866982</v>
       </c>
       <c r="I34" s="109"/>
     </row>

</xml_diff>

<commit_message>
links between sheets on the Modes spreadsheet
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -103,8 +103,7 @@
             <charset val="1"/>
           </rPr>
           <t>Vertical = 110.75
-Pitch = -1.465
-</t>
+Pitch = -1.465</t>
         </r>
         <r>
           <rPr>
@@ -502,7 +501,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4194" uniqueCount="3307">
   <si>
-    <t>  in /home/bravel/commissioning/CRS, do sh pvs.sh | xclip, then paste into appropriate column</t>
+    <t>in /home/bravel/commissioning/CRS, do sh pvs.sh | xclip, then paste into appropriate column</t>
   </si>
   <si>
     <t>Mode A</t>
@@ -11399,6 +11398,10 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11464,10 +11467,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11654,12 +11653,12 @@
   </sheetPr>
   <dimension ref="1:66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="P54" activeCellId="0" sqref="P54"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="J60" activeCellId="0" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -15423,8 +15422,8 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16819,8 +16818,9 @@
       <c r="E24" s="74" t="s">
         <v>245</v>
       </c>
-      <c r="F24" s="74" t="n">
-        <v>25.5</v>
+      <c r="F24" s="95" t="n">
+        <f aca="false">'Modes A-F'!E54</f>
+        <v>29.573</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="74" t="s">
@@ -16841,8 +16841,9 @@
       <c r="E25" s="74" t="s">
         <v>247</v>
       </c>
-      <c r="F25" s="74" t="n">
-        <v>-42.6</v>
+      <c r="F25" s="95" t="n">
+        <f aca="false">'Modes A-F'!G54</f>
+        <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
       <c r="H25" s="74" t="s">
@@ -16863,8 +16864,9 @@
       <c r="E26" s="74" t="s">
         <v>249</v>
       </c>
-      <c r="F26" s="74" t="n">
-        <v>-17.25</v>
+      <c r="F26" s="95" t="n">
+        <f aca="false">'Modes A-F'!I54</f>
+        <v>-20.5991</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="74" t="s">
@@ -16885,8 +16887,9 @@
       <c r="E27" s="74" t="s">
         <v>251</v>
       </c>
-      <c r="F27" s="74" t="n">
-        <v>46.1092</v>
+      <c r="F27" s="95" t="n">
+        <f aca="false">'Modes A-F'!K54</f>
+        <v>45.575</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -16903,8 +16906,9 @@
       <c r="E28" s="74" t="s">
         <v>252</v>
       </c>
-      <c r="F28" s="74" t="n">
-        <v>46.1092</v>
+      <c r="F28" s="95" t="n">
+        <f aca="false">'Modes A-F'!M54</f>
+        <v>44.962</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -16921,8 +16925,9 @@
       <c r="E29" s="74" t="s">
         <v>253</v>
       </c>
-      <c r="F29" s="74" t="n">
-        <v>19.5956</v>
+      <c r="F29" s="95" t="n">
+        <f aca="false">'Modes A-F'!O54</f>
+        <v>19.847</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -16939,8 +16944,9 @@
       <c r="E30" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="F30" s="74" t="n">
-        <v>32.4638</v>
+      <c r="F30" s="95" t="n">
+        <f aca="false">'Modes A-F'!T54</f>
+        <v>51.2907</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -17016,14 +17022,14 @@
       <c r="D1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="96" t="s">
         <v>255</v>
       </c>
-      <c r="F1" s="95"/>
-      <c r="G1" s="96" t="s">
+      <c r="F1" s="96"/>
+      <c r="G1" s="97" t="s">
         <v>256</v>
       </c>
-      <c r="H1" s="96"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17049,25 +17055,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="98" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="98" t="s">
+      <c r="C3" s="99" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="98" t="s">
+      <c r="D3" s="99" t="s">
         <v>257</v>
       </c>
-      <c r="E3" s="98" t="n">
+      <c r="E3" s="99" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="98" t="n">
+      <c r="F3" s="99" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="99" t="n">
+      <c r="G3" s="100" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="100" t="n">
+      <c r="H3" s="101" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17130,11 +17136,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="101" t="s">
+      <c r="I6" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17146,9 +17152,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17175,7 +17181,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -17190,26 +17196,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="102"/>
-      <c r="B1" s="103"/>
-      <c r="C1" s="103"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="104" t="s">
+      <c r="A1" s="103"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="105" t="s">
         <v>262</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="105" t="s">
+      <c r="G1" s="106" t="s">
         <v>263</v>
       </c>
-      <c r="H1" s="106" t="s">
+      <c r="H1" s="107" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="107"/>
-      <c r="D2" s="108" t="s">
+      <c r="A2" s="108"/>
+      <c r="D2" s="109" t="s">
         <v>265</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17218,22 +17224,22 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="109"/>
+      <c r="G2" s="110"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="110" t="s">
+      <c r="A3" s="111" t="s">
         <v>266</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="108" t="s">
+      <c r="D3" s="109" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="111" t="n">
+      <c r="E3" s="112" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="112" t="n">
+      <c r="F3" s="95" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
@@ -17247,21 +17253,21 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="111" t="s">
         <v>268</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="108" t="s">
+      <c r="D4" s="109" t="s">
         <v>269</v>
       </c>
-      <c r="E4" s="112" t="n">
+      <c r="E4" s="95" t="n">
         <f aca="false">'Modes A-F'!K56</f>
         <v>129</v>
       </c>
-      <c r="F4" s="112" t="n">
+      <c r="F4" s="95" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
         <v>100.088913266688</v>
       </c>
@@ -17318,8 +17324,8 @@
       </c>
       <c r="B8" s="120"/>
       <c r="C8" s="120"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="103"/>
+      <c r="D8" s="104"/>
+      <c r="E8" s="104"/>
       <c r="F8" s="121" t="s">
         <v>273</v>
       </c>
@@ -17328,26 +17334,26 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="107"/>
-      <c r="D9" s="108" t="s">
+      <c r="A9" s="108"/>
+      <c r="D9" s="109" t="s">
         <v>265</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="109" t="n">
+      <c r="G9" s="110" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="111" t="s">
         <v>274</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="108" t="s">
+      <c r="D10" s="109" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="114" t="n">
@@ -17361,14 +17367,14 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="110" t="s">
+      <c r="A11" s="111" t="s">
         <v>275</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="108" t="s">
+      <c r="D11" s="109" t="s">
         <v>269</v>
       </c>
       <c r="E11" s="114" t="n">
@@ -17409,20 +17415,20 @@
       </c>
       <c r="B16" s="120"/>
       <c r="C16" s="120"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
+      <c r="D16" s="104"/>
+      <c r="E16" s="104"/>
       <c r="F16" s="121" t="s">
         <v>273</v>
       </c>
-      <c r="G16" s="103" t="n">
+      <c r="G16" s="104" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="103"/>
+      <c r="H16" s="104"/>
       <c r="I16" s="122"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="107"/>
-      <c r="D17" s="108" t="s">
+      <c r="A17" s="108"/>
+      <c r="D17" s="109" t="s">
         <v>265</v>
       </c>
       <c r="E17" s="0" t="n">
@@ -17435,19 +17441,19 @@
       <c r="H17" s="126" t="s">
         <v>277</v>
       </c>
-      <c r="I17" s="109" t="n">
+      <c r="I17" s="110" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="110" t="s">
+      <c r="A18" s="111" t="s">
         <v>278</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="108" t="s">
+      <c r="D18" s="109" t="s">
         <v>279</v>
       </c>
       <c r="E18" s="0" t="n">
@@ -17457,11 +17463,11 @@
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="109"/>
+      <c r="I18" s="110"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="107"/>
-      <c r="D19" s="108" t="s">
+      <c r="A19" s="108"/>
+      <c r="D19" s="109" t="s">
         <v>280</v>
       </c>
       <c r="E19" s="0" t="n">
@@ -17472,31 +17478,31 @@
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="109"/>
+      <c r="I19" s="110"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="107"/>
-      <c r="D20" s="108"/>
+      <c r="A20" s="108"/>
+      <c r="D20" s="109"/>
       <c r="G20" s="128" t="s">
         <v>281</v>
       </c>
-      <c r="I20" s="109"/>
+      <c r="I20" s="110"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="107"/>
+      <c r="A21" s="108"/>
       <c r="F21" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="I21" s="109"/>
+      <c r="I21" s="110"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="111" t="s">
         <v>266</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="108" t="s">
+      <c r="D22" s="109" t="s">
         <v>267</v>
       </c>
       <c r="E22" s="114" t="n">
@@ -17511,17 +17517,17 @@
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
         <v>-33.44202924884</v>
       </c>
-      <c r="I22" s="109"/>
+      <c r="I22" s="110"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="111" t="s">
         <v>268</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="108" t="s">
+      <c r="D23" s="109" t="s">
         <v>269</v>
       </c>
       <c r="E23" s="114" t="n">
@@ -17536,7 +17542,7 @@
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
         <v>42.4358981480704</v>
       </c>
-      <c r="I23" s="109"/>
+      <c r="I23" s="110"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="115" t="s">
@@ -17571,20 +17577,20 @@
       </c>
       <c r="B28" s="134"/>
       <c r="C28" s="134"/>
-      <c r="D28" s="103"/>
-      <c r="E28" s="103"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="104"/>
       <c r="F28" s="121" t="s">
         <v>273</v>
       </c>
-      <c r="G28" s="103" t="n">
+      <c r="G28" s="104" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="103"/>
+      <c r="H28" s="104"/>
       <c r="I28" s="122"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="107"/>
-      <c r="D29" s="108" t="s">
+      <c r="A29" s="108"/>
+      <c r="D29" s="109" t="s">
         <v>265</v>
       </c>
       <c r="E29" s="0" t="n">
@@ -17597,19 +17603,19 @@
       <c r="H29" s="126" t="s">
         <v>277</v>
       </c>
-      <c r="I29" s="109" t="n">
+      <c r="I29" s="110" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="111" t="s">
         <v>278</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="108" t="s">
+      <c r="D30" s="109" t="s">
         <v>279</v>
       </c>
       <c r="E30" s="0" t="n">
@@ -17619,11 +17625,11 @@
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="109"/>
+      <c r="I30" s="110"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="107"/>
-      <c r="D31" s="108" t="s">
+      <c r="A31" s="108"/>
+      <c r="D31" s="109" t="s">
         <v>280</v>
       </c>
       <c r="E31" s="0" t="n">
@@ -17634,31 +17640,31 @@
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="109"/>
+      <c r="I31" s="110"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="107"/>
-      <c r="D32" s="108"/>
+      <c r="A32" s="108"/>
+      <c r="D32" s="109"/>
       <c r="G32" s="128" t="s">
         <v>281</v>
       </c>
-      <c r="I32" s="109"/>
+      <c r="I32" s="110"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="107"/>
+      <c r="A33" s="108"/>
       <c r="F33" s="129" t="s">
         <v>263</v>
       </c>
-      <c r="I33" s="109"/>
+      <c r="I33" s="110"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="111" t="s">
         <v>266</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="108" t="s">
+      <c r="D34" s="109" t="s">
         <v>267</v>
       </c>
       <c r="E34" s="114" t="n">
@@ -17673,17 +17679,17 @@
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
         <v>-60.4500007866982</v>
       </c>
-      <c r="I34" s="109"/>
+      <c r="I34" s="110"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="110" t="s">
+      <c r="A35" s="111" t="s">
         <v>268</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="108" t="s">
+      <c r="D35" s="109" t="s">
         <v>269</v>
       </c>
       <c r="E35" s="114" t="n">
@@ -17698,7 +17704,7 @@
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
         <v>13.5227875381681</v>
       </c>
-      <c r="I35" s="109"/>
+      <c r="I35" s="110"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="115" t="s">

</xml_diff>

<commit_message>
update Modes and cadashboard
also implement single source for DCM parameters for BlueSky and
non-BlueSky applications
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -11653,12 +11653,12 @@
   </sheetPr>
   <dimension ref="1:66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="J60" activeCellId="0" sqref="J60"/>
+      <selection pane="bottomRight" activeCell="O58" activeCellId="0" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -14637,10 +14637,10 @@
         <v>-241810</v>
       </c>
       <c r="K54" s="57" t="n">
-        <v>45.575</v>
+        <v>44.825</v>
       </c>
       <c r="L54" s="28" t="n">
-        <v>419898</v>
+        <v>412437</v>
       </c>
       <c r="M54" s="57" t="n">
         <v>44.962</v>
@@ -14800,7 +14800,7 @@
         <v>10042276</v>
       </c>
       <c r="O56" s="60" t="n">
-        <v>103.91</v>
+        <v>101.91</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8736787</v>
@@ -14862,7 +14862,7 @@
         <v>7596748</v>
       </c>
       <c r="O57" s="61" t="n">
-        <v>100.43</v>
+        <v>98.43</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>6110187</v>
@@ -14916,7 +14916,7 @@
         <v>6400000</v>
       </c>
       <c r="O58" s="61" t="n">
-        <v>100.43</v>
+        <v>98.43</v>
       </c>
       <c r="P58" s="30" t="n">
         <v>4913439</v>
@@ -15422,8 +15422,8 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="1" sqref="O58 F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16889,7 +16889,7 @@
       </c>
       <c r="F27" s="95" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>45.575</v>
+        <v>44.825</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -16997,7 +16997,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="O58 G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -17181,7 +17181,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="O58 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -17273,11 +17273,11 @@
       </c>
       <c r="G4" s="113" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>103.91</v>
+        <v>101.91</v>
       </c>
       <c r="H4" s="114" t="n">
         <f aca="false">G4-F4</f>
-        <v>3.82108673331224</v>
+        <v>1.821086733312</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17302,17 +17302,17 @@
       </c>
       <c r="G5" s="119" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>100.43</v>
+        <v>98.43</v>
       </c>
       <c r="H5" s="114" t="n">
         <f aca="false">G5-F5</f>
-        <v>3.80609712834968</v>
+        <v>1.80609712834971</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="114" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>2.79035495998454</v>
+        <v>1.45702162665114</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>272</v>
@@ -17757,7 +17757,7 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O58 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -23829,7 +23829,7 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="O58 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
change dcm_roll homing speed, update Modes
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11657,11 +11657,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="N38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="O40" activeCellId="0" sqref="O40:P41"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="K42" activeCellId="0" sqref="K42:P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11670,7 +11670,8 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0408163265306"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.219387755102"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.3724489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.5612244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8622448979592"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.5612244897959"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="2" width="15.5612244897959"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="15.5612244897959"/>
@@ -13814,49 +13815,49 @@
         <v>141</v>
       </c>
       <c r="E42" s="37" t="n">
-        <v>209762</v>
+        <v>212225</v>
       </c>
       <c r="F42" s="35" t="n">
-        <v>209763</v>
+        <v>212225</v>
       </c>
       <c r="G42" s="37" t="n">
-        <v>209762</v>
+        <v>212225</v>
       </c>
       <c r="H42" s="35" t="n">
-        <v>209763</v>
+        <v>212225</v>
       </c>
       <c r="I42" s="37" t="n">
-        <v>209762</v>
+        <v>212225</v>
       </c>
       <c r="J42" s="35" t="n">
-        <v>209763</v>
-      </c>
-      <c r="K42" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" s="45" t="n">
-        <v>0</v>
+        <v>212225</v>
+      </c>
+      <c r="K42" s="37" t="n">
+        <v>212225</v>
+      </c>
+      <c r="L42" s="35" t="n">
+        <v>212225</v>
       </c>
       <c r="M42" s="37" t="n">
-        <v>0</v>
+        <v>212225</v>
       </c>
       <c r="N42" s="35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" s="45" t="n">
-        <v>0</v>
+        <v>212225</v>
+      </c>
+      <c r="O42" s="37" t="n">
+        <v>212225</v>
+      </c>
+      <c r="P42" s="35" t="n">
+        <v>212225</v>
       </c>
       <c r="Q42" s="26"/>
       <c r="R42" s="26"/>
       <c r="S42" s="26"/>
       <c r="T42" s="56" t="n">
-        <v>119996</v>
+        <v>112238</v>
       </c>
       <c r="U42" s="45" t="n">
-        <v>119996</v>
+        <v>112238</v>
       </c>
       <c r="V42" s="0"/>
       <c r="W42" s="0"/>
@@ -14451,7 +14452,7 @@
       <c r="P51" s="32" t="n">
         <v>36496</v>
       </c>
-      <c r="T51" s="33" t="n">
+      <c r="T51" s="31" t="n">
         <v>0.5</v>
       </c>
       <c r="U51" s="32" t="n">
@@ -14508,7 +14509,7 @@
       <c r="Q52" s="26"/>
       <c r="R52" s="26"/>
       <c r="S52" s="26"/>
-      <c r="T52" s="37" t="n">
+      <c r="T52" s="38" t="n">
         <v>-0.5</v>
       </c>
       <c r="U52" s="45" t="n">
@@ -14658,10 +14659,10 @@
         <v>145846</v>
       </c>
       <c r="T54" s="58" t="n">
-        <v>51.2907</v>
+        <v>52.606</v>
       </c>
       <c r="U54" s="28" t="n">
-        <v>477063</v>
+        <v>490252</v>
       </c>
       <c r="V54" s="0"/>
       <c r="W54" s="0"/>
@@ -15426,7 +15427,7 @@
   <dimension ref="1:31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="1" sqref="O40:P41 C25"/>
+      <selection pane="topLeft" activeCell="C25" activeCellId="1" sqref="K42:P42 C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16949,7 +16950,7 @@
       </c>
       <c r="F30" s="95" t="n">
         <f aca="false">'Modes A-F'!T54</f>
-        <v>51.2907</v>
+        <v>52.606</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
@@ -17000,7 +17001,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="O40:P41 G11"/>
+      <selection pane="bottomRight" activeCell="G11" activeCellId="1" sqref="K42:P42 G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -17184,7 +17185,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="O40:P41 E4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="1" sqref="K42:P42 E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -17760,7 +17761,7 @@
   <dimension ref="A1:CX484"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O40:P41 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="K42:P42 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -23832,7 +23833,7 @@
   <dimension ref="A1:G2383"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="O40:P41 B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="K42:P42 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
update Modes, slot numbers in cadashboard
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="247" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -10700,7 +10700,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10729,6 +10729,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF3333"/>
         <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
     <fill>
@@ -11020,7 +11026,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="147">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11265,7 +11271,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11273,7 +11295,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11329,7 +11363,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11377,7 +11411,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11569,7 +11603,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11629,7 +11663,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFF9999"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF2DED5"/>
       <rgbColor rgb="FF3366FF"/>
@@ -11661,11 +11695,11 @@
   <dimension ref="1:66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="I38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="N32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
-      <selection pane="bottomRight" activeCell="G62" activeCellId="0" sqref="G62"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="T55" activeCellId="0" sqref="T55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -11866,7 +11900,7 @@
       <c r="P5" s="25"/>
       <c r="Q5" s="26"/>
       <c r="R5" s="26" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="S5" s="26"/>
       <c r="T5" s="27"/>
@@ -11911,7 +11945,7 @@
       <c r="O6" s="30"/>
       <c r="P6" s="32"/>
       <c r="R6" s="0" t="n">
-        <v>1.1</v>
+        <v>-0.4006</v>
       </c>
       <c r="T6" s="30"/>
       <c r="U6" s="32"/>
@@ -11936,7 +11970,7 @@
       <c r="O7" s="30"/>
       <c r="P7" s="32"/>
       <c r="R7" s="0" t="n">
-        <v>0.6</v>
+        <v>1.1</v>
       </c>
       <c r="T7" s="30"/>
       <c r="U7" s="32"/>
@@ -11994,7 +12028,7 @@
       <c r="O9" s="31"/>
       <c r="P9" s="34"/>
       <c r="R9" s="0" t="n">
-        <v>2.0948</v>
+        <v>0.59132</v>
       </c>
       <c r="T9" s="30"/>
       <c r="U9" s="32"/>
@@ -12023,7 +12057,7 @@
       <c r="O10" s="31"/>
       <c r="P10" s="34"/>
       <c r="R10" s="0" t="n">
-        <v>2.06708</v>
+        <v>3.10056</v>
       </c>
       <c r="T10" s="30"/>
       <c r="U10" s="32"/>
@@ -12052,7 +12086,7 @@
       <c r="O11" s="31"/>
       <c r="P11" s="34"/>
       <c r="R11" s="0" t="n">
-        <v>4.1</v>
+        <v>3.5994</v>
       </c>
       <c r="T11" s="30"/>
       <c r="U11" s="32"/>
@@ -12081,7 +12115,7 @@
       <c r="O12" s="31"/>
       <c r="P12" s="34"/>
       <c r="R12" s="0" t="n">
-        <v>0.50004</v>
+        <v>0.75</v>
       </c>
       <c r="T12" s="30"/>
       <c r="U12" s="32"/>
@@ -12110,7 +12144,7 @@
       <c r="O13" s="31"/>
       <c r="P13" s="34"/>
       <c r="R13" s="0" t="n">
-        <v>-1.49904</v>
+        <v>-2.99692</v>
       </c>
       <c r="T13" s="30"/>
       <c r="U13" s="32"/>
@@ -12139,7 +12173,7 @@
       <c r="O14" s="31"/>
       <c r="P14" s="34"/>
       <c r="R14" s="0" t="n">
-        <v>-0.413</v>
+        <v>-1.44644</v>
       </c>
       <c r="T14" s="30"/>
       <c r="U14" s="32"/>
@@ -12168,7 +12202,7 @@
       <c r="O15" s="31"/>
       <c r="P15" s="34"/>
       <c r="R15" s="0" t="n">
-        <v>-1.9002</v>
+        <v>-4.40048</v>
       </c>
       <c r="T15" s="30"/>
       <c r="U15" s="32"/>
@@ -12198,7 +12232,7 @@
       <c r="P16" s="39"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26" t="n">
-        <v>-0.10008</v>
+        <v>-0.34996</v>
       </c>
       <c r="S16" s="26"/>
       <c r="T16" s="27"/>
@@ -14629,41 +14663,41 @@
         <v>181</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>28.6621</v>
+        <v>28.6041</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>250802</v>
+        <v>250227</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="57" t="n">
-        <v>-21.286</v>
+        <v>-21.8487</v>
       </c>
       <c r="J54" s="28" t="n">
-        <v>-248676</v>
+        <v>-254305</v>
       </c>
       <c r="K54" s="57" t="n">
-        <v>44.014</v>
+        <v>42.895</v>
       </c>
       <c r="L54" s="28" t="n">
-        <v>404304</v>
+        <v>393129</v>
       </c>
       <c r="M54" s="57" t="n">
-        <v>43.915</v>
+        <v>43.656</v>
       </c>
       <c r="N54" s="28" t="n">
-        <v>404328</v>
+        <v>400737</v>
       </c>
       <c r="O54" s="57" t="n">
-        <v>18.169</v>
+        <v>16.844</v>
       </c>
       <c r="P54" s="28" t="n">
-        <v>145846</v>
+        <v>132625</v>
       </c>
       <c r="T54" s="58" t="n">
-        <v>52.6071</v>
+        <v>52.1071</v>
       </c>
       <c r="U54" s="28" t="n">
         <v>490232</v>
@@ -14778,40 +14812,40 @@
         <v>188</v>
       </c>
       <c r="E56" s="60" t="n">
-        <v>112.987</v>
+        <v>113.287</v>
       </c>
       <c r="F56" s="25" t="n">
-        <v>9209080</v>
-      </c>
-      <c r="G56" s="60" t="n">
+        <v>9224687</v>
+      </c>
+      <c r="G56" s="61" t="n">
         <v>24.4104</v>
       </c>
-      <c r="H56" s="23" t="n">
+      <c r="H56" s="62" t="n">
         <v>4600216</v>
       </c>
       <c r="I56" s="60" t="n">
-        <v>58.859</v>
+        <v>58.3089</v>
       </c>
       <c r="J56" s="23" t="n">
-        <v>6392661</v>
+        <v>6364039</v>
       </c>
       <c r="K56" s="60" t="n">
-        <v>128.679</v>
+        <v>127.735</v>
       </c>
       <c r="L56" s="23" t="n">
-        <v>10025575</v>
+        <v>9976463</v>
       </c>
       <c r="M56" s="60" t="n">
-        <v>128.526</v>
+        <v>127.735</v>
       </c>
       <c r="N56" s="23" t="n">
-        <v>10017600</v>
+        <v>9976463</v>
       </c>
       <c r="O56" s="60" t="n">
-        <v>100.534</v>
+        <v>99.605</v>
       </c>
       <c r="P56" s="23" t="n">
-        <v>8561136</v>
+        <v>8512779</v>
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" s="26"/>
@@ -14839,41 +14873,41 @@
       <c r="D57" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="E57" s="61" t="n">
-        <v>111.113</v>
+      <c r="E57" s="63" t="n">
+        <v>106.013</v>
       </c>
       <c r="F57" s="32" t="n">
-        <v>6666042</v>
-      </c>
-      <c r="G57" s="61" t="n">
+        <v>6400669</v>
+      </c>
+      <c r="G57" s="64" t="n">
         <v>12.81</v>
       </c>
-      <c r="H57" s="32" t="n">
+      <c r="H57" s="65" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="61" t="n">
-        <v>52.229</v>
+      <c r="I57" s="63" t="n">
+        <v>44.4788</v>
       </c>
       <c r="J57" s="32" t="n">
-        <v>3602156</v>
-      </c>
-      <c r="K57" s="61" t="n">
-        <v>128.447</v>
+        <v>3198895</v>
+      </c>
+      <c r="K57" s="63" t="n">
+        <v>120.891</v>
       </c>
       <c r="L57" s="32" t="n">
-        <v>7567975</v>
-      </c>
-      <c r="M57" s="61" t="n">
-        <v>128.294</v>
+        <v>7174815</v>
+      </c>
+      <c r="M57" s="63" t="n">
+        <v>120.891</v>
       </c>
       <c r="N57" s="32" t="n">
-        <v>7560000</v>
-      </c>
-      <c r="O57" s="61" t="n">
-        <v>100.302</v>
+        <v>7174815</v>
+      </c>
+      <c r="O57" s="63" t="n">
+        <v>89.3728</v>
       </c>
       <c r="P57" s="32" t="n">
-        <v>6103536</v>
+        <v>5534847</v>
       </c>
       <c r="T57" s="30" t="n">
         <v>138.4</v>
@@ -14893,41 +14927,41 @@
       <c r="D58" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="E58" s="61" t="n">
-        <v>111.113</v>
+      <c r="E58" s="63" t="n">
+        <v>106.013</v>
       </c>
       <c r="F58" s="28" t="n">
-        <v>5469294</v>
-      </c>
-      <c r="G58" s="61" t="n">
+        <v>5203921</v>
+      </c>
+      <c r="G58" s="64" t="n">
         <v>12.81</v>
       </c>
-      <c r="H58" s="32" t="n">
+      <c r="H58" s="65" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="61" t="n">
-        <v>52.229</v>
+      <c r="I58" s="63" t="n">
+        <v>44.4788</v>
       </c>
       <c r="J58" s="32" t="n">
-        <v>2405408</v>
-      </c>
-      <c r="K58" s="61" t="n">
-        <v>128.447</v>
+        <v>2002147</v>
+      </c>
+      <c r="K58" s="63" t="n">
+        <v>120.891</v>
       </c>
       <c r="L58" s="32" t="n">
-        <v>6371227</v>
-      </c>
-      <c r="M58" s="61" t="n">
-        <v>128.294</v>
+        <v>5978067</v>
+      </c>
+      <c r="M58" s="63" t="n">
+        <v>120.891</v>
       </c>
       <c r="N58" s="32" t="n">
-        <v>6363252</v>
-      </c>
-      <c r="O58" s="61" t="n">
-        <v>100.302</v>
-      </c>
-      <c r="P58" s="62" t="n">
-        <v>4906788</v>
+        <v>5978067</v>
+      </c>
+      <c r="O58" s="63" t="n">
+        <v>89.3728</v>
+      </c>
+      <c r="P58" s="66" t="n">
+        <v>4338099</v>
       </c>
       <c r="T58" s="27" t="n">
         <v>138.4</v>
@@ -14952,43 +14986,43 @@
       <c r="D59" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="E59" s="61" t="n">
+      <c r="E59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="F59" s="28" t="n">
         <v>-412000</v>
       </c>
-      <c r="G59" s="61" t="n">
+      <c r="G59" s="64" t="n">
         <v>-0.6</v>
       </c>
-      <c r="H59" s="28" t="n">
+      <c r="H59" s="67" t="n">
         <v>-412000</v>
       </c>
-      <c r="I59" s="61" t="n">
+      <c r="I59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="J59" s="28" t="n">
         <v>-412000</v>
       </c>
-      <c r="K59" s="61" t="n">
+      <c r="K59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="L59" s="28" t="n">
         <v>-412000</v>
       </c>
-      <c r="M59" s="61" t="n">
+      <c r="M59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="N59" s="28" t="n">
         <v>-412000</v>
       </c>
-      <c r="O59" s="61" t="n">
+      <c r="O59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="P59" s="28" t="n">
         <v>-412000</v>
       </c>
-      <c r="T59" s="61" t="n">
+      <c r="T59" s="63" t="n">
         <v>-0.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -15006,46 +15040,46 @@
       <c r="D60" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="E60" s="63" t="n">
+      <c r="E60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="F60" s="47" t="n">
         <v>-199443</v>
       </c>
-      <c r="G60" s="63" t="n">
+      <c r="G60" s="69" t="n">
         <v>33.3721</v>
       </c>
-      <c r="H60" s="47" t="n">
+      <c r="H60" s="70" t="n">
         <v>-199443</v>
       </c>
-      <c r="I60" s="63" t="n">
+      <c r="I60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="J60" s="47" t="n">
         <v>-199443</v>
       </c>
-      <c r="K60" s="63" t="n">
+      <c r="K60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="L60" s="47" t="n">
         <v>-199443</v>
       </c>
-      <c r="M60" s="63" t="n">
+      <c r="M60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="N60" s="47" t="n">
         <v>-199443</v>
       </c>
-      <c r="O60" s="63" t="n">
+      <c r="O60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="P60" s="47" t="n">
         <v>-199443</v>
       </c>
-      <c r="Q60" s="64"/>
-      <c r="R60" s="64"/>
-      <c r="S60" s="64"/>
-      <c r="T60" s="63" t="n">
+      <c r="Q60" s="71"/>
+      <c r="R60" s="71"/>
+      <c r="S60" s="71"/>
+      <c r="T60" s="68" t="n">
         <v>33.3721</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15058,52 +15092,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="65" t="s">
+      <c r="A61" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="66" t="s">
+      <c r="B61" s="73" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="67" t="s">
+      <c r="C61" s="74" t="s">
         <v>203</v>
       </c>
-      <c r="D61" s="67" t="s">
+      <c r="D61" s="74" t="s">
         <v>204</v>
       </c>
-      <c r="E61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="69" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="69" t="n">
+      <c r="E61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="76" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15114,8 +15148,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="65"/>
-      <c r="B62" s="70" t="s">
+      <c r="A62" s="72"/>
+      <c r="B62" s="77" t="s">
         <v>205</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15168,8 +15202,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="65"/>
-      <c r="B63" s="70" t="s">
+      <c r="A63" s="72"/>
+      <c r="B63" s="77" t="s">
         <v>208</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15222,8 +15256,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="65"/>
-      <c r="B64" s="70" t="s">
+      <c r="A64" s="72"/>
+      <c r="B64" s="77" t="s">
         <v>211</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15276,8 +15310,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="65"/>
-      <c r="B65" s="70" t="s">
+      <c r="A65" s="72"/>
+      <c r="B65" s="77" t="s">
         <v>214</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15330,53 +15364,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="65"/>
-      <c r="B66" s="71" t="s">
+      <c r="A66" s="72"/>
+      <c r="B66" s="78" t="s">
         <v>217</v>
       </c>
-      <c r="C66" s="72" t="s">
+      <c r="C66" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="72" t="s">
+      <c r="D66" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="E66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="63" t="n">
+      <c r="E66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="68" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15431,39 +15465,39 @@
   <dimension ref="1:31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="75" width="3.0969387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="75" width="13.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="75" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="82" width="3.0969387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="82" width="13.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="82" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="75"/>
+    <row r="1" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="82"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="AMJ1" s="75"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="AMJ1" s="82"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="84" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16484,168 +16518,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="82" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="78"/>
-      <c r="B3" s="79"/>
-      <c r="C3" s="80" t="s">
+    <row r="3" s="89" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="85"/>
+      <c r="B3" s="86"/>
+      <c r="C3" s="87" t="s">
         <v>221</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="87" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="81" t="s">
+      <c r="E3" s="88" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="78"/>
-      <c r="L3" s="78"/>
-      <c r="AMJ3" s="78"/>
-    </row>
-    <row r="4" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75"/>
-      <c r="B4" s="79" t="s">
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="AMJ3" s="85"/>
+    </row>
+    <row r="4" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="82"/>
+      <c r="B4" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75" t="n">
+      <c r="C4" s="82"/>
+      <c r="D4" s="82" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="83" t="n">
+      <c r="E4" s="90" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="AMJ4" s="75"/>
-    </row>
-    <row r="5" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75"/>
-      <c r="B5" s="79" t="s">
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="AMJ4" s="82"/>
+    </row>
+    <row r="5" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="82"/>
+      <c r="B5" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="82" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="75" t="n">
+      <c r="D5" s="82" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="AMJ5" s="75"/>
-    </row>
-    <row r="6" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75"/>
-      <c r="B6" s="79" t="s">
+      <c r="E5" s="90"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="AMJ5" s="82"/>
+    </row>
+    <row r="6" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="82"/>
+      <c r="B6" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="82" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="75" t="n">
+      <c r="D6" s="82" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="AMJ6" s="75"/>
-    </row>
-    <row r="7" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75"/>
-      <c r="B7" s="79" t="s">
+      <c r="E6" s="90"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="AMJ6" s="82"/>
+    </row>
+    <row r="7" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="82"/>
+      <c r="B7" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="82" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="75" t="n">
+      <c r="D7" s="82" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="AMJ7" s="75"/>
-    </row>
-    <row r="8" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="75"/>
-      <c r="B8" s="79" t="s">
+      <c r="E7" s="90"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="AMJ7" s="82"/>
+    </row>
+    <row r="8" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="82"/>
+      <c r="B8" s="86" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="82" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="75" t="n">
+      <c r="D8" s="82" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="75"/>
-      <c r="K8" s="75"/>
-      <c r="L8" s="75"/>
-      <c r="AMJ8" s="75"/>
-    </row>
-    <row r="9" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="75"/>
-      <c r="B9" s="79" t="s">
+      <c r="E8" s="90"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="AMJ8" s="82"/>
+    </row>
+    <row r="9" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="82"/>
+      <c r="B9" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75" t="n">
+      <c r="C9" s="82"/>
+      <c r="D9" s="82" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-      <c r="AMJ9" s="75"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="AMJ9" s="82"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="91" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="85"/>
-      <c r="D10" s="85" t="n">
+      <c r="C10" s="92"/>
+      <c r="D10" s="92" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="86"/>
+      <c r="E10" s="93"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="95"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16654,8 +16688,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="87"/>
-      <c r="C12" s="88"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="95"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16664,82 +16698,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="96" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="89"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="90" t="s">
+      <c r="B14" s="97" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="91" t="s">
+      <c r="C14" s="98" t="s">
         <v>237</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="83"/>
+      <c r="E14" s="90"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="79" t="s">
+      <c r="B15" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="C15" s="75" t="n">
+      <c r="C15" s="82" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="83"/>
+      <c r="E15" s="90"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="79" t="s">
+      <c r="B16" s="86" t="s">
         <v>238</v>
       </c>
-      <c r="C16" s="92" t="n">
+      <c r="C16" s="99" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="83"/>
+      <c r="E16" s="90"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="86" t="s">
         <v>239</v>
       </c>
-      <c r="C17" s="75" t="n">
+      <c r="C17" s="82" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="83"/>
+      <c r="E17" s="90"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="84" t="s">
+      <c r="B18" s="91" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="85" t="n">
+      <c r="C18" s="92" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="86"/>
+      <c r="D18" s="92"/>
+      <c r="E18" s="93"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16766,213 +16800,213 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="89" t="s">
+      <c r="B21" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="89"/>
-      <c r="H21" s="89"/>
-      <c r="I21" s="89"/>
+      <c r="C21" s="96"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="96"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="96"/>
+      <c r="I21" s="96"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="93" t="s">
+      <c r="B22" s="100" t="s">
         <v>241</v>
       </c>
-      <c r="C22" s="93"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="87" t="s">
+      <c r="C22" s="100"/>
+      <c r="D22" s="83"/>
+      <c r="E22" s="94" t="s">
         <v>242</v>
       </c>
-      <c r="F22" s="87"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="94" t="s">
+      <c r="F22" s="94"/>
+      <c r="G22" s="83"/>
+      <c r="H22" s="101" t="s">
         <v>243</v>
       </c>
-      <c r="I22" s="94"/>
+      <c r="I22" s="101"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="97" t="s">
         <v>244</v>
       </c>
-      <c r="C23" s="91" t="s">
+      <c r="C23" s="98" t="s">
         <v>237</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="76" t="s">
+      <c r="E23" s="83" t="s">
         <v>244</v>
       </c>
-      <c r="F23" s="91" t="s">
+      <c r="F23" s="98" t="s">
         <v>237</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="76" t="s">
+      <c r="H23" s="83" t="s">
         <v>245</v>
       </c>
-      <c r="I23" s="95" t="s">
+      <c r="I23" s="102" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="86" t="s">
         <v>246</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="75" t="s">
+      <c r="E24" s="82" t="s">
         <v>246</v>
       </c>
-      <c r="F24" s="96" t="n">
+      <c r="F24" s="103" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>28.6621</v>
+        <v>28.6041</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="75" t="s">
+      <c r="H24" s="82" t="s">
         <v>247</v>
       </c>
-      <c r="I24" s="83" t="n">
+      <c r="I24" s="90" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="86" t="s">
         <v>248</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="75" t="s">
+      <c r="E25" s="82" t="s">
         <v>248</v>
       </c>
-      <c r="F25" s="96" t="n">
+      <c r="F25" s="103" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="75" t="s">
+      <c r="H25" s="82" t="s">
         <v>249</v>
       </c>
-      <c r="I25" s="83" t="n">
+      <c r="I25" s="90" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="86" t="s">
         <v>250</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="75" t="s">
+      <c r="E26" s="82" t="s">
         <v>250</v>
       </c>
-      <c r="F26" s="96" t="n">
+      <c r="F26" s="103" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-21.286</v>
+        <v>-21.8487</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="75" t="s">
+      <c r="H26" s="82" t="s">
         <v>251</v>
       </c>
-      <c r="I26" s="83" t="n">
+      <c r="I26" s="90" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="86" t="s">
         <v>252</v>
       </c>
-      <c r="C27" s="75" t="n">
+      <c r="C27" s="82" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="75" t="s">
+      <c r="E27" s="82" t="s">
         <v>252</v>
       </c>
-      <c r="F27" s="96" t="n">
+      <c r="F27" s="103" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>44.014</v>
+        <v>42.895</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="83"/>
+      <c r="I27" s="90"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="86" t="s">
         <v>253</v>
       </c>
-      <c r="C28" s="75" t="n">
+      <c r="C28" s="82" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="75" t="s">
+      <c r="E28" s="82" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="96" t="n">
+      <c r="F28" s="103" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.915</v>
+        <v>43.656</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="83"/>
+      <c r="I28" s="90"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="79" t="s">
+      <c r="B29" s="86" t="s">
         <v>254</v>
       </c>
-      <c r="C29" s="75" t="n">
+      <c r="C29" s="82" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="75" t="s">
+      <c r="E29" s="82" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="96" t="n">
+      <c r="F29" s="103" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>18.169</v>
+        <v>16.844</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="83"/>
+      <c r="I29" s="90"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="79" t="s">
+      <c r="B30" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="75" t="n">
+      <c r="C30" s="82" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="75" t="s">
+      <c r="E30" s="82" t="s">
         <v>255</v>
       </c>
-      <c r="F30" s="96" t="n">
+      <c r="F30" s="103" t="n">
         <f aca="false">'Modes A-F'!T54</f>
-        <v>52.6071</v>
+        <v>52.1071</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="83"/>
+      <c r="I30" s="90"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="84" t="s">
+      <c r="B31" s="91" t="s">
         <v>247</v>
       </c>
-      <c r="C31" s="85" t="n">
+      <c r="C31" s="92" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="85"/>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="86"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17030,14 +17064,14 @@
       <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="104" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="97"/>
-      <c r="G1" s="98" t="s">
+      <c r="F1" s="104"/>
+      <c r="G1" s="105" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="98"/>
+      <c r="H1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17063,25 +17097,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="99" t="s">
+      <c r="B3" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="100" t="s">
+      <c r="C3" s="107" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="100" t="s">
+      <c r="D3" s="107" t="s">
         <v>258</v>
       </c>
-      <c r="E3" s="100" t="n">
+      <c r="E3" s="107" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="100" t="n">
+      <c r="F3" s="107" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="101" t="n">
+      <c r="G3" s="108" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="102" t="n">
+      <c r="H3" s="109" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17144,11 +17178,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="103" t="s">
+      <c r="I6" s="110" t="s">
         <v>261</v>
       </c>
-      <c r="J6" s="103"/>
-      <c r="K6" s="103"/>
+      <c r="J6" s="110"/>
+      <c r="K6" s="110"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17160,9 +17194,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="103"/>
-      <c r="J7" s="103"/>
-      <c r="K7" s="103"/>
+      <c r="I7" s="110"/>
+      <c r="J7" s="110"/>
+      <c r="K7" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17204,26 +17238,26 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="104"/>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="105"/>
-      <c r="E1" s="106" t="s">
+      <c r="A1" s="111"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="113" t="s">
         <v>263</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="107" t="s">
+      <c r="G1" s="114" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="115" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="109"/>
-      <c r="D2" s="110" t="s">
+      <c r="A2" s="116"/>
+      <c r="D2" s="117" t="s">
         <v>266</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17232,514 +17266,514 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="111"/>
+      <c r="G2" s="118"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="112" t="s">
+      <c r="A3" s="119" t="s">
         <v>267</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="117" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="113" t="n">
+      <c r="E3" s="120" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="96" t="n">
+      <c r="F3" s="103" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="114" t="n">
+      <c r="G3" s="121" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>18.169</v>
-      </c>
-      <c r="H3" s="115" t="n">
+        <v>16.844</v>
+      </c>
+      <c r="H3" s="122" t="n">
         <f aca="false">G3-F3</f>
-        <v>-0.934118981708298</v>
+        <v>-2.2591189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="112" t="s">
+      <c r="A4" s="119" t="s">
         <v>269</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="117" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="96" t="n">
+      <c r="E4" s="103" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>128.679</v>
-      </c>
-      <c r="F4" s="96" t="n">
+        <v>127.735</v>
+      </c>
+      <c r="F4" s="103" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>99.7679132666878</v>
-      </c>
-      <c r="G4" s="114" t="n">
+        <v>98.8239132666878</v>
+      </c>
+      <c r="G4" s="121" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>100.534</v>
-      </c>
-      <c r="H4" s="115" t="n">
+        <v>99.605</v>
+      </c>
+      <c r="H4" s="122" t="n">
         <f aca="false">G4-F4</f>
-        <v>0.76608673331225</v>
+        <v>0.78108673331225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="123" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="117" t="n">
+      <c r="B5" s="124" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="D5" s="118" t="s">
+      <c r="C5" s="124"/>
+      <c r="D5" s="125" t="s">
         <v>272</v>
       </c>
-      <c r="E5" s="119" t="n">
+      <c r="E5" s="126" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>128.447</v>
-      </c>
-      <c r="F5" s="119" t="n">
+        <v>120.891</v>
+      </c>
+      <c r="F5" s="126" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>96.0709028716503</v>
-      </c>
-      <c r="G5" s="120" t="n">
+        <v>88.5149028716504</v>
+      </c>
+      <c r="G5" s="127" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>100.302</v>
-      </c>
-      <c r="H5" s="115" t="n">
+        <v>89.3728</v>
+      </c>
+      <c r="H5" s="122" t="n">
         <f aca="false">G5-F5</f>
-        <v>4.23109712834967</v>
+        <v>0.857897128349649</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="115" t="n">
+      <c r="H6" s="122" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>1.35435495998454</v>
+        <v>-0.206711706682133</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="121" t="s">
+      <c r="A8" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="121"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="122" t="s">
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="129" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="123" t="n">
+      <c r="G8" s="130" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="109"/>
-      <c r="D9" s="110" t="s">
+      <c r="A9" s="116"/>
+      <c r="D9" s="117" t="s">
         <v>266</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="111" t="n">
+      <c r="G9" s="118" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="112" t="s">
+      <c r="A10" s="119" t="s">
         <v>275</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="117" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="115" t="n">
+      <c r="E10" s="122" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>28.6621</v>
-      </c>
-      <c r="F10" s="115"/>
-      <c r="G10" s="124" t="n">
+        <v>28.6041</v>
+      </c>
+      <c r="F10" s="122"/>
+      <c r="G10" s="131" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>30.8435000290853</v>
+        <v>30.7855000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="119" t="s">
         <v>276</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="110" t="s">
+      <c r="D11" s="117" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="115" t="n">
+      <c r="E11" s="122" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>111.113</v>
-      </c>
-      <c r="F11" s="115"/>
-      <c r="G11" s="124" t="n">
+        <v>106.013</v>
+      </c>
+      <c r="F11" s="122"/>
+      <c r="G11" s="131" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>113.421400030779</v>
+        <v>108.321400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="123" t="s">
         <v>277</v>
       </c>
-      <c r="B12" s="117" t="n">
+      <c r="B12" s="124" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="117"/>
-      <c r="D12" s="118" t="s">
+      <c r="C12" s="124"/>
+      <c r="D12" s="125" t="s">
         <v>272</v>
       </c>
-      <c r="E12" s="125" t="n">
+      <c r="E12" s="132" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>111.113</v>
-      </c>
-      <c r="F12" s="125"/>
-      <c r="G12" s="126" t="n">
+        <v>106.013</v>
+      </c>
+      <c r="F12" s="132"/>
+      <c r="G12" s="133" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>113.652400033859</v>
+        <v>108.552400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="122" t="s">
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="129" t="s">
         <v>274</v>
       </c>
-      <c r="G16" s="105" t="n">
+      <c r="G16" s="112" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="105"/>
-      <c r="I16" s="123"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="130"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="109"/>
-      <c r="D17" s="110" t="s">
+      <c r="A17" s="116"/>
+      <c r="D17" s="117" t="s">
         <v>266</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="64" t="n">
+      <c r="G17" s="71" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="127" t="s">
+      <c r="H17" s="134" t="s">
         <v>278</v>
       </c>
-      <c r="I17" s="111" t="n">
+      <c r="I17" s="118" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="112" t="s">
+      <c r="A18" s="119" t="s">
         <v>279</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="110" t="s">
+      <c r="D18" s="117" t="s">
         <v>280</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="128" t="n">
+      <c r="G18" s="135" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="111"/>
+      <c r="I18" s="118"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="109"/>
-      <c r="D19" s="110" t="s">
+      <c r="A19" s="116"/>
+      <c r="D19" s="117" t="s">
         <v>281</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="64" t="n">
+      <c r="G19" s="71" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="111"/>
+      <c r="I19" s="118"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="109"/>
-      <c r="D20" s="110"/>
-      <c r="G20" s="129" t="s">
+      <c r="A20" s="116"/>
+      <c r="D20" s="117"/>
+      <c r="G20" s="136" t="s">
         <v>282</v>
       </c>
-      <c r="I20" s="111"/>
+      <c r="I20" s="118"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="109"/>
-      <c r="F21" s="130" t="s">
+      <c r="A21" s="116"/>
+      <c r="F21" s="137" t="s">
         <v>264</v>
       </c>
-      <c r="I21" s="111"/>
+      <c r="I21" s="118"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="119" t="s">
         <v>267</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="110" t="s">
+      <c r="D22" s="117" t="s">
         <v>268</v>
       </c>
-      <c r="E22" s="115" t="n">
+      <c r="E22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-39.3042914229833</v>
-      </c>
-      <c r="F22" s="131" t="n">
+        <v>-39.3622914229833</v>
+      </c>
+      <c r="F22" s="138" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-21.286</v>
-      </c>
-      <c r="G22" s="115" t="n">
+        <v>-21.8487</v>
+      </c>
+      <c r="G22" s="122" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-34.35292924884</v>
-      </c>
-      <c r="I22" s="111"/>
+        <v>-34.4109292488399</v>
+      </c>
+      <c r="I22" s="118"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="112" t="s">
+      <c r="A23" s="119" t="s">
         <v>269</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="110" t="s">
+      <c r="D23" s="117" t="s">
         <v>270</v>
       </c>
-      <c r="E23" s="115" t="n">
+      <c r="E23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>38.3522674801944</v>
-      </c>
-      <c r="F23" s="131" t="n">
+        <v>33.2522674801944</v>
+      </c>
+      <c r="F23" s="138" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>58.859</v>
-      </c>
-      <c r="G23" s="115" t="n">
+        <v>58.3089</v>
+      </c>
+      <c r="G23" s="122" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>43.6528981480704</v>
-      </c>
-      <c r="I23" s="111"/>
+        <v>38.5528981480704</v>
+      </c>
+      <c r="I23" s="118"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="116" t="s">
+      <c r="A24" s="123" t="s">
         <v>271</v>
       </c>
-      <c r="B24" s="117" t="n">
+      <c r="B24" s="124" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="117"/>
-      <c r="D24" s="118" t="s">
+      <c r="C24" s="124"/>
+      <c r="D24" s="125" t="s">
         <v>272</v>
       </c>
-      <c r="E24" s="125" t="n">
+      <c r="E24" s="132" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>29.6318517843995</v>
-      </c>
-      <c r="F24" s="132" t="n">
+        <v>24.5318517843995</v>
+      </c>
+      <c r="F24" s="139" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>52.229</v>
-      </c>
-      <c r="G24" s="133" t="n">
+        <v>44.4788</v>
+      </c>
+      <c r="G24" s="140" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>35.567766090482</v>
-      </c>
-      <c r="H24" s="117"/>
-      <c r="I24" s="134"/>
+        <v>30.467766090482</v>
+      </c>
+      <c r="H24" s="124"/>
+      <c r="I24" s="141"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="135" t="s">
+      <c r="A28" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="135"/>
-      <c r="C28" s="135"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="122" t="s">
+      <c r="B28" s="142"/>
+      <c r="C28" s="142"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="112"/>
+      <c r="F28" s="129" t="s">
         <v>274</v>
       </c>
-      <c r="G28" s="105" t="n">
+      <c r="G28" s="112" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="105"/>
-      <c r="I28" s="123"/>
+      <c r="H28" s="112"/>
+      <c r="I28" s="130"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="109"/>
-      <c r="D29" s="110" t="s">
+      <c r="A29" s="116"/>
+      <c r="D29" s="117" t="s">
         <v>266</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="64" t="n">
+      <c r="G29" s="71" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="127" t="s">
+      <c r="H29" s="134" t="s">
         <v>278</v>
       </c>
-      <c r="I29" s="111" t="n">
+      <c r="I29" s="118" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="112" t="s">
+      <c r="A30" s="119" t="s">
         <v>279</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="110" t="s">
+      <c r="D30" s="117" t="s">
         <v>280</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="128" t="n">
+      <c r="G30" s="135" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="111"/>
+      <c r="I30" s="118"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="109"/>
-      <c r="D31" s="110" t="s">
+      <c r="A31" s="116"/>
+      <c r="D31" s="117" t="s">
         <v>281</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="64" t="n">
+      <c r="G31" s="71" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="111"/>
+      <c r="I31" s="118"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="109"/>
-      <c r="D32" s="110"/>
-      <c r="G32" s="129" t="s">
+      <c r="A32" s="116"/>
+      <c r="D32" s="117"/>
+      <c r="G32" s="136" t="s">
         <v>282</v>
       </c>
-      <c r="I32" s="111"/>
+      <c r="I32" s="118"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="109"/>
-      <c r="F33" s="130" t="s">
+      <c r="A33" s="116"/>
+      <c r="F33" s="137" t="s">
         <v>264</v>
       </c>
-      <c r="I33" s="111"/>
+      <c r="I33" s="118"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="112" t="s">
+      <c r="A34" s="119" t="s">
         <v>267</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="110" t="s">
+      <c r="D34" s="117" t="s">
         <v>268</v>
       </c>
-      <c r="E34" s="115" t="n">
+      <c r="E34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-66.3125236638297</v>
-      </c>
-      <c r="F34" s="131" t="n">
+        <v>-66.3705236638297</v>
+      </c>
+      <c r="F34" s="138" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="115" t="n">
+      <c r="G34" s="122" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-61.3609007866982</v>
-      </c>
-      <c r="I34" s="111"/>
+        <v>-61.4189007866982</v>
+      </c>
+      <c r="I34" s="118"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="112" t="s">
+      <c r="A35" s="119" t="s">
         <v>269</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="110" t="s">
+      <c r="D35" s="117" t="s">
         <v>270</v>
       </c>
-      <c r="E35" s="115" t="n">
+      <c r="E35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>9.43887777734649</v>
-      </c>
-      <c r="F35" s="131" t="n">
+        <v>4.3388777773465</v>
+      </c>
+      <c r="F35" s="138" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="115" t="n">
+      <c r="G35" s="122" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>14.7397875381681</v>
-      </c>
-      <c r="I35" s="111"/>
+        <v>9.63978753816814</v>
+      </c>
+      <c r="I35" s="118"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="116" t="s">
+      <c r="A36" s="123" t="s">
         <v>271</v>
       </c>
-      <c r="B36" s="117" t="n">
+      <c r="B36" s="124" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="117"/>
-      <c r="D36" s="118" t="s">
+      <c r="C36" s="124"/>
+      <c r="D36" s="125" t="s">
         <v>272</v>
       </c>
-      <c r="E36" s="125" t="n">
+      <c r="E36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>-2.74682432571097</v>
-      </c>
-      <c r="F36" s="132" t="n">
+        <v>-7.84682432571097</v>
+      </c>
+      <c r="F36" s="139" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="125" t="n">
+      <c r="G36" s="132" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>3.18940252276749</v>
-      </c>
-      <c r="H36" s="117"/>
-      <c r="I36" s="134"/>
+        <v>-1.9105974772325</v>
+      </c>
+      <c r="H36" s="124"/>
+      <c r="I36" s="141"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17842,7 +17876,7 @@
       <c r="A9" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="136" t="n">
+      <c r="B9" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17866,7 +17900,7 @@
       <c r="A12" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="B12" s="136" t="n">
+      <c r="B12" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -17962,7 +17996,7 @@
       <c r="A24" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="B24" s="136" t="n">
+      <c r="B24" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17986,7 +18020,7 @@
       <c r="A27" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B27" s="136" t="n">
+      <c r="B27" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18082,7 +18116,7 @@
       <c r="A39" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="B39" s="136" t="n">
+      <c r="B39" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18106,7 +18140,7 @@
       <c r="A42" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B42" s="136" t="n">
+      <c r="B42" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18202,7 +18236,7 @@
       <c r="A54" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="B54" s="136" t="n">
+      <c r="B54" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18226,7 +18260,7 @@
       <c r="A57" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="B57" s="136" t="n">
+      <c r="B57" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18290,7 +18324,7 @@
       <c r="A65" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="B65" s="136" t="n">
+      <c r="B65" s="143" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18298,7 +18332,7 @@
       <c r="A66" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B66" s="136" t="n">
+      <c r="B66" s="143" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18306,7 +18340,7 @@
       <c r="A67" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B67" s="136" t="n">
+      <c r="B67" s="143" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18314,7 +18348,7 @@
       <c r="A68" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B68" s="136" t="n">
+      <c r="B68" s="143" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18634,7 +18668,7 @@
       <c r="A108" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="B108" s="136" t="n">
+      <c r="B108" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18658,7 +18692,7 @@
       <c r="A111" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="B111" s="136" t="n">
+      <c r="B111" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18754,7 +18788,7 @@
       <c r="A123" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="B123" s="136" t="n">
+      <c r="B123" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18778,7 +18812,7 @@
       <c r="A126" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="B126" s="136" t="n">
+      <c r="B126" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18874,7 +18908,7 @@
       <c r="A138" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="B138" s="136" t="n">
+      <c r="B138" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18898,7 +18932,7 @@
       <c r="A141" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="B141" s="136" t="n">
+      <c r="B141" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18994,7 +19028,7 @@
       <c r="A153" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="B153" s="136" t="n">
+      <c r="B153" s="143" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19018,7 +19052,7 @@
       <c r="A156" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="B156" s="136" t="n">
+      <c r="B156" s="143" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19082,7 +19116,7 @@
       <c r="A164" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="B164" s="136" t="n">
+      <c r="B164" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19090,7 +19124,7 @@
       <c r="A165" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B165" s="136" t="n">
+      <c r="B165" s="143" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19098,7 +19132,7 @@
       <c r="A166" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B166" s="136" t="n">
+      <c r="B166" s="143" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19106,7 +19140,7 @@
       <c r="A167" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B167" s="136" t="n">
+      <c r="B167" s="143" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19242,7 +19276,7 @@
       <c r="A184" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="B184" s="136" t="n">
+      <c r="B184" s="143" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19250,7 +19284,7 @@
       <c r="A185" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="B185" s="136" t="n">
+      <c r="B185" s="143" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19282,7 +19316,7 @@
       <c r="A189" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="B189" s="136" t="n">
+      <c r="B189" s="143" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19306,7 +19340,7 @@
       <c r="A192" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="B192" s="136" t="n">
+      <c r="B192" s="143" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19314,7 +19348,7 @@
       <c r="A193" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B193" s="136" t="n">
+      <c r="B193" s="143" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19322,7 +19356,7 @@
       <c r="A194" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B194" s="136" t="n">
+      <c r="B194" s="143" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19330,7 +19364,7 @@
       <c r="A195" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="B195" s="136" t="n">
+      <c r="B195" s="143" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20754,40 +20788,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="136" t="n">
+      <c r="C337" s="143" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="136" t="n">
+      <c r="D337" s="143" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="136" t="n">
+      <c r="E337" s="143" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="136" t="n">
+      <c r="F337" s="143" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="136" t="n">
+      <c r="G337" s="143" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="136" t="n">
+      <c r="H337" s="143" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="136" t="n">
+      <c r="I337" s="143" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="136" t="n">
+      <c r="J337" s="143" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="136" t="n">
+      <c r="K337" s="143" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="136" t="n">
+      <c r="L337" s="143" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="136" t="n">
+      <c r="M337" s="143" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="136" t="n">
+      <c r="N337" s="143" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20798,40 +20832,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="136" t="n">
+      <c r="C338" s="143" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="136" t="n">
+      <c r="D338" s="143" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="136" t="n">
+      <c r="E338" s="143" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="136" t="n">
+      <c r="F338" s="143" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="136" t="n">
+      <c r="G338" s="143" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="136" t="n">
+      <c r="H338" s="143" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="136" t="n">
+      <c r="I338" s="143" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="136" t="n">
+      <c r="J338" s="143" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="136" t="n">
+      <c r="K338" s="143" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="136" t="n">
+      <c r="L338" s="143" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="136" t="n">
+      <c r="M338" s="143" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="136" t="n">
+      <c r="N338" s="143" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20842,40 +20876,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="136" t="n">
+      <c r="C339" s="143" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="136" t="n">
+      <c r="D339" s="143" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="136" t="n">
+      <c r="E339" s="143" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="136" t="n">
+      <c r="F339" s="143" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="136" t="n">
+      <c r="G339" s="143" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="136" t="n">
+      <c r="H339" s="143" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="136" t="n">
+      <c r="I339" s="143" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="136" t="n">
+      <c r="J339" s="143" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="136" t="n">
+      <c r="K339" s="143" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="136" t="n">
+      <c r="L339" s="143" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="136" t="n">
+      <c r="M339" s="143" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="136" t="n">
+      <c r="N339" s="143" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -20886,40 +20920,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="136" t="n">
+      <c r="C340" s="143" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="136" t="n">
+      <c r="D340" s="143" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="136" t="n">
+      <c r="E340" s="143" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="136" t="n">
+      <c r="F340" s="143" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="136" t="n">
+      <c r="G340" s="143" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="136" t="n">
+      <c r="H340" s="143" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="136" t="n">
+      <c r="I340" s="143" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="136" t="n">
+      <c r="J340" s="143" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="136" t="n">
+      <c r="K340" s="143" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="136" t="n">
+      <c r="L340" s="143" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="136" t="n">
+      <c r="M340" s="143" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="136" t="n">
+      <c r="N340" s="143" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21634,40 +21668,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="136" t="n">
+      <c r="C357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="136" t="n">
+      <c r="D357" s="143" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="136" t="n">
+      <c r="E357" s="143" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="136" t="n">
+      <c r="F357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="136" t="n">
+      <c r="G357" s="143" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="136" t="n">
+      <c r="H357" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="136" t="n">
+      <c r="I357" s="143" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="136" t="n">
+      <c r="J357" s="143" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="136" t="n">
+      <c r="K357" s="143" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="136" t="n">
+      <c r="L357" s="143" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="136" t="n">
+      <c r="M357" s="143" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="136" t="n">
+      <c r="N357" s="143" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21678,40 +21712,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="136" t="n">
+      <c r="C358" s="143" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="136" t="n">
+      <c r="D358" s="143" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="136" t="n">
+      <c r="E358" s="143" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="136" t="n">
+      <c r="F358" s="143" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="136" t="n">
+      <c r="G358" s="143" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="136" t="n">
+      <c r="H358" s="143" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="136" t="n">
+      <c r="I358" s="143" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="136" t="n">
+      <c r="J358" s="143" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="136" t="n">
+      <c r="K358" s="143" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="136" t="n">
+      <c r="L358" s="143" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="136" t="n">
+      <c r="M358" s="143" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="136" t="n">
+      <c r="N358" s="143" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21722,40 +21756,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="136" t="n">
+      <c r="C359" s="143" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="136" t="n">
+      <c r="D359" s="143" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="136" t="n">
+      <c r="E359" s="143" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="136" t="n">
+      <c r="F359" s="143" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="136" t="n">
+      <c r="G359" s="143" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="136" t="n">
+      <c r="H359" s="143" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="136" t="n">
+      <c r="I359" s="143" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="136" t="n">
+      <c r="J359" s="143" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="136" t="n">
+      <c r="K359" s="143" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="136" t="n">
+      <c r="L359" s="143" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="136" t="n">
+      <c r="M359" s="143" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="136" t="n">
+      <c r="N359" s="143" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21766,40 +21800,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="136" t="n">
+      <c r="C360" s="143" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="136" t="n">
+      <c r="D360" s="143" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="136" t="n">
+      <c r="E360" s="143" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="136" t="n">
+      <c r="F360" s="143" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="136" t="n">
+      <c r="G360" s="143" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="136" t="n">
+      <c r="H360" s="143" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="136" t="n">
+      <c r="I360" s="143" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="136" t="n">
+      <c r="J360" s="143" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="136" t="n">
+      <c r="K360" s="143" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="136" t="n">
+      <c r="L360" s="143" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="136" t="n">
+      <c r="M360" s="143" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="136" t="n">
+      <c r="N360" s="143" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -21942,7 +21976,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="136" t="n">
+      <c r="C364" s="143" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -21986,7 +22020,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="136" t="n">
+      <c r="C365" s="143" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -22030,7 +22064,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="136" t="n">
+      <c r="C366" s="143" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22074,7 +22108,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="136" t="n">
+      <c r="C367" s="143" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23851,13 +23885,13 @@
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="137" t="s">
+      <c r="B1" s="144" t="s">
         <v>813</v>
       </c>
-      <c r="C1" s="137" t="n">
+      <c r="C1" s="144" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="137" t="s">
+      <c r="D1" s="144" t="s">
         <v>814</v>
       </c>
     </row>
@@ -23865,10 +23899,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="137" t="s">
+      <c r="B2" s="144" t="s">
         <v>815</v>
       </c>
-      <c r="C2" s="137" t="n">
+      <c r="C2" s="144" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -23876,10 +23910,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="137" t="s">
+      <c r="B3" s="144" t="s">
         <v>816</v>
       </c>
-      <c r="C3" s="137" t="n">
+      <c r="C3" s="144" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -23983,7 +24017,7 @@
       <c r="B16" s="0" t="s">
         <v>831</v>
       </c>
-      <c r="C16" s="136" t="n">
+      <c r="C16" s="143" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -23991,7 +24025,7 @@
       <c r="B17" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C17" s="136" t="n">
+      <c r="C17" s="143" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -23999,7 +24033,7 @@
       <c r="B18" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C18" s="136" t="n">
+      <c r="C18" s="143" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -24007,7 +24041,7 @@
       <c r="B19" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="C19" s="136" t="n">
+      <c r="C19" s="143" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24495,7 +24529,7 @@
       <c r="B80" s="0" t="s">
         <v>902</v>
       </c>
-      <c r="C80" s="136" t="n">
+      <c r="C80" s="143" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24543,7 +24577,7 @@
       <c r="B86" s="0" t="s">
         <v>908</v>
       </c>
-      <c r="C86" s="136" t="n">
+      <c r="C86" s="143" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24575,7 +24609,7 @@
       <c r="B90" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="C90" s="136" t="n">
+      <c r="C90" s="143" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24663,7 +24697,7 @@
       <c r="B101" s="0" t="s">
         <v>924</v>
       </c>
-      <c r="C101" s="136" t="n">
+      <c r="C101" s="143" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24839,7 +24873,7 @@
       <c r="B123" s="0" t="s">
         <v>948</v>
       </c>
-      <c r="C123" s="136" t="n">
+      <c r="C123" s="143" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -24903,7 +24937,7 @@
       <c r="B131" s="0" t="s">
         <v>956</v>
       </c>
-      <c r="C131" s="136" t="n">
+      <c r="C131" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -24919,7 +24953,7 @@
       <c r="B133" s="0" t="s">
         <v>958</v>
       </c>
-      <c r="C133" s="136" t="n">
+      <c r="C133" s="143" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25439,7 +25473,7 @@
       <c r="B198" s="0" t="s">
         <v>1025</v>
       </c>
-      <c r="C198" s="136" t="n">
+      <c r="C198" s="143" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25487,7 +25521,7 @@
       <c r="B204" s="0" t="s">
         <v>1031</v>
       </c>
-      <c r="C204" s="136" t="n">
+      <c r="C204" s="143" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25519,7 +25553,7 @@
       <c r="B208" s="0" t="s">
         <v>1035</v>
       </c>
-      <c r="C208" s="136" t="n">
+      <c r="C208" s="143" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25607,7 +25641,7 @@
       <c r="B219" s="0" t="s">
         <v>1046</v>
       </c>
-      <c r="C219" s="136" t="n">
+      <c r="C219" s="143" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25783,7 +25817,7 @@
       <c r="B241" s="0" t="s">
         <v>1069</v>
       </c>
-      <c r="C241" s="136" t="n">
+      <c r="C241" s="143" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25847,7 +25881,7 @@
       <c r="B249" s="0" t="s">
         <v>1077</v>
       </c>
-      <c r="C249" s="136" t="n">
+      <c r="C249" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25863,7 +25897,7 @@
       <c r="B251" s="0" t="s">
         <v>1079</v>
       </c>
-      <c r="C251" s="136" t="n">
+      <c r="C251" s="143" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26383,7 +26417,7 @@
       <c r="B316" s="0" t="s">
         <v>1144</v>
       </c>
-      <c r="C316" s="136" t="n">
+      <c r="C316" s="143" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26431,7 +26465,7 @@
       <c r="B322" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="C322" s="136" t="n">
+      <c r="C322" s="143" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26463,7 +26497,7 @@
       <c r="B326" s="0" t="s">
         <v>1154</v>
       </c>
-      <c r="C326" s="136" t="n">
+      <c r="C326" s="143" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26551,7 +26585,7 @@
       <c r="B337" s="0" t="s">
         <v>1165</v>
       </c>
-      <c r="C337" s="136" t="n">
+      <c r="C337" s="143" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26727,7 +26761,7 @@
       <c r="B359" s="0" t="s">
         <v>1188</v>
       </c>
-      <c r="C359" s="136" t="n">
+      <c r="C359" s="143" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26791,7 +26825,7 @@
       <c r="B367" s="0" t="s">
         <v>1196</v>
       </c>
-      <c r="C367" s="136" t="n">
+      <c r="C367" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26807,7 +26841,7 @@
       <c r="B369" s="0" t="s">
         <v>1198</v>
       </c>
-      <c r="C369" s="136" t="n">
+      <c r="C369" s="143" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27327,7 +27361,7 @@
       <c r="B434" s="0" t="s">
         <v>1263</v>
       </c>
-      <c r="C434" s="136" t="n">
+      <c r="C434" s="143" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27375,7 +27409,7 @@
       <c r="B440" s="0" t="s">
         <v>1269</v>
       </c>
-      <c r="C440" s="136" t="n">
+      <c r="C440" s="143" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27407,7 +27441,7 @@
       <c r="B444" s="0" t="s">
         <v>1273</v>
       </c>
-      <c r="C444" s="136" t="n">
+      <c r="C444" s="143" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27495,7 +27529,7 @@
       <c r="B455" s="0" t="s">
         <v>1284</v>
       </c>
-      <c r="C455" s="136" t="n">
+      <c r="C455" s="143" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27671,7 +27705,7 @@
       <c r="B477" s="0" t="s">
         <v>1307</v>
       </c>
-      <c r="C477" s="136" t="n">
+      <c r="C477" s="143" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27735,7 +27769,7 @@
       <c r="B485" s="0" t="s">
         <v>1315</v>
       </c>
-      <c r="C485" s="136" t="n">
+      <c r="C485" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27751,7 +27785,7 @@
       <c r="B487" s="0" t="s">
         <v>1317</v>
       </c>
-      <c r="C487" s="136" t="n">
+      <c r="C487" s="143" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27839,7 +27873,7 @@
       <c r="B498" s="0" t="s">
         <v>1328</v>
       </c>
-      <c r="C498" s="136" t="n">
+      <c r="C498" s="143" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27847,7 +27881,7 @@
       <c r="B499" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C499" s="136" t="n">
+      <c r="C499" s="143" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27855,7 +27889,7 @@
       <c r="B500" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C500" s="136" t="n">
+      <c r="C500" s="143" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27863,7 +27897,7 @@
       <c r="B501" s="0" t="s">
         <v>1331</v>
       </c>
-      <c r="C501" s="136" t="n">
+      <c r="C501" s="143" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28431,7 +28465,7 @@
       <c r="B572" s="0" t="s">
         <v>1402</v>
       </c>
-      <c r="C572" s="136" t="n">
+      <c r="C572" s="143" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28479,7 +28513,7 @@
       <c r="B578" s="0" t="s">
         <v>1408</v>
       </c>
-      <c r="C578" s="136" t="n">
+      <c r="C578" s="143" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28511,7 +28545,7 @@
       <c r="B582" s="0" t="s">
         <v>1412</v>
       </c>
-      <c r="C582" s="136" t="n">
+      <c r="C582" s="143" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28599,7 +28633,7 @@
       <c r="B593" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="C593" s="136" t="n">
+      <c r="C593" s="143" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28775,7 +28809,7 @@
       <c r="B615" s="0" t="s">
         <v>1446</v>
       </c>
-      <c r="C615" s="136" t="n">
+      <c r="C615" s="143" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28839,7 +28873,7 @@
       <c r="B623" s="0" t="s">
         <v>1454</v>
       </c>
-      <c r="C623" s="136" t="n">
+      <c r="C623" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28855,7 +28889,7 @@
       <c r="B625" s="0" t="s">
         <v>1456</v>
       </c>
-      <c r="C625" s="136" t="n">
+      <c r="C625" s="143" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29375,7 +29409,7 @@
       <c r="B690" s="0" t="s">
         <v>1521</v>
       </c>
-      <c r="C690" s="136" t="n">
+      <c r="C690" s="143" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29423,7 +29457,7 @@
       <c r="B696" s="0" t="s">
         <v>1527</v>
       </c>
-      <c r="C696" s="136" t="n">
+      <c r="C696" s="143" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29455,7 +29489,7 @@
       <c r="B700" s="0" t="s">
         <v>1531</v>
       </c>
-      <c r="C700" s="136" t="n">
+      <c r="C700" s="143" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29543,7 +29577,7 @@
       <c r="B711" s="0" t="s">
         <v>1542</v>
       </c>
-      <c r="C711" s="136" t="n">
+      <c r="C711" s="143" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29719,7 +29753,7 @@
       <c r="B733" s="0" t="s">
         <v>1565</v>
       </c>
-      <c r="C733" s="136" t="n">
+      <c r="C733" s="143" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29783,7 +29817,7 @@
       <c r="B741" s="0" t="s">
         <v>1573</v>
       </c>
-      <c r="C741" s="136" t="n">
+      <c r="C741" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29799,7 +29833,7 @@
       <c r="B743" s="0" t="s">
         <v>1575</v>
       </c>
-      <c r="C743" s="136" t="n">
+      <c r="C743" s="143" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30355,7 +30389,7 @@
       <c r="B811" s="0" t="s">
         <v>1651</v>
       </c>
-      <c r="C811" s="136" t="n">
+      <c r="C811" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30871,7 +30905,7 @@
       <c r="B874" s="0" t="s">
         <v>1716</v>
       </c>
-      <c r="C874" s="136" t="n">
+      <c r="C874" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31387,7 +31421,7 @@
       <c r="B937" s="0" t="s">
         <v>1781</v>
       </c>
-      <c r="C937" s="136" t="n">
+      <c r="C937" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31903,7 +31937,7 @@
       <c r="B1000" s="0" t="s">
         <v>1846</v>
       </c>
-      <c r="C1000" s="136" t="n">
+      <c r="C1000" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32419,7 +32453,7 @@
       <c r="B1063" s="0" t="s">
         <v>1911</v>
       </c>
-      <c r="C1063" s="136" t="n">
+      <c r="C1063" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32935,7 +32969,7 @@
       <c r="B1126" s="0" t="s">
         <v>1976</v>
       </c>
-      <c r="C1126" s="136" t="n">
+      <c r="C1126" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33451,7 +33485,7 @@
       <c r="B1189" s="0" t="s">
         <v>2041</v>
       </c>
-      <c r="C1189" s="136" t="n">
+      <c r="C1189" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33967,7 +34001,7 @@
       <c r="B1252" s="0" t="s">
         <v>2106</v>
       </c>
-      <c r="C1252" s="136" t="n">
+      <c r="C1252" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34483,7 +34517,7 @@
       <c r="B1315" s="0" t="s">
         <v>2171</v>
       </c>
-      <c r="C1315" s="136" t="n">
+      <c r="C1315" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34999,7 +35033,7 @@
       <c r="B1378" s="0" t="s">
         <v>2236</v>
       </c>
-      <c r="C1378" s="136" t="n">
+      <c r="C1378" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35515,7 +35549,7 @@
       <c r="B1441" s="0" t="s">
         <v>2301</v>
       </c>
-      <c r="C1441" s="136" t="n">
+      <c r="C1441" s="143" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35963,7 +35997,7 @@
       <c r="B1497" s="0" t="s">
         <v>2360</v>
       </c>
-      <c r="C1497" s="136" t="n">
+      <c r="C1497" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36589,7 +36623,7 @@
       <c r="B1576" s="0" t="s">
         <v>2444</v>
       </c>
-      <c r="C1576" s="136" t="n">
+      <c r="C1576" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36758,7 +36792,7 @@
       <c r="B1596" s="0" t="s">
         <v>2466</v>
       </c>
-      <c r="C1596" s="136" t="n">
+      <c r="C1596" s="143" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36766,7 +36800,7 @@
       <c r="B1597" s="0" t="s">
         <v>2467</v>
       </c>
-      <c r="C1597" s="136" t="n">
+      <c r="C1597" s="143" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37646,7 +37680,7 @@
       <c r="B1707" s="0" t="s">
         <v>2578</v>
       </c>
-      <c r="C1707" s="136" t="n">
+      <c r="C1707" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37662,7 +37696,7 @@
       <c r="B1709" s="0" t="s">
         <v>2580</v>
       </c>
-      <c r="C1709" s="136" t="n">
+      <c r="C1709" s="143" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38182,7 +38216,7 @@
       <c r="B1774" s="0" t="s">
         <v>2645</v>
       </c>
-      <c r="C1774" s="136" t="n">
+      <c r="C1774" s="143" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38262,7 +38296,7 @@
       <c r="B1784" s="0" t="s">
         <v>2655</v>
       </c>
-      <c r="C1784" s="136" t="n">
+      <c r="C1784" s="143" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38350,7 +38384,7 @@
       <c r="B1795" s="0" t="s">
         <v>2666</v>
       </c>
-      <c r="C1795" s="136" t="n">
+      <c r="C1795" s="143" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38526,7 +38560,7 @@
       <c r="B1817" s="0" t="s">
         <v>2689</v>
       </c>
-      <c r="C1817" s="136" t="n">
+      <c r="C1817" s="143" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38590,7 +38624,7 @@
       <c r="B1825" s="0" t="s">
         <v>2697</v>
       </c>
-      <c r="C1825" s="136" t="n">
+      <c r="C1825" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38606,7 +38640,7 @@
       <c r="B1827" s="0" t="s">
         <v>2699</v>
       </c>
-      <c r="C1827" s="136" t="n">
+      <c r="C1827" s="143" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39209,7 +39243,7 @@
       <c r="B1902" s="0" t="s">
         <v>2776</v>
       </c>
-      <c r="C1902" s="136" t="n">
+      <c r="C1902" s="143" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39257,7 +39291,7 @@
       <c r="B1908" s="0" t="s">
         <v>2782</v>
       </c>
-      <c r="C1908" s="136" t="n">
+      <c r="C1908" s="143" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39289,7 +39323,7 @@
       <c r="B1912" s="0" t="s">
         <v>2786</v>
       </c>
-      <c r="C1912" s="136" t="n">
+      <c r="C1912" s="143" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39377,7 +39411,7 @@
       <c r="B1923" s="0" t="s">
         <v>2797</v>
       </c>
-      <c r="C1923" s="136" t="n">
+      <c r="C1923" s="143" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39553,7 +39587,7 @@
       <c r="B1945" s="0" t="s">
         <v>2820</v>
       </c>
-      <c r="C1945" s="136" t="n">
+      <c r="C1945" s="143" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39617,7 +39651,7 @@
       <c r="B1953" s="0" t="s">
         <v>2828</v>
       </c>
-      <c r="C1953" s="136" t="n">
+      <c r="C1953" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39633,7 +39667,7 @@
       <c r="B1955" s="0" t="s">
         <v>2830</v>
       </c>
-      <c r="C1955" s="136" t="n">
+      <c r="C1955" s="143" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40153,7 +40187,7 @@
       <c r="B2020" s="0" t="s">
         <v>2895</v>
       </c>
-      <c r="C2020" s="136" t="n">
+      <c r="C2020" s="143" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40201,7 +40235,7 @@
       <c r="B2026" s="0" t="s">
         <v>2901</v>
       </c>
-      <c r="C2026" s="136" t="n">
+      <c r="C2026" s="143" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40233,7 +40267,7 @@
       <c r="B2030" s="0" t="s">
         <v>2905</v>
       </c>
-      <c r="C2030" s="136" t="n">
+      <c r="C2030" s="143" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40321,7 +40355,7 @@
       <c r="B2041" s="0" t="s">
         <v>2916</v>
       </c>
-      <c r="C2041" s="136" t="n">
+      <c r="C2041" s="143" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40497,7 +40531,7 @@
       <c r="B2063" s="0" t="s">
         <v>2939</v>
       </c>
-      <c r="C2063" s="136" t="n">
+      <c r="C2063" s="143" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40561,7 +40595,7 @@
       <c r="B2071" s="0" t="s">
         <v>2947</v>
       </c>
-      <c r="C2071" s="136" t="n">
+      <c r="C2071" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40577,7 +40611,7 @@
       <c r="B2073" s="0" t="s">
         <v>2949</v>
       </c>
-      <c r="C2073" s="136" t="n">
+      <c r="C2073" s="143" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41097,7 +41131,7 @@
       <c r="B2138" s="0" t="s">
         <v>3014</v>
       </c>
-      <c r="C2138" s="136" t="n">
+      <c r="C2138" s="143" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41145,7 +41179,7 @@
       <c r="B2144" s="0" t="s">
         <v>3020</v>
       </c>
-      <c r="C2144" s="136" t="n">
+      <c r="C2144" s="143" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41177,7 +41211,7 @@
       <c r="B2148" s="0" t="s">
         <v>3024</v>
       </c>
-      <c r="C2148" s="136" t="n">
+      <c r="C2148" s="143" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41265,7 +41299,7 @@
       <c r="B2159" s="0" t="s">
         <v>3035</v>
       </c>
-      <c r="C2159" s="136" t="n">
+      <c r="C2159" s="143" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41441,7 +41475,7 @@
       <c r="B2181" s="0" t="s">
         <v>3058</v>
       </c>
-      <c r="C2181" s="136" t="n">
+      <c r="C2181" s="143" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41505,7 +41539,7 @@
       <c r="B2189" s="0" t="s">
         <v>3066</v>
       </c>
-      <c r="C2189" s="136" t="n">
+      <c r="C2189" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41521,7 +41555,7 @@
       <c r="B2191" s="0" t="s">
         <v>3068</v>
       </c>
-      <c r="C2191" s="136" t="n">
+      <c r="C2191" s="143" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42097,7 +42131,7 @@
       <c r="B2263" s="0" t="s">
         <v>3143</v>
       </c>
-      <c r="C2263" s="136" t="n">
+      <c r="C2263" s="143" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42384,7 +42418,7 @@
       <c r="F2297" s="0" t="s">
         <v>3188</v>
       </c>
-      <c r="G2297" s="138" t="n">
+      <c r="G2297" s="145" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42476,7 +42510,7 @@
       <c r="B2307" s="0" t="s">
         <v>3202</v>
       </c>
-      <c r="C2307" s="136" t="n">
+      <c r="C2307" s="143" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42562,7 +42596,7 @@
       <c r="B2317" s="0" t="s">
         <v>3218</v>
       </c>
-      <c r="C2317" s="136" t="n">
+      <c r="C2317" s="143" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42570,7 +42604,7 @@
       <c r="B2318" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="C2318" s="136" t="n">
+      <c r="C2318" s="143" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42586,7 +42620,7 @@
       <c r="B2320" s="0" t="s">
         <v>3221</v>
       </c>
-      <c r="C2320" s="136" t="n">
+      <c r="C2320" s="143" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42634,7 +42668,7 @@
       <c r="C2326" s="0" t="s">
         <v>3229</v>
       </c>
-      <c r="D2326" s="139" t="n">
+      <c r="D2326" s="146" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42685,7 +42719,7 @@
       <c r="C2332" s="0" t="s">
         <v>3237</v>
       </c>
-      <c r="D2332" s="139" t="n">
+      <c r="D2332" s="146" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42704,7 +42738,7 @@
       <c r="D2334" s="0" t="s">
         <v>3240</v>
       </c>
-      <c r="E2334" s="139" t="n">
+      <c r="E2334" s="146" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42762,7 +42796,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="139" t="n">
+      <c r="F2339" s="146" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43234,7 +43268,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="139" t="n">
+      <c r="F2380" s="146" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add reports from IP management tool
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="247" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="247" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Modes A-F" sheetId="1" state="visible" r:id="rId2"/>
@@ -11694,7 +11694,7 @@
   </sheetPr>
   <dimension ref="1:66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="N32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
@@ -15464,8 +15464,8 @@
   </sheetPr>
   <dimension ref="1:31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16915,7 +16915,7 @@
         <v>251</v>
       </c>
       <c r="I26" s="90" t="n">
-        <v>3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix xafs_table in Modes.xlsx
update cadashboard and camove
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -10643,14 +10643,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00E+000"/>
-    <numFmt numFmtId="169" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="170" formatCode="HH:MM:SS"/>
+    <numFmt numFmtId="168" formatCode="General"/>
+    <numFmt numFmtId="169" formatCode="0.00E+000"/>
+    <numFmt numFmtId="170" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="171" formatCode="HH:MM:SS"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -10781,7 +10782,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -10803,7 +10804,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFF99"/>
+        <bgColor rgb="FFFFFFD7"/>
       </patternFill>
     </fill>
     <fill>
@@ -10814,7 +10815,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
@@ -11107,7 +11114,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -11348,15 +11355,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11364,11 +11375,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11376,7 +11387,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11384,11 +11395,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11444,7 +11455,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11492,7 +11503,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="7" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="26" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11604,7 +11615,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11680,19 +11691,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -11708,7 +11719,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFCCFF"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFFF3333"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000CC"/>
@@ -11726,7 +11737,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFCCFF"/>
       <rgbColor rgb="FF330066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -11744,7 +11755,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF9999"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF2DED5"/>
       <rgbColor rgb="FF3366FF"/>
@@ -11776,14 +11787,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="N29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
-      <selection pane="bottomRight" activeCell="U54" activeCellId="0" sqref="U54"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
+      <selection pane="bottomRight" activeCell="F58" activeCellId="0" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -11799,10 +11810,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="15.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="13.82"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="17.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="22" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14744,35 +14753,35 @@
         <v>181</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>29.305</v>
+        <v>30.904</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>257236</v>
+        <v>270207</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="57" t="n">
-        <v>-22.453</v>
+        <v>-22.857</v>
       </c>
       <c r="J54" s="28" t="n">
-        <v>-260370</v>
-      </c>
-      <c r="K54" s="57" t="n">
-        <v>42.826</v>
+        <v>-264424</v>
+      </c>
+      <c r="K54" s="60" t="n">
+        <v>43.326</v>
       </c>
       <c r="L54" s="28" t="n">
         <v>393955</v>
       </c>
       <c r="M54" s="57" t="n">
-        <v>43.157</v>
+        <v>43.654</v>
       </c>
       <c r="N54" s="28" t="n">
-        <v>395728</v>
+        <v>400720</v>
       </c>
       <c r="O54" s="57" t="n">
-        <v>16.941</v>
+        <v>17.5398</v>
       </c>
       <c r="P54" s="28" t="n">
         <v>133595</v>
@@ -14815,40 +14824,40 @@
         <v>184</v>
       </c>
       <c r="E55" s="37" t="n">
-        <v>-3.3653</v>
+        <v>5.5112</v>
       </c>
       <c r="F55" s="35" t="n">
-        <v>-3</v>
-      </c>
-      <c r="G55" s="38" t="n">
-        <v>-3.3653</v>
-      </c>
-      <c r="H55" s="45" t="n">
-        <v>-3</v>
+        <v>88762</v>
+      </c>
+      <c r="G55" s="37" t="n">
+        <v>5.5112</v>
+      </c>
+      <c r="H55" s="35" t="n">
+        <v>88762</v>
       </c>
       <c r="I55" s="37" t="n">
-        <v>-3.3653</v>
+        <v>5.5112</v>
       </c>
       <c r="J55" s="35" t="n">
-        <v>-3</v>
-      </c>
-      <c r="K55" s="38" t="n">
-        <v>-3.3635</v>
-      </c>
-      <c r="L55" s="45" t="n">
-        <v>15</v>
+        <v>88762</v>
+      </c>
+      <c r="K55" s="37" t="n">
+        <v>5.5112</v>
+      </c>
+      <c r="L55" s="35" t="n">
+        <v>88762</v>
       </c>
       <c r="M55" s="37" t="n">
-        <v>-3.3635</v>
+        <v>5.5112</v>
       </c>
       <c r="N55" s="35" t="n">
-        <v>15</v>
-      </c>
-      <c r="O55" s="38" t="n">
-        <v>-3.3648</v>
-      </c>
-      <c r="P55" s="45" t="n">
-        <v>2</v>
+        <v>88762</v>
+      </c>
+      <c r="O55" s="37" t="n">
+        <v>5.5112</v>
+      </c>
+      <c r="P55" s="35" t="n">
+        <v>88762</v>
       </c>
       <c r="Q55" s="26"/>
       <c r="R55" s="26"/>
@@ -14892,41 +14901,41 @@
       <c r="D56" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E56" s="60" t="n">
-        <v>113.122</v>
+      <c r="E56" s="61" t="n">
+        <v>117.737</v>
       </c>
       <c r="F56" s="25" t="n">
-        <v>9216103</v>
-      </c>
-      <c r="G56" s="61" t="n">
+        <v>9456218</v>
+      </c>
+      <c r="G56" s="62" t="n">
         <v>24.4104</v>
       </c>
-      <c r="H56" s="62" t="n">
+      <c r="H56" s="63" t="n">
         <v>4600216</v>
       </c>
-      <c r="I56" s="60" t="n">
-        <v>56.616</v>
+      <c r="I56" s="61" t="n">
+        <v>59.419</v>
       </c>
       <c r="J56" s="23" t="n">
-        <v>6275942</v>
-      </c>
-      <c r="K56" s="60" t="n">
-        <v>126.022</v>
+        <v>6421815</v>
+      </c>
+      <c r="K56" s="61" t="n">
+        <v>127.717</v>
       </c>
       <c r="L56" s="23" t="n">
-        <v>9887325</v>
-      </c>
-      <c r="M56" s="60" t="n">
-        <v>126.022</v>
+        <v>9975528</v>
+      </c>
+      <c r="M56" s="61" t="n">
+        <v>129.275</v>
       </c>
       <c r="N56" s="23" t="n">
-        <v>9887325</v>
-      </c>
-      <c r="O56" s="60" t="n">
-        <v>98.461</v>
+        <v>10056598</v>
+      </c>
+      <c r="O56" s="61" t="n">
+        <v>101.258</v>
       </c>
       <c r="P56" s="23" t="n">
-        <v>8453249</v>
+        <v>8598781</v>
       </c>
       <c r="Q56" s="26"/>
       <c r="R56" s="26"/>
@@ -14954,41 +14963,41 @@
       <c r="D57" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="E57" s="63" t="n">
-        <v>110.088</v>
+      <c r="E57" s="64" t="n">
+        <v>117.793</v>
       </c>
       <c r="F57" s="32" t="n">
-        <v>6612707</v>
-      </c>
-      <c r="G57" s="64" t="n">
+        <v>7013607</v>
+      </c>
+      <c r="G57" s="65" t="n">
         <v>12.81</v>
       </c>
-      <c r="H57" s="65" t="n">
+      <c r="H57" s="66" t="n">
         <v>1551088</v>
       </c>
-      <c r="I57" s="63" t="n">
-        <v>46.772</v>
+      <c r="I57" s="64" t="n">
+        <v>51.275</v>
       </c>
       <c r="J57" s="32" t="n">
-        <v>3318211</v>
-      </c>
-      <c r="K57" s="63" t="n">
-        <v>123.378</v>
+        <v>3552538</v>
+      </c>
+      <c r="K57" s="64" t="n">
+        <v>127.673</v>
       </c>
       <c r="L57" s="32" t="n">
-        <v>7304221</v>
-      </c>
-      <c r="M57" s="63" t="n">
-        <v>123.378</v>
+        <v>7527711</v>
+      </c>
+      <c r="M57" s="64" t="n">
+        <v>130.031</v>
       </c>
       <c r="N57" s="32" t="n">
-        <v>7304221</v>
-      </c>
-      <c r="O57" s="63" t="n">
-        <v>92.517</v>
+        <v>7650409</v>
+      </c>
+      <c r="O57" s="64" t="n">
+        <v>98.114</v>
       </c>
       <c r="P57" s="32" t="n">
-        <v>5698439</v>
+        <v>5989663</v>
       </c>
       <c r="T57" s="30" t="n">
         <v>138.4</v>
@@ -15008,41 +15017,41 @@
       <c r="D58" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="E58" s="63" t="n">
-        <v>110.088</v>
+      <c r="E58" s="64" t="n">
+        <v>117.793</v>
       </c>
       <c r="F58" s="28" t="n">
-        <v>5415959</v>
-      </c>
-      <c r="G58" s="64" t="n">
+        <v>5816859</v>
+      </c>
+      <c r="G58" s="65" t="n">
         <v>12.81</v>
       </c>
-      <c r="H58" s="65" t="n">
+      <c r="H58" s="66" t="n">
         <v>354340</v>
       </c>
-      <c r="I58" s="63" t="n">
-        <v>46.772</v>
+      <c r="I58" s="64" t="n">
+        <v>51.275</v>
       </c>
       <c r="J58" s="32" t="n">
-        <v>2121463</v>
-      </c>
-      <c r="K58" s="63" t="n">
-        <v>123.378</v>
+        <v>2355790</v>
+      </c>
+      <c r="K58" s="64" t="n">
+        <v>127.673</v>
       </c>
       <c r="L58" s="32" t="n">
-        <v>6107473</v>
-      </c>
-      <c r="M58" s="63" t="n">
-        <v>123.378</v>
+        <v>6330963</v>
+      </c>
+      <c r="M58" s="64" t="n">
+        <v>130.031</v>
       </c>
       <c r="N58" s="32" t="n">
-        <v>6107473</v>
-      </c>
-      <c r="O58" s="63" t="n">
-        <v>92.517</v>
-      </c>
-      <c r="P58" s="66" t="n">
-        <v>4501691</v>
+        <v>6453661</v>
+      </c>
+      <c r="O58" s="64" t="n">
+        <v>98.114</v>
+      </c>
+      <c r="P58" s="67" t="n">
+        <v>4792915</v>
       </c>
       <c r="T58" s="27" t="n">
         <v>138.4</v>
@@ -15067,43 +15076,43 @@
       <c r="D59" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="E59" s="63" t="n">
-        <v>-0.6</v>
+      <c r="E59" s="64" t="n">
+        <v>-11.0621</v>
       </c>
       <c r="F59" s="28" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="G59" s="64" t="n">
-        <v>-0.6</v>
-      </c>
-      <c r="H59" s="67" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="I59" s="63" t="n">
-        <v>-0.6</v>
+        <v>-202758</v>
+      </c>
+      <c r="G59" s="65" t="n">
+        <v>-11.0621</v>
+      </c>
+      <c r="H59" s="68" t="n">
+        <v>-202758</v>
+      </c>
+      <c r="I59" s="64" t="n">
+        <v>-11.0621</v>
       </c>
       <c r="J59" s="28" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="K59" s="63" t="n">
-        <v>-0.6</v>
+        <v>-202758</v>
+      </c>
+      <c r="K59" s="64" t="n">
+        <v>-11.0621</v>
       </c>
       <c r="L59" s="28" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="M59" s="63" t="n">
-        <v>-0.6</v>
+        <v>-202758</v>
+      </c>
+      <c r="M59" s="64" t="n">
+        <v>-11.0621</v>
       </c>
       <c r="N59" s="28" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="O59" s="63" t="n">
-        <v>-0.6</v>
+        <v>-202758</v>
+      </c>
+      <c r="O59" s="64" t="n">
+        <v>-11.0621</v>
       </c>
       <c r="P59" s="28" t="n">
-        <v>-412000</v>
-      </c>
-      <c r="T59" s="63" t="n">
+        <v>-202758</v>
+      </c>
+      <c r="T59" s="64" t="n">
         <v>-0.6</v>
       </c>
       <c r="U59" s="28" t="n">
@@ -15121,46 +15130,46 @@
       <c r="D60" s="35" t="s">
         <v>200</v>
       </c>
-      <c r="E60" s="68" t="n">
-        <v>33.3721</v>
+      <c r="E60" s="69" t="n">
+        <v>16.38985</v>
       </c>
       <c r="F60" s="47" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="G60" s="69" t="n">
-        <v>33.3721</v>
-      </c>
-      <c r="H60" s="70" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="I60" s="68" t="n">
-        <v>33.3721</v>
+        <v>140203</v>
+      </c>
+      <c r="G60" s="70" t="n">
+        <v>16.38985</v>
+      </c>
+      <c r="H60" s="71" t="n">
+        <v>140203</v>
+      </c>
+      <c r="I60" s="69" t="n">
+        <v>16.38985</v>
       </c>
       <c r="J60" s="47" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="K60" s="68" t="n">
-        <v>33.3721</v>
+        <v>140203</v>
+      </c>
+      <c r="K60" s="69" t="n">
+        <v>16.38985</v>
       </c>
       <c r="L60" s="47" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="M60" s="68" t="n">
-        <v>33.3721</v>
+        <v>140203</v>
+      </c>
+      <c r="M60" s="69" t="n">
+        <v>16.38985</v>
       </c>
       <c r="N60" s="47" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="O60" s="68" t="n">
-        <v>33.3721</v>
+        <v>140203</v>
+      </c>
+      <c r="O60" s="69" t="n">
+        <v>16.38985</v>
       </c>
       <c r="P60" s="47" t="n">
-        <v>-199443</v>
-      </c>
-      <c r="Q60" s="71"/>
-      <c r="R60" s="71"/>
-      <c r="S60" s="71"/>
-      <c r="T60" s="68" t="n">
+        <v>140203</v>
+      </c>
+      <c r="Q60" s="72"/>
+      <c r="R60" s="72"/>
+      <c r="S60" s="72"/>
+      <c r="T60" s="69" t="n">
         <v>33.3721</v>
       </c>
       <c r="U60" s="47" t="n">
@@ -15173,52 +15182,52 @@
       <c r="Z60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="72" t="s">
+      <c r="A61" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="73" t="s">
+      <c r="B61" s="74" t="s">
         <v>202</v>
       </c>
-      <c r="C61" s="74" t="s">
+      <c r="C61" s="75" t="s">
         <v>203</v>
       </c>
-      <c r="D61" s="74" t="s">
+      <c r="D61" s="75" t="s">
         <v>204</v>
       </c>
-      <c r="E61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="G61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="H61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="I61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="K61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="L61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="M61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="N61" s="76" t="n">
-        <v>0</v>
-      </c>
-      <c r="O61" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="P61" s="76" t="n">
+      <c r="E61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="F61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="J61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="L61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="N61" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="O61" s="76" t="n">
+        <v>0</v>
+      </c>
+      <c r="P61" s="77" t="n">
         <v>0</v>
       </c>
       <c r="T61" s="30" t="n">
@@ -15229,8 +15238,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="72"/>
-      <c r="B62" s="77" t="s">
+      <c r="A62" s="73"/>
+      <c r="B62" s="78" t="s">
         <v>205</v>
       </c>
       <c r="C62" s="0" t="s">
@@ -15283,8 +15292,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="72"/>
-      <c r="B63" s="77" t="s">
+      <c r="A63" s="73"/>
+      <c r="B63" s="78" t="s">
         <v>208</v>
       </c>
       <c r="C63" s="0" t="s">
@@ -15337,8 +15346,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="72"/>
-      <c r="B64" s="77" t="s">
+      <c r="A64" s="73"/>
+      <c r="B64" s="78" t="s">
         <v>211</v>
       </c>
       <c r="C64" s="0" t="s">
@@ -15391,8 +15400,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="72"/>
-      <c r="B65" s="77" t="s">
+      <c r="A65" s="73"/>
+      <c r="B65" s="78" t="s">
         <v>214</v>
       </c>
       <c r="C65" s="0" t="s">
@@ -15445,53 +15454,53 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="72"/>
-      <c r="B66" s="78" t="s">
+      <c r="A66" s="73"/>
+      <c r="B66" s="79" t="s">
         <v>217</v>
       </c>
-      <c r="C66" s="79" t="s">
+      <c r="C66" s="80" t="s">
         <v>218</v>
       </c>
-      <c r="D66" s="79" t="s">
+      <c r="D66" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="E66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="F66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="G66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="H66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="I66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="J66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="K66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="L66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="M66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="N66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="O66" s="80" t="n">
-        <v>0</v>
-      </c>
-      <c r="P66" s="81" t="n">
-        <v>0</v>
-      </c>
-      <c r="T66" s="68" t="n">
+      <c r="E66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="F66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="69" t="n">
         <v>0</v>
       </c>
       <c r="U66" s="47" t="n">
@@ -15545,40 +15554,40 @@
   </sheetPr>
   <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I27" activeCellId="0" sqref="I27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="82" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="82" width="13.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="82" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="83" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="2" style="83" width="13.26"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="83" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="82"/>
+    <row r="1" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="83"/>
       <c r="B1" s="0"/>
       <c r="C1" s="0"/>
       <c r="D1" s="0"/>
       <c r="E1" s="0"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="AMJ1" s="82"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="AMJ1" s="83"/>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
@@ -16599,168 +16608,168 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" s="89" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="85"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87" t="s">
+    <row r="3" s="90" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="86"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="88" t="s">
         <v>221</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D3" s="88" t="s">
         <v>222</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="89" t="s">
         <v>223</v>
       </c>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="85"/>
-      <c r="L3" s="85"/>
-      <c r="AMJ3" s="85"/>
-    </row>
-    <row r="4" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82"/>
-      <c r="B4" s="86" t="s">
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="AMJ3" s="86"/>
+    </row>
+    <row r="4" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="83"/>
+      <c r="B4" s="87" t="s">
         <v>224</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82" t="n">
+      <c r="C4" s="83"/>
+      <c r="D4" s="83" t="n">
         <v>55</v>
       </c>
-      <c r="E4" s="90" t="n">
+      <c r="E4" s="91" t="n">
         <v>55</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="82"/>
-      <c r="H4" s="82"/>
-      <c r="I4" s="82"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="82"/>
-      <c r="AMJ4" s="82"/>
-    </row>
-    <row r="5" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="82"/>
-      <c r="B5" s="86" t="s">
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
+      <c r="I4" s="83"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="83"/>
+      <c r="L4" s="83"/>
+      <c r="AMJ4" s="83"/>
+    </row>
+    <row r="5" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="83"/>
+      <c r="B5" s="87" t="s">
         <v>225</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="83" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="82" t="n">
+      <c r="D5" s="83" t="n">
         <v>-46.5</v>
       </c>
-      <c r="E5" s="90"/>
-      <c r="F5" s="82"/>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="AMJ5" s="82"/>
-    </row>
-    <row r="6" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="82"/>
-      <c r="B6" s="86" t="s">
+      <c r="E5" s="91"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="AMJ5" s="83"/>
+    </row>
+    <row r="6" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="83"/>
+      <c r="B6" s="87" t="s">
         <v>227</v>
       </c>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="83" t="s">
         <v>228</v>
       </c>
-      <c r="D6" s="82" t="n">
+      <c r="D6" s="83" t="n">
         <v>-20.5</v>
       </c>
-      <c r="E6" s="90"/>
-      <c r="F6" s="82"/>
-      <c r="G6" s="82"/>
-      <c r="H6" s="82"/>
-      <c r="I6" s="82"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="82"/>
-      <c r="AMJ6" s="82"/>
-    </row>
-    <row r="7" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="82"/>
-      <c r="B7" s="86" t="s">
+      <c r="E6" s="91"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
+      <c r="AMJ6" s="83"/>
+    </row>
+    <row r="7" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="83"/>
+      <c r="B7" s="87" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="83" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="82" t="n">
+      <c r="D7" s="83" t="n">
         <v>5.5</v>
       </c>
-      <c r="E7" s="90"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="AMJ7" s="82"/>
-    </row>
-    <row r="8" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="82"/>
-      <c r="B8" s="86" t="s">
+      <c r="E7" s="91"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="AMJ7" s="83"/>
+    </row>
+    <row r="8" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="83"/>
+      <c r="B8" s="87" t="s">
         <v>231</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="82" t="n">
+      <c r="D8" s="83" t="n">
         <v>31</v>
       </c>
-      <c r="E8" s="90"/>
-      <c r="F8" s="82"/>
-      <c r="G8" s="82"/>
-      <c r="H8" s="82"/>
-      <c r="I8" s="82"/>
-      <c r="J8" s="82"/>
-      <c r="K8" s="82"/>
-      <c r="L8" s="82"/>
-      <c r="AMJ8" s="82"/>
-    </row>
-    <row r="9" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="82"/>
-      <c r="B9" s="86" t="s">
+      <c r="E8" s="91"/>
+      <c r="F8" s="83"/>
+      <c r="G8" s="83"/>
+      <c r="H8" s="83"/>
+      <c r="I8" s="83"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="83"/>
+      <c r="L8" s="83"/>
+      <c r="AMJ8" s="83"/>
+    </row>
+    <row r="9" s="84" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="83"/>
+      <c r="B9" s="87" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82" t="n">
+      <c r="C9" s="83"/>
+      <c r="D9" s="83" t="n">
         <v>-52.6</v>
       </c>
-      <c r="E9" s="90"/>
-      <c r="F9" s="82"/>
-      <c r="G9" s="82"/>
-      <c r="H9" s="82"/>
-      <c r="I9" s="82"/>
-      <c r="J9" s="82"/>
-      <c r="K9" s="82"/>
-      <c r="L9" s="82"/>
-      <c r="AMJ9" s="82"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="AMJ9" s="83"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="92" t="s">
         <v>234</v>
       </c>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92" t="n">
+      <c r="C10" s="93"/>
+      <c r="D10" s="93" t="n">
         <v>-52</v>
       </c>
-      <c r="E10" s="93"/>
+      <c r="E10" s="94"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="94"/>
-      <c r="C11" s="95"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="96"/>
       <c r="D11" s="0"/>
       <c r="E11" s="0"/>
       <c r="F11" s="0"/>
@@ -16769,8 +16778,8 @@
       <c r="I11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="94"/>
-      <c r="C12" s="95"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="96"/>
       <c r="D12" s="0"/>
       <c r="E12" s="0"/>
       <c r="F12" s="0"/>
@@ -16779,82 +16788,82 @@
       <c r="I12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="97" t="s">
         <v>235</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="0"/>
       <c r="G13" s="0"/>
       <c r="H13" s="0"/>
       <c r="I13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="97" t="s">
+      <c r="B14" s="98" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="98" t="s">
+      <c r="C14" s="99" t="s">
         <v>237</v>
       </c>
       <c r="D14" s="0"/>
-      <c r="E14" s="90"/>
+      <c r="E14" s="91"/>
       <c r="F14" s="0"/>
       <c r="G14" s="0"/>
       <c r="H14" s="0"/>
       <c r="I14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="87" t="s">
         <v>224</v>
       </c>
-      <c r="C15" s="82" t="n">
+      <c r="C15" s="83" t="n">
         <v>67</v>
       </c>
       <c r="D15" s="0"/>
-      <c r="E15" s="90"/>
+      <c r="E15" s="91"/>
       <c r="F15" s="0"/>
       <c r="G15" s="0"/>
       <c r="H15" s="0"/>
       <c r="I15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="86" t="s">
+      <c r="B16" s="87" t="s">
         <v>238</v>
       </c>
-      <c r="C16" s="99" t="n">
+      <c r="C16" s="100" t="n">
         <v>-1.5</v>
       </c>
       <c r="D16" s="0"/>
-      <c r="E16" s="90"/>
+      <c r="E16" s="91"/>
       <c r="F16" s="0"/>
       <c r="G16" s="0"/>
       <c r="H16" s="0"/>
       <c r="I16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="87" t="s">
         <v>239</v>
       </c>
-      <c r="C17" s="82" t="n">
+      <c r="C17" s="83" t="n">
         <v>33</v>
       </c>
       <c r="D17" s="0"/>
-      <c r="E17" s="90"/>
+      <c r="E17" s="91"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
       <c r="I17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="92" t="s">
         <v>240</v>
       </c>
-      <c r="C18" s="92" t="n">
+      <c r="C18" s="93" t="n">
         <v>53</v>
       </c>
-      <c r="D18" s="92"/>
-      <c r="E18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
@@ -16881,213 +16890,213 @@
       <c r="I20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="96" t="s">
+      <c r="B21" s="97" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="96"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="96"/>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="96"/>
-      <c r="I21" s="96"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="97"/>
+      <c r="F21" s="97"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="101" t="s">
         <v>241</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="83"/>
-      <c r="E22" s="94" t="s">
+      <c r="C22" s="101"/>
+      <c r="D22" s="84"/>
+      <c r="E22" s="95" t="s">
         <v>242</v>
       </c>
-      <c r="F22" s="94"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="101" t="s">
+      <c r="F22" s="95"/>
+      <c r="G22" s="84"/>
+      <c r="H22" s="102" t="s">
         <v>243</v>
       </c>
-      <c r="I22" s="101"/>
+      <c r="I22" s="102"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="97" t="s">
+      <c r="B23" s="98" t="s">
         <v>244</v>
       </c>
-      <c r="C23" s="98" t="s">
+      <c r="C23" s="99" t="s">
         <v>237</v>
       </c>
       <c r="D23" s="0"/>
-      <c r="E23" s="83" t="s">
+      <c r="E23" s="84" t="s">
         <v>244</v>
       </c>
-      <c r="F23" s="98" t="s">
+      <c r="F23" s="99" t="s">
         <v>237</v>
       </c>
       <c r="G23" s="0"/>
-      <c r="H23" s="83" t="s">
+      <c r="H23" s="84" t="s">
         <v>245</v>
       </c>
-      <c r="I23" s="102" t="s">
+      <c r="I23" s="103" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="87" t="s">
         <v>246</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>33</v>
       </c>
       <c r="D24" s="0"/>
-      <c r="E24" s="82" t="s">
+      <c r="E24" s="83" t="s">
         <v>246</v>
       </c>
-      <c r="F24" s="103" t="n">
+      <c r="F24" s="104" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>29.305</v>
+        <v>30.904</v>
       </c>
       <c r="G24" s="0"/>
-      <c r="H24" s="82" t="s">
+      <c r="H24" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="I24" s="90" t="n">
+      <c r="I24" s="91" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="86" t="s">
+      <c r="B25" s="87" t="s">
         <v>248</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>-66.743</v>
       </c>
       <c r="D25" s="0"/>
-      <c r="E25" s="82" t="s">
+      <c r="E25" s="83" t="s">
         <v>248</v>
       </c>
-      <c r="F25" s="103" t="n">
+      <c r="F25" s="104" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
       <c r="G25" s="0"/>
-      <c r="H25" s="82" t="s">
+      <c r="H25" s="83" t="s">
         <v>249</v>
       </c>
-      <c r="I25" s="90" t="n">
+      <c r="I25" s="91" t="n">
         <v>-17.5</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="87" t="s">
         <v>250</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>-48.1824</v>
       </c>
       <c r="D26" s="0"/>
-      <c r="E26" s="82" t="s">
+      <c r="E26" s="83" t="s">
         <v>250</v>
       </c>
-      <c r="F26" s="103" t="n">
+      <c r="F26" s="104" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.453</v>
+        <v>-22.857</v>
       </c>
       <c r="G26" s="0"/>
-      <c r="H26" s="82" t="s">
+      <c r="H26" s="83" t="s">
         <v>251</v>
       </c>
-      <c r="I26" s="90" t="n">
+      <c r="I26" s="91" t="n">
         <v>6.5</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="86" t="s">
+      <c r="B27" s="87" t="s">
         <v>252</v>
       </c>
-      <c r="C27" s="82" t="n">
+      <c r="C27" s="83" t="n">
         <v>27.1</v>
       </c>
       <c r="D27" s="0"/>
-      <c r="E27" s="82" t="s">
+      <c r="E27" s="83" t="s">
         <v>252</v>
       </c>
-      <c r="F27" s="103" t="n">
+      <c r="F27" s="104" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>42.826</v>
+        <v>43.326</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
-      <c r="I27" s="90"/>
+      <c r="I27" s="91"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="86" t="s">
+      <c r="B28" s="87" t="s">
         <v>253</v>
       </c>
-      <c r="C28" s="82" t="n">
+      <c r="C28" s="83" t="n">
         <v>27.1</v>
       </c>
       <c r="D28" s="0"/>
-      <c r="E28" s="82" t="s">
+      <c r="E28" s="83" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="103" t="n">
+      <c r="F28" s="104" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.157</v>
+        <v>43.654</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
-      <c r="I28" s="90"/>
+      <c r="I28" s="91"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="86" t="s">
+      <c r="B29" s="87" t="s">
         <v>254</v>
       </c>
-      <c r="C29" s="82" t="n">
+      <c r="C29" s="83" t="n">
         <v>2.8</v>
       </c>
       <c r="D29" s="0"/>
-      <c r="E29" s="82" t="s">
+      <c r="E29" s="83" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="103" t="n">
+      <c r="F29" s="104" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>16.941</v>
+        <v>17.5398</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
-      <c r="I29" s="90"/>
+      <c r="I29" s="91"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="86" t="s">
+      <c r="B30" s="87" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="82" t="n">
+      <c r="C30" s="83" t="n">
         <v>15</v>
       </c>
       <c r="D30" s="0"/>
-      <c r="E30" s="82" t="s">
+      <c r="E30" s="83" t="s">
         <v>255</v>
       </c>
-      <c r="F30" s="103" t="n">
+      <c r="F30" s="104" t="n">
         <f aca="false">'Modes A-F'!T54</f>
         <v>53.33</v>
       </c>
       <c r="G30" s="0"/>
       <c r="H30" s="0"/>
-      <c r="I30" s="90"/>
+      <c r="I30" s="91"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="91" t="s">
+      <c r="B31" s="92" t="s">
         <v>247</v>
       </c>
-      <c r="C31" s="92" t="n">
+      <c r="C31" s="93" t="n">
         <v>55</v>
       </c>
-      <c r="D31" s="92"/>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="93"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="93"/>
+      <c r="G31" s="93"/>
+      <c r="H31" s="93"/>
+      <c r="I31" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17123,16 +17132,14 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.17"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17145,14 +17152,14 @@
       <c r="D1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="105" t="s">
         <v>256</v>
       </c>
-      <c r="F1" s="104"/>
-      <c r="G1" s="105" t="s">
+      <c r="F1" s="105"/>
+      <c r="G1" s="106" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="105"/>
+      <c r="H1" s="106"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="44" t="s">
@@ -17178,25 +17185,25 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="107" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="107" t="s">
+      <c r="C3" s="108" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="107" t="s">
+      <c r="D3" s="108" t="s">
         <v>258</v>
       </c>
-      <c r="E3" s="107" t="n">
+      <c r="E3" s="108" t="n">
         <v>8.77968</v>
       </c>
-      <c r="F3" s="107" t="n">
+      <c r="F3" s="108" t="n">
         <v>-2703</v>
       </c>
-      <c r="G3" s="108" t="n">
+      <c r="G3" s="109" t="n">
         <v>7.16226</v>
       </c>
-      <c r="H3" s="109" t="n">
+      <c r="H3" s="110" t="n">
         <v>-6620</v>
       </c>
     </row>
@@ -17259,11 +17266,11 @@
       <c r="G6" s="1" t="n">
         <v>15.99439325</v>
       </c>
-      <c r="I6" s="110" t="s">
+      <c r="I6" s="111" t="s">
         <v>261</v>
       </c>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="s">
@@ -17275,9 +17282,9 @@
       <c r="G7" s="1" t="n">
         <v>1.63763854</v>
       </c>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110"/>
-      <c r="K7" s="110"/>
+      <c r="I7" s="111"/>
+      <c r="J7" s="111"/>
+      <c r="K7" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17307,38 +17314,36 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112"/>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="113" t="s">
+      <c r="A1" s="112"/>
+      <c r="B1" s="113"/>
+      <c r="C1" s="113"/>
+      <c r="D1" s="113"/>
+      <c r="E1" s="114" t="s">
         <v>263</v>
       </c>
-      <c r="F1" s="113" t="s">
+      <c r="F1" s="114" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="115" t="s">
         <v>264</v>
       </c>
-      <c r="H1" s="115" t="s">
+      <c r="H1" s="116" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="116"/>
-      <c r="D2" s="117" t="s">
+      <c r="A2" s="117"/>
+      <c r="D2" s="118" t="s">
         <v>266</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -17347,514 +17352,514 @@
       <c r="F2" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="118"/>
+      <c r="G2" s="119"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="120" t="s">
         <v>267</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D3" s="117" t="s">
+      <c r="D3" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="120" t="n">
+      <c r="E3" s="121" t="n">
         <v>46.1092</v>
       </c>
-      <c r="F3" s="103" t="n">
+      <c r="F3" s="104" t="n">
         <f aca="false">E3-B3*TAN(2*(F2-E2)/1000)</f>
         <v>19.1031189817083</v>
       </c>
-      <c r="G3" s="121" t="n">
+      <c r="G3" s="122" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>16.941</v>
-      </c>
-      <c r="H3" s="122" t="n">
+        <v>17.5398</v>
+      </c>
+      <c r="H3" s="123" t="n">
         <f aca="false">G3-F3</f>
-        <v>-2.1621189817083</v>
+        <v>-1.5633189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="119" t="s">
+      <c r="A4" s="120" t="s">
         <v>269</v>
       </c>
       <c r="B4" s="0" t="n">
         <f aca="false">B3+635</f>
         <v>9637</v>
       </c>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="103" t="n">
+      <c r="E4" s="104" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>126.022</v>
-      </c>
-      <c r="F4" s="103" t="n">
+        <v>127.717</v>
+      </c>
+      <c r="F4" s="104" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>97.1109132666878</v>
-      </c>
-      <c r="G4" s="121" t="n">
+        <v>98.8059132666877</v>
+      </c>
+      <c r="G4" s="122" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>98.461</v>
-      </c>
-      <c r="H4" s="122" t="n">
+        <v>101.258</v>
+      </c>
+      <c r="H4" s="123" t="n">
         <f aca="false">G4-F4</f>
-        <v>1.35008673331224</v>
+        <v>2.45208673331224</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="123" t="s">
+      <c r="A5" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="124" t="n">
+      <c r="B5" s="125" t="n">
         <f aca="false">B3+1790</f>
         <v>10792</v>
       </c>
-      <c r="C5" s="124"/>
-      <c r="D5" s="125" t="s">
+      <c r="C5" s="125"/>
+      <c r="D5" s="126" t="s">
         <v>272</v>
       </c>
-      <c r="E5" s="126" t="n">
+      <c r="E5" s="127" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>123.378</v>
-      </c>
-      <c r="F5" s="126" t="n">
+        <v>127.673</v>
+      </c>
+      <c r="F5" s="127" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>91.0019028716503</v>
-      </c>
-      <c r="G5" s="127" t="n">
+        <v>95.2969028716503</v>
+      </c>
+      <c r="G5" s="128" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>92.517</v>
-      </c>
-      <c r="H5" s="122" t="n">
+        <v>98.114</v>
+      </c>
+      <c r="H5" s="123" t="n">
         <f aca="false">G5-F5</f>
-        <v>1.51509712834965</v>
+        <v>2.81709712834967</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="122" t="n">
+      <c r="H6" s="123" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>0.23435495998453</v>
+        <v>1.23528829331787</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="128" t="s">
+      <c r="A8" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="128"/>
-      <c r="C8" s="128"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="129" t="s">
+      <c r="B8" s="129"/>
+      <c r="C8" s="129"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="130" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="130" t="n">
+      <c r="G8" s="131" t="n">
         <v>-0.1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="116"/>
-      <c r="D9" s="117" t="s">
+      <c r="A9" s="117"/>
+      <c r="D9" s="118" t="s">
         <v>266</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3.5</v>
       </c>
-      <c r="G9" s="118" t="n">
+      <c r="G9" s="119" t="n">
         <f aca="false">E9+G8</f>
         <v>3.4</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="119" t="s">
+      <c r="A10" s="120" t="s">
         <v>275</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>10907</v>
       </c>
-      <c r="D10" s="117" t="s">
+      <c r="D10" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="E10" s="122" t="n">
+      <c r="E10" s="123" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>29.305</v>
-      </c>
-      <c r="F10" s="122"/>
-      <c r="G10" s="131" t="n">
+        <v>30.904</v>
+      </c>
+      <c r="F10" s="123"/>
+      <c r="G10" s="132" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>31.4864000290853</v>
+        <v>33.0854000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="119" t="s">
+      <c r="A11" s="120" t="s">
         <v>276</v>
       </c>
       <c r="B11" s="0" t="n">
         <f aca="false">B10+635</f>
         <v>11542</v>
       </c>
-      <c r="D11" s="117" t="s">
+      <c r="D11" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="122" t="n">
+      <c r="E11" s="123" t="n">
         <f aca="false">'Modes A-F'!E57</f>
-        <v>110.088</v>
-      </c>
-      <c r="F11" s="122"/>
-      <c r="G11" s="131" t="n">
+        <v>117.793</v>
+      </c>
+      <c r="F11" s="123"/>
+      <c r="G11" s="132" t="n">
         <f aca="false">E11-B11*TAN(2*(G9-E9)/1000)</f>
-        <v>112.396400030779</v>
+        <v>120.101400030779</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="123" t="s">
+      <c r="A12" s="124" t="s">
         <v>277</v>
       </c>
-      <c r="B12" s="124" t="n">
+      <c r="B12" s="125" t="n">
         <f aca="false">B10+1790</f>
         <v>12697</v>
       </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="125" t="s">
+      <c r="C12" s="125"/>
+      <c r="D12" s="126" t="s">
         <v>272</v>
       </c>
-      <c r="E12" s="132" t="n">
+      <c r="E12" s="133" t="n">
         <f aca="false">'Modes A-F'!E58</f>
-        <v>110.088</v>
-      </c>
-      <c r="F12" s="132"/>
-      <c r="G12" s="133" t="n">
+        <v>117.793</v>
+      </c>
+      <c r="F12" s="133"/>
+      <c r="G12" s="134" t="n">
         <f aca="false">E12-B12*TAN(2*(G9-E9)/1000)</f>
-        <v>112.627400033859</v>
+        <v>120.332400033859</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="128" t="s">
+      <c r="A16" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="128"/>
-      <c r="C16" s="128"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="112"/>
-      <c r="F16" s="129" t="s">
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="130" t="s">
         <v>274</v>
       </c>
-      <c r="G16" s="112" t="n">
+      <c r="G16" s="113" t="n">
         <v>0.275</v>
       </c>
-      <c r="H16" s="112"/>
-      <c r="I16" s="130"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="131"/>
     </row>
     <row r="17" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="116"/>
-      <c r="D17" s="117" t="s">
+      <c r="A17" s="117"/>
+      <c r="D17" s="118" t="s">
         <v>266</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G17" s="71" t="n">
+      <c r="G17" s="72" t="n">
         <f aca="false">E17+G16</f>
         <v>3.5</v>
       </c>
-      <c r="H17" s="134" t="s">
+      <c r="H17" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="I17" s="118" t="n">
+      <c r="I17" s="119" t="n">
         <f aca="false">B18*TAN(2*(E9-G17)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="119" t="s">
+      <c r="A18" s="120" t="s">
         <v>279</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D18" s="117" t="s">
+      <c r="D18" s="118" t="s">
         <v>280</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>-7.25</v>
       </c>
-      <c r="G18" s="135" t="n">
+      <c r="G18" s="136" t="n">
         <f aca="false">E18+B18*TAN(2*(G17-E17)/1000)</f>
         <v>-6.20059989418549</v>
       </c>
-      <c r="I18" s="118"/>
+      <c r="I18" s="119"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="116"/>
-      <c r="D19" s="117" t="s">
+      <c r="A19" s="117"/>
+      <c r="D19" s="118" t="s">
         <v>281</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">3.5 + (3.5-E17)</f>
         <v>3.775</v>
       </c>
-      <c r="G19" s="71" t="n">
+      <c r="G19" s="72" t="n">
         <f aca="false">E19-G16</f>
         <v>3.5</v>
       </c>
-      <c r="I19" s="118"/>
+      <c r="I19" s="119"/>
     </row>
     <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="116"/>
-      <c r="D20" s="117"/>
-      <c r="G20" s="136" t="s">
+      <c r="A20" s="117"/>
+      <c r="D20" s="118"/>
+      <c r="G20" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="I20" s="118"/>
+      <c r="I20" s="119"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="116"/>
-      <c r="F21" s="137" t="s">
+      <c r="A21" s="117"/>
+      <c r="F21" s="138" t="s">
         <v>264</v>
       </c>
-      <c r="I21" s="118"/>
+      <c r="I21" s="119"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="119" t="s">
+      <c r="A22" s="120" t="s">
         <v>267</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D22" s="117" t="s">
+      <c r="D22" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="E22" s="122" t="n">
+      <c r="E22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-38.6613914229833</v>
-      </c>
-      <c r="F22" s="138" t="n">
+        <v>-37.0623914229833</v>
+      </c>
+      <c r="F22" s="139" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.453</v>
-      </c>
-      <c r="G22" s="122" t="n">
+        <v>-22.857</v>
+      </c>
+      <c r="G22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-33.7100292488399</v>
-      </c>
-      <c r="I22" s="118"/>
+        <v>-32.11102924884</v>
+      </c>
+      <c r="I22" s="119"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="119" t="s">
+      <c r="A23" s="120" t="s">
         <v>269</v>
       </c>
       <c r="B23" s="0" t="n">
         <f aca="false">B22+635</f>
         <v>9637</v>
       </c>
-      <c r="D23" s="117" t="s">
+      <c r="D23" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="E23" s="122" t="n">
+      <c r="E23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(E19)/1000)+I17</f>
-        <v>37.3272674801944</v>
-      </c>
-      <c r="F23" s="138" t="n">
+        <v>45.0322674801944</v>
+      </c>
+      <c r="F23" s="139" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>56.616</v>
-      </c>
-      <c r="G23" s="122" t="n">
+        <v>59.419</v>
+      </c>
+      <c r="G23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
-        <v>42.6278981480704</v>
-      </c>
-      <c r="I23" s="118"/>
+        <v>50.3328981480704</v>
+      </c>
+      <c r="I23" s="119"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="123" t="s">
+      <c r="A24" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="B24" s="124" t="n">
+      <c r="B24" s="125" t="n">
         <f aca="false">B22+1790</f>
         <v>10792</v>
       </c>
-      <c r="C24" s="124"/>
-      <c r="D24" s="125" t="s">
+      <c r="C24" s="125"/>
+      <c r="D24" s="126" t="s">
         <v>272</v>
       </c>
-      <c r="E24" s="132" t="n">
+      <c r="E24" s="133" t="n">
         <f aca="false">E12-B24*TAN(2*(E19)/1000)+I17</f>
-        <v>28.6068517843995</v>
-      </c>
-      <c r="F24" s="139" t="n">
+        <v>36.3118517843995</v>
+      </c>
+      <c r="F24" s="140" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>46.772</v>
-      </c>
-      <c r="G24" s="140" t="n">
+        <v>51.275</v>
+      </c>
+      <c r="G24" s="141" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
-        <v>34.542766090482</v>
-      </c>
-      <c r="H24" s="124"/>
-      <c r="I24" s="141"/>
+        <v>42.247766090482</v>
+      </c>
+      <c r="H24" s="125"/>
+      <c r="I24" s="142"/>
     </row>
     <row r="28" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="142" t="s">
+      <c r="A28" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="142"/>
-      <c r="C28" s="142"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="129" t="s">
+      <c r="B28" s="143"/>
+      <c r="C28" s="143"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="130" t="s">
         <v>274</v>
       </c>
-      <c r="G28" s="112" t="n">
+      <c r="G28" s="113" t="n">
         <v>0.275</v>
       </c>
-      <c r="H28" s="112"/>
-      <c r="I28" s="130"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="131"/>
     </row>
     <row r="29" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="116"/>
-      <c r="D29" s="117" t="s">
+      <c r="A29" s="117"/>
+      <c r="D29" s="118" t="s">
         <v>266</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>3.225</v>
       </c>
-      <c r="G29" s="71" t="n">
+      <c r="G29" s="72" t="n">
         <f aca="false">E29+G28</f>
         <v>3.5</v>
       </c>
-      <c r="H29" s="134" t="s">
+      <c r="H29" s="135" t="s">
         <v>278</v>
       </c>
-      <c r="I29" s="118" t="n">
+      <c r="I29" s="119" t="n">
         <f aca="false">B30*TAN(2*(E9-G29)/1000)</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="119" t="s">
+      <c r="A30" s="120" t="s">
         <v>279</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>1908</v>
       </c>
-      <c r="D30" s="117" t="s">
+      <c r="D30" s="118" t="s">
         <v>280</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>-6.583</v>
       </c>
-      <c r="G30" s="135" t="n">
+      <c r="G30" s="136" t="n">
         <f aca="false">E30+B30*TAN(2*(G29-E29)/1000)</f>
         <v>-5.53359989418549</v>
       </c>
-      <c r="I30" s="118"/>
+      <c r="I30" s="119"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="116"/>
-      <c r="D31" s="117" t="s">
+      <c r="A31" s="117"/>
+      <c r="D31" s="118" t="s">
         <v>281</v>
       </c>
       <c r="E31" s="0" t="n">
         <f aca="false">5+(3.5-E29)</f>
         <v>5.275</v>
       </c>
-      <c r="G31" s="71" t="n">
+      <c r="G31" s="72" t="n">
         <f aca="false">E31-G28</f>
         <v>5</v>
       </c>
-      <c r="I31" s="118"/>
+      <c r="I31" s="119"/>
     </row>
     <row r="32" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="116"/>
-      <c r="D32" s="117"/>
-      <c r="G32" s="136" t="s">
+      <c r="A32" s="117"/>
+      <c r="D32" s="118"/>
+      <c r="G32" s="137" t="s">
         <v>282</v>
       </c>
-      <c r="I32" s="118"/>
+      <c r="I32" s="119"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="116"/>
-      <c r="F33" s="137" t="s">
+      <c r="A33" s="117"/>
+      <c r="F33" s="138" t="s">
         <v>264</v>
       </c>
-      <c r="I33" s="118"/>
+      <c r="I33" s="119"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="119" t="s">
+      <c r="A34" s="120" t="s">
         <v>267</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>9002</v>
       </c>
-      <c r="D34" s="117" t="s">
+      <c r="D34" s="118" t="s">
         <v>268</v>
       </c>
-      <c r="E34" s="122" t="n">
+      <c r="E34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-65.6696236638297</v>
-      </c>
-      <c r="F34" s="138" t="n">
+        <v>-64.0706236638297</v>
+      </c>
+      <c r="F34" s="139" t="n">
         <f aca="false">'Modes A-F'!G54</f>
         <v>-55.188</v>
       </c>
-      <c r="G34" s="122" t="n">
+      <c r="G34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-60.7180007866982</v>
-      </c>
-      <c r="I34" s="118"/>
+        <v>-59.1190007866982</v>
+      </c>
+      <c r="I34" s="119"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="119" t="s">
+      <c r="A35" s="120" t="s">
         <v>269</v>
       </c>
       <c r="B35" s="0" t="n">
         <f aca="false">B34+635</f>
         <v>9637</v>
       </c>
-      <c r="D35" s="117" t="s">
+      <c r="D35" s="118" t="s">
         <v>270</v>
       </c>
-      <c r="E35" s="122" t="n">
+      <c r="E35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(E31)/1000)</f>
-        <v>8.41387777734649</v>
-      </c>
-      <c r="F35" s="138" t="n">
+        <v>16.1188777773465</v>
+      </c>
+      <c r="F35" s="139" t="n">
         <f aca="false">'Modes A-F'!G56</f>
         <v>24.4104</v>
       </c>
-      <c r="G35" s="122" t="n">
+      <c r="G35" s="123" t="n">
         <f aca="false">E11-B35*TAN(2*(G31)/1000)+I29</f>
-        <v>13.7147875381681</v>
-      </c>
-      <c r="I35" s="118"/>
+        <v>21.4197875381681</v>
+      </c>
+      <c r="I35" s="119"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="123" t="s">
+      <c r="A36" s="124" t="s">
         <v>271</v>
       </c>
-      <c r="B36" s="124" t="n">
+      <c r="B36" s="125" t="n">
         <f aca="false">B34+1790</f>
         <v>10792</v>
       </c>
-      <c r="C36" s="124"/>
-      <c r="D36" s="125" t="s">
+      <c r="C36" s="125"/>
+      <c r="D36" s="126" t="s">
         <v>272</v>
       </c>
-      <c r="E36" s="132" t="n">
+      <c r="E36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(E31)/1000)</f>
-        <v>-3.77182432571098</v>
-      </c>
-      <c r="F36" s="139" t="n">
+        <v>3.93317567428903</v>
+      </c>
+      <c r="F36" s="140" t="n">
         <f aca="false">'Modes A-F'!G57</f>
         <v>12.81</v>
       </c>
-      <c r="G36" s="132" t="n">
+      <c r="G36" s="133" t="n">
         <f aca="false">E12-B36*TAN(2*(G31)/1000)+I29</f>
-        <v>2.16440252276749</v>
-      </c>
-      <c r="H36" s="124"/>
-      <c r="I36" s="141"/>
+        <v>9.8694025227675</v>
+      </c>
+      <c r="H36" s="125"/>
+      <c r="I36" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -17883,10 +17888,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17957,7 +17961,7 @@
       <c r="A9" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="143" t="n">
+      <c r="B9" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -17981,7 +17985,7 @@
       <c r="A12" s="0" t="s">
         <v>294</v>
       </c>
-      <c r="B12" s="143" t="n">
+      <c r="B12" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18077,7 +18081,7 @@
       <c r="A24" s="0" t="s">
         <v>306</v>
       </c>
-      <c r="B24" s="143" t="n">
+      <c r="B24" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18101,7 +18105,7 @@
       <c r="A27" s="0" t="s">
         <v>309</v>
       </c>
-      <c r="B27" s="143" t="n">
+      <c r="B27" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18197,7 +18201,7 @@
       <c r="A39" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="B39" s="143" t="n">
+      <c r="B39" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18221,7 +18225,7 @@
       <c r="A42" s="0" t="s">
         <v>324</v>
       </c>
-      <c r="B42" s="143" t="n">
+      <c r="B42" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18317,7 +18321,7 @@
       <c r="A54" s="0" t="s">
         <v>336</v>
       </c>
-      <c r="B54" s="143" t="n">
+      <c r="B54" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18341,7 +18345,7 @@
       <c r="A57" s="0" t="s">
         <v>339</v>
       </c>
-      <c r="B57" s="143" t="n">
+      <c r="B57" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18405,7 +18409,7 @@
       <c r="A65" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="B65" s="143" t="n">
+      <c r="B65" s="144" t="n">
         <v>8.1921E-011</v>
       </c>
     </row>
@@ -18413,7 +18417,7 @@
       <c r="A66" s="0" t="s">
         <v>348</v>
       </c>
-      <c r="B66" s="143" t="n">
+      <c r="B66" s="144" t="n">
         <v>6.1817E-009</v>
       </c>
     </row>
@@ -18421,7 +18425,7 @@
       <c r="A67" s="0" t="s">
         <v>349</v>
       </c>
-      <c r="B67" s="143" t="n">
+      <c r="B67" s="144" t="n">
         <v>-8.139E-009</v>
       </c>
     </row>
@@ -18429,7 +18433,7 @@
       <c r="A68" s="0" t="s">
         <v>350</v>
       </c>
-      <c r="B68" s="143" t="n">
+      <c r="B68" s="144" t="n">
         <v>4.2612E-009</v>
       </c>
     </row>
@@ -18749,7 +18753,7 @@
       <c r="A108" s="0" t="s">
         <v>390</v>
       </c>
-      <c r="B108" s="143" t="n">
+      <c r="B108" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18773,7 +18777,7 @@
       <c r="A111" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="B111" s="143" t="n">
+      <c r="B111" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18869,7 +18873,7 @@
       <c r="A123" s="0" t="s">
         <v>405</v>
       </c>
-      <c r="B123" s="143" t="n">
+      <c r="B123" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -18893,7 +18897,7 @@
       <c r="A126" s="0" t="s">
         <v>408</v>
       </c>
-      <c r="B126" s="143" t="n">
+      <c r="B126" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -18989,7 +18993,7 @@
       <c r="A138" s="0" t="s">
         <v>420</v>
       </c>
-      <c r="B138" s="143" t="n">
+      <c r="B138" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19013,7 +19017,7 @@
       <c r="A141" s="0" t="s">
         <v>423</v>
       </c>
-      <c r="B141" s="143" t="n">
+      <c r="B141" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19109,7 +19113,7 @@
       <c r="A153" s="0" t="s">
         <v>435</v>
       </c>
-      <c r="B153" s="143" t="n">
+      <c r="B153" s="144" t="n">
         <v>1E-006</v>
       </c>
     </row>
@@ -19133,7 +19137,7 @@
       <c r="A156" s="0" t="s">
         <v>438</v>
       </c>
-      <c r="B156" s="143" t="n">
+      <c r="B156" s="144" t="n">
         <v>1E-005</v>
       </c>
     </row>
@@ -19197,7 +19201,7 @@
       <c r="A164" s="0" t="s">
         <v>446</v>
       </c>
-      <c r="B164" s="143" t="n">
+      <c r="B164" s="144" t="n">
         <v>1.9024E-008</v>
       </c>
     </row>
@@ -19205,7 +19209,7 @@
       <c r="A165" s="0" t="s">
         <v>447</v>
       </c>
-      <c r="B165" s="143" t="n">
+      <c r="B165" s="144" t="n">
         <v>-9.5679E-009</v>
       </c>
     </row>
@@ -19213,7 +19217,7 @@
       <c r="A166" s="0" t="s">
         <v>448</v>
       </c>
-      <c r="B166" s="143" t="n">
+      <c r="B166" s="144" t="n">
         <v>-1.1631E-009</v>
       </c>
     </row>
@@ -19221,7 +19225,7 @@
       <c r="A167" s="0" t="s">
         <v>449</v>
       </c>
-      <c r="B167" s="143" t="n">
+      <c r="B167" s="144" t="n">
         <v>1.027E-008</v>
       </c>
     </row>
@@ -19357,7 +19361,7 @@
       <c r="A184" s="0" t="s">
         <v>466</v>
       </c>
-      <c r="B184" s="143" t="n">
+      <c r="B184" s="144" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19365,7 +19369,7 @@
       <c r="A185" s="0" t="s">
         <v>467</v>
       </c>
-      <c r="B185" s="143" t="n">
+      <c r="B185" s="144" t="n">
         <v>2.8833E-008</v>
       </c>
     </row>
@@ -19397,7 +19401,7 @@
       <c r="A189" s="0" t="s">
         <v>471</v>
       </c>
-      <c r="B189" s="143" t="n">
+      <c r="B189" s="144" t="n">
         <v>4761600</v>
       </c>
     </row>
@@ -19421,7 +19425,7 @@
       <c r="A192" s="0" t="s">
         <v>474</v>
       </c>
-      <c r="B192" s="143" t="n">
+      <c r="B192" s="144" t="n">
         <v>2.8343E-008</v>
       </c>
     </row>
@@ -19429,7 +19433,7 @@
       <c r="A193" s="0" t="s">
         <v>475</v>
       </c>
-      <c r="B193" s="143" t="n">
+      <c r="B193" s="144" t="n">
         <v>-7.401E-010</v>
       </c>
     </row>
@@ -19437,7 +19441,7 @@
       <c r="A194" s="0" t="s">
         <v>476</v>
       </c>
-      <c r="B194" s="143" t="n">
+      <c r="B194" s="144" t="n">
         <v>-1.4084E-009</v>
       </c>
     </row>
@@ -19445,7 +19449,7 @@
       <c r="A195" s="0" t="s">
         <v>477</v>
       </c>
-      <c r="B195" s="143" t="n">
+      <c r="B195" s="144" t="n">
         <v>2.0325E-008</v>
       </c>
     </row>
@@ -20869,40 +20873,40 @@
       <c r="B337" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C337" s="143" t="n">
+      <c r="C337" s="144" t="n">
         <v>8.3006E-011</v>
       </c>
-      <c r="D337" s="143" t="n">
+      <c r="D337" s="144" t="n">
         <v>8.2839E-011</v>
       </c>
-      <c r="E337" s="143" t="n">
+      <c r="E337" s="144" t="n">
         <v>8.2777E-011</v>
       </c>
-      <c r="F337" s="143" t="n">
+      <c r="F337" s="144" t="n">
         <v>8.1528E-011</v>
       </c>
-      <c r="G337" s="143" t="n">
+      <c r="G337" s="144" t="n">
         <v>8.2662E-011</v>
       </c>
-      <c r="H337" s="143" t="n">
+      <c r="H337" s="144" t="n">
         <v>8.3572E-011</v>
       </c>
-      <c r="I337" s="143" t="n">
+      <c r="I337" s="144" t="n">
         <v>8.489E-011</v>
       </c>
-      <c r="J337" s="143" t="n">
+      <c r="J337" s="144" t="n">
         <v>8.3896E-011</v>
       </c>
-      <c r="K337" s="143" t="n">
+      <c r="K337" s="144" t="n">
         <v>8.2012E-011</v>
       </c>
-      <c r="L337" s="143" t="n">
+      <c r="L337" s="144" t="n">
         <v>8.0897E-011</v>
       </c>
-      <c r="M337" s="143" t="n">
+      <c r="M337" s="144" t="n">
         <v>8.29E-011</v>
       </c>
-      <c r="N337" s="143" t="n">
+      <c r="N337" s="144" t="n">
         <v>8.0797E-011</v>
       </c>
     </row>
@@ -20913,40 +20917,40 @@
       <c r="B338" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C338" s="143" t="n">
+      <c r="C338" s="144" t="n">
         <v>6.3068E-009</v>
       </c>
-      <c r="D338" s="143" t="n">
+      <c r="D338" s="144" t="n">
         <v>6.0737E-009</v>
       </c>
-      <c r="E338" s="143" t="n">
+      <c r="E338" s="144" t="n">
         <v>6.6921E-009</v>
       </c>
-      <c r="F338" s="143" t="n">
+      <c r="F338" s="144" t="n">
         <v>5.7007E-009</v>
       </c>
-      <c r="G338" s="143" t="n">
+      <c r="G338" s="144" t="n">
         <v>5.6393E-009</v>
       </c>
-      <c r="H338" s="143" t="n">
+      <c r="H338" s="144" t="n">
         <v>6.6627E-009</v>
       </c>
-      <c r="I338" s="143" t="n">
+      <c r="I338" s="144" t="n">
         <v>6.6038E-009</v>
       </c>
-      <c r="J338" s="143" t="n">
+      <c r="J338" s="144" t="n">
         <v>5.87E-009</v>
       </c>
-      <c r="K338" s="143" t="n">
+      <c r="K338" s="144" t="n">
         <v>6.1792E-009</v>
       </c>
-      <c r="L338" s="143" t="n">
+      <c r="L338" s="144" t="n">
         <v>5.3276E-009</v>
       </c>
-      <c r="M338" s="143" t="n">
+      <c r="M338" s="144" t="n">
         <v>6.513E-009</v>
       </c>
-      <c r="N338" s="143" t="n">
+      <c r="N338" s="144" t="n">
         <v>5.9829E-009</v>
       </c>
     </row>
@@ -20957,40 +20961,40 @@
       <c r="B339" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C339" s="143" t="n">
+      <c r="C339" s="144" t="n">
         <v>-7.2948E-009</v>
       </c>
-      <c r="D339" s="143" t="n">
+      <c r="D339" s="144" t="n">
         <v>-7.6015E-009</v>
       </c>
-      <c r="E339" s="143" t="n">
+      <c r="E339" s="144" t="n">
         <v>-7.4862E-009</v>
       </c>
-      <c r="F339" s="143" t="n">
+      <c r="F339" s="144" t="n">
         <v>-8.5513E-009</v>
       </c>
-      <c r="G339" s="143" t="n">
+      <c r="G339" s="144" t="n">
         <v>-8.3206E-009</v>
       </c>
-      <c r="H339" s="143" t="n">
+      <c r="H339" s="144" t="n">
         <v>-7.5942E-009</v>
       </c>
-      <c r="I339" s="143" t="n">
+      <c r="I339" s="144" t="n">
         <v>-7.5377E-009</v>
       </c>
-      <c r="J339" s="143" t="n">
+      <c r="J339" s="144" t="n">
         <v>-8.5415E-009</v>
       </c>
-      <c r="K339" s="143" t="n">
+      <c r="K339" s="144" t="n">
         <v>-7.7635E-009</v>
       </c>
-      <c r="L339" s="143" t="n">
+      <c r="L339" s="144" t="n">
         <v>-8.0482E-009</v>
       </c>
-      <c r="M339" s="143" t="n">
+      <c r="M339" s="144" t="n">
         <v>-8.2175E-009</v>
       </c>
-      <c r="N339" s="143" t="n">
+      <c r="N339" s="144" t="n">
         <v>-7.9966E-009</v>
       </c>
     </row>
@@ -21001,40 +21005,40 @@
       <c r="B340" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C340" s="143" t="n">
+      <c r="C340" s="144" t="n">
         <v>4.8625E-009</v>
       </c>
-      <c r="D340" s="143" t="n">
+      <c r="D340" s="144" t="n">
         <v>4.433E-009</v>
       </c>
-      <c r="E340" s="143" t="n">
+      <c r="E340" s="144" t="n">
         <v>3.4611E-009</v>
       </c>
-      <c r="F340" s="143" t="n">
+      <c r="F340" s="144" t="n">
         <v>3.9372E-009</v>
       </c>
-      <c r="G340" s="143" t="n">
+      <c r="G340" s="144" t="n">
         <v>4.8526E-009</v>
       </c>
-      <c r="H340" s="143" t="n">
+      <c r="H340" s="144" t="n">
         <v>4.5041E-009</v>
       </c>
-      <c r="I340" s="143" t="n">
+      <c r="I340" s="144" t="n">
         <v>4.5311E-009</v>
       </c>
-      <c r="J340" s="143" t="n">
+      <c r="J340" s="144" t="n">
         <v>4.2882E-009</v>
       </c>
-      <c r="K340" s="143" t="n">
+      <c r="K340" s="144" t="n">
         <v>4.4551E-009</v>
       </c>
-      <c r="L340" s="143" t="n">
+      <c r="L340" s="144" t="n">
         <v>4.136E-009</v>
       </c>
-      <c r="M340" s="143" t="n">
+      <c r="M340" s="144" t="n">
         <v>3.9078E-009</v>
       </c>
-      <c r="N340" s="143" t="n">
+      <c r="N340" s="144" t="n">
         <v>3.9593E-009</v>
       </c>
     </row>
@@ -21749,40 +21753,40 @@
       <c r="B357" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C357" s="143" t="n">
+      <c r="C357" s="144" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="D357" s="143" t="n">
+      <c r="D357" s="144" t="n">
         <v>1.9514E-008</v>
       </c>
-      <c r="E357" s="143" t="n">
+      <c r="E357" s="144" t="n">
         <v>1.8533E-008</v>
       </c>
-      <c r="F357" s="143" t="n">
+      <c r="F357" s="144" t="n">
         <v>2.1231E-008</v>
       </c>
-      <c r="G357" s="143" t="n">
+      <c r="G357" s="144" t="n">
         <v>2.4174E-008</v>
       </c>
-      <c r="H357" s="143" t="n">
+      <c r="H357" s="144" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="I357" s="143" t="n">
+      <c r="I357" s="144" t="n">
         <v>2.8588E-008</v>
       </c>
-      <c r="J357" s="143" t="n">
+      <c r="J357" s="144" t="n">
         <v>1.9024E-008</v>
       </c>
-      <c r="K357" s="143" t="n">
+      <c r="K357" s="144" t="n">
         <v>3.2757E-008</v>
       </c>
-      <c r="L357" s="143" t="n">
+      <c r="L357" s="144" t="n">
         <v>3.5455E-008</v>
       </c>
-      <c r="M357" s="143" t="n">
+      <c r="M357" s="144" t="n">
         <v>2.025E-008</v>
       </c>
-      <c r="N357" s="143" t="n">
+      <c r="N357" s="144" t="n">
         <v>2.1231E-008</v>
       </c>
     </row>
@@ -21793,40 +21797,40 @@
       <c r="B358" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C358" s="143" t="n">
+      <c r="C358" s="144" t="n">
         <v>-1.766E-008</v>
       </c>
-      <c r="D358" s="143" t="n">
+      <c r="D358" s="144" t="n">
         <v>-4.4184E-009</v>
       </c>
-      <c r="E358" s="143" t="n">
+      <c r="E358" s="144" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="F358" s="143" t="n">
+      <c r="F358" s="144" t="n">
         <v>-1.1039E-008</v>
       </c>
-      <c r="G358" s="143" t="n">
+      <c r="G358" s="144" t="n">
         <v>-9.5679E-009</v>
       </c>
-      <c r="H358" s="143" t="n">
+      <c r="H358" s="144" t="n">
         <v>-1.1284E-008</v>
       </c>
-      <c r="I358" s="143" t="n">
+      <c r="I358" s="144" t="n">
         <v>-2.2114E-009</v>
       </c>
-      <c r="J358" s="143" t="n">
+      <c r="J358" s="144" t="n">
         <v>-5.3992E-009</v>
       </c>
-      <c r="K358" s="143" t="n">
+      <c r="K358" s="144" t="n">
         <v>9.7642E-010</v>
       </c>
-      <c r="L358" s="143" t="n">
+      <c r="L358" s="144" t="n">
         <v>6.3712E-009</v>
       </c>
-      <c r="M358" s="143" t="n">
+      <c r="M358" s="144" t="n">
         <v>-1.153E-008</v>
       </c>
-      <c r="N358" s="143" t="n">
+      <c r="N358" s="144" t="n">
         <v>-9.8131E-009</v>
       </c>
     </row>
@@ -21837,40 +21841,40 @@
       <c r="B359" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C359" s="143" t="n">
+      <c r="C359" s="144" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="D359" s="143" t="n">
+      <c r="D359" s="144" t="n">
         <v>-4.3514E-009</v>
       </c>
-      <c r="E359" s="143" t="n">
+      <c r="E359" s="144" t="n">
         <v>-6.0682E-009</v>
       </c>
-      <c r="F359" s="143" t="n">
+      <c r="F359" s="144" t="n">
         <v>-9.0112E-009</v>
       </c>
-      <c r="G359" s="143" t="n">
+      <c r="G359" s="144" t="n">
         <v>-4.5967E-009</v>
       </c>
-      <c r="H359" s="143" t="n">
+      <c r="H359" s="144" t="n">
         <v>-1.0483E-008</v>
       </c>
-      <c r="I359" s="143" t="n">
+      <c r="I359" s="144" t="n">
         <v>7.6659E-009</v>
       </c>
-      <c r="J359" s="143" t="n">
+      <c r="J359" s="144" t="n">
         <v>-3.3704E-009</v>
       </c>
-      <c r="K359" s="143" t="n">
+      <c r="K359" s="144" t="n">
         <v>6.6849E-009</v>
       </c>
-      <c r="L359" s="143" t="n">
+      <c r="L359" s="144" t="n">
         <v>5.2134E-009</v>
       </c>
-      <c r="M359" s="143" t="n">
+      <c r="M359" s="144" t="n">
         <v>-1.6536E-009</v>
       </c>
-      <c r="N359" s="143" t="n">
+      <c r="N359" s="144" t="n">
         <v>-5.5777E-009</v>
       </c>
     </row>
@@ -21881,40 +21885,40 @@
       <c r="B360" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C360" s="143" t="n">
+      <c r="C360" s="144" t="n">
         <v>7.8174E-009</v>
       </c>
-      <c r="D360" s="143" t="n">
+      <c r="D360" s="144" t="n">
         <v>2.3513E-008</v>
       </c>
-      <c r="E360" s="143" t="n">
+      <c r="E360" s="144" t="n">
         <v>1.7382E-008</v>
       </c>
-      <c r="F360" s="143" t="n">
+      <c r="F360" s="144" t="n">
         <v>1.1006E-008</v>
       </c>
-      <c r="G360" s="143" t="n">
+      <c r="G360" s="144" t="n">
         <v>1.5665E-008</v>
       </c>
-      <c r="H360" s="143" t="n">
+      <c r="H360" s="144" t="n">
         <v>1.2477E-008</v>
       </c>
-      <c r="I360" s="143" t="n">
+      <c r="I360" s="144" t="n">
         <v>2.057E-008</v>
       </c>
-      <c r="J360" s="143" t="n">
+      <c r="J360" s="144" t="n">
         <v>1.9835E-008</v>
       </c>
-      <c r="K360" s="143" t="n">
+      <c r="K360" s="144" t="n">
         <v>2.5721E-008</v>
       </c>
-      <c r="L360" s="143" t="n">
+      <c r="L360" s="144" t="n">
         <v>2.5475E-008</v>
       </c>
-      <c r="M360" s="143" t="n">
+      <c r="M360" s="144" t="n">
         <v>1.076E-008</v>
       </c>
-      <c r="N360" s="143" t="n">
+      <c r="N360" s="144" t="n">
         <v>1.3213E-008</v>
       </c>
     </row>
@@ -22057,7 +22061,7 @@
       <c r="B364" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C364" s="143" t="n">
+      <c r="C364" s="144" t="n">
         <v>2.8343E-008</v>
       </c>
       <c r="D364" s="0" t="n">
@@ -22101,7 +22105,7 @@
       <c r="B365" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C365" s="143" t="n">
+      <c r="C365" s="144" t="n">
         <v>-7.401E-010</v>
       </c>
       <c r="D365" s="0" t="n">
@@ -22145,7 +22149,7 @@
       <c r="B366" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C366" s="143" t="n">
+      <c r="C366" s="144" t="n">
         <v>-1.4084E-009</v>
       </c>
       <c r="D366" s="0" t="n">
@@ -22189,7 +22193,7 @@
       <c r="B367" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C367" s="143" t="n">
+      <c r="C367" s="144" t="n">
         <v>2.0325E-008</v>
       </c>
       <c r="D367" s="0" t="n">
@@ -23951,28 +23955,27 @@
   </sheetPr>
   <dimension ref="A1:G2383"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A44" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B1" s="144" t="s">
+      <c r="B1" s="145" t="s">
         <v>813</v>
       </c>
-      <c r="C1" s="144" t="n">
+      <c r="C1" s="145" t="n">
         <v>350</v>
       </c>
-      <c r="D1" s="144" t="s">
+      <c r="D1" s="145" t="s">
         <v>814</v>
       </c>
     </row>
@@ -23980,10 +23983,10 @@
       <c r="A2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="145" t="s">
         <v>815</v>
       </c>
-      <c r="C2" s="144" t="n">
+      <c r="C2" s="145" t="n">
         <v>0.5</v>
       </c>
     </row>
@@ -23991,10 +23994,10 @@
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="144" t="s">
+      <c r="B3" s="145" t="s">
         <v>816</v>
       </c>
-      <c r="C3" s="144" t="n">
+      <c r="C3" s="145" t="n">
         <v>0.0004</v>
       </c>
     </row>
@@ -24098,7 +24101,7 @@
       <c r="B16" s="0" t="s">
         <v>831</v>
       </c>
-      <c r="C16" s="143" t="n">
+      <c r="C16" s="144" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -24106,7 +24109,7 @@
       <c r="B17" s="0" t="s">
         <v>832</v>
       </c>
-      <c r="C17" s="143" t="n">
+      <c r="C17" s="144" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -24114,7 +24117,7 @@
       <c r="B18" s="0" t="s">
         <v>833</v>
       </c>
-      <c r="C18" s="143" t="n">
+      <c r="C18" s="144" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -24122,7 +24125,7 @@
       <c r="B19" s="0" t="s">
         <v>834</v>
       </c>
-      <c r="C19" s="143" t="n">
+      <c r="C19" s="144" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -24610,7 +24613,7 @@
       <c r="B80" s="0" t="s">
         <v>902</v>
       </c>
-      <c r="C80" s="143" t="n">
+      <c r="C80" s="144" t="n">
         <v>1.58855E-007</v>
       </c>
     </row>
@@ -24658,7 +24661,7 @@
       <c r="B86" s="0" t="s">
         <v>908</v>
       </c>
-      <c r="C86" s="143" t="n">
+      <c r="C86" s="144" t="n">
         <v>1.58316E-007</v>
       </c>
     </row>
@@ -24690,7 +24693,7 @@
       <c r="B90" s="0" t="s">
         <v>912</v>
       </c>
-      <c r="C90" s="143" t="n">
+      <c r="C90" s="144" t="n">
         <v>1.57838E-007</v>
       </c>
     </row>
@@ -24778,7 +24781,7 @@
       <c r="B101" s="0" t="s">
         <v>924</v>
       </c>
-      <c r="C101" s="143" t="n">
+      <c r="C101" s="144" t="n">
         <v>2.397E-009</v>
       </c>
     </row>
@@ -24954,7 +24957,7 @@
       <c r="B123" s="0" t="s">
         <v>948</v>
       </c>
-      <c r="C123" s="143" t="n">
+      <c r="C123" s="144" t="n">
         <v>2.37898E-010</v>
       </c>
     </row>
@@ -25018,7 +25021,7 @@
       <c r="B131" s="0" t="s">
         <v>956</v>
       </c>
-      <c r="C131" s="143" t="n">
+      <c r="C131" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25034,7 +25037,7 @@
       <c r="B133" s="0" t="s">
         <v>958</v>
       </c>
-      <c r="C133" s="143" t="n">
+      <c r="C133" s="144" t="n">
         <v>1.97895E-005</v>
       </c>
     </row>
@@ -25554,7 +25557,7 @@
       <c r="B198" s="0" t="s">
         <v>1025</v>
       </c>
-      <c r="C198" s="143" t="n">
+      <c r="C198" s="144" t="n">
         <v>2.78422E-007</v>
       </c>
     </row>
@@ -25602,7 +25605,7 @@
       <c r="B204" s="0" t="s">
         <v>1031</v>
       </c>
-      <c r="C204" s="143" t="n">
+      <c r="C204" s="144" t="n">
         <v>2.77565E-007</v>
       </c>
     </row>
@@ -25634,7 +25637,7 @@
       <c r="B208" s="0" t="s">
         <v>1035</v>
       </c>
-      <c r="C208" s="143" t="n">
+      <c r="C208" s="144" t="n">
         <v>2.76716E-007</v>
       </c>
     </row>
@@ -25722,7 +25725,7 @@
       <c r="B219" s="0" t="s">
         <v>1046</v>
       </c>
-      <c r="C219" s="143" t="n">
+      <c r="C219" s="144" t="n">
         <v>5.98328E-009</v>
       </c>
     </row>
@@ -25898,7 +25901,7 @@
       <c r="B241" s="0" t="s">
         <v>1069</v>
       </c>
-      <c r="C241" s="143" t="n">
+      <c r="C241" s="144" t="n">
         <v>4.11728E-010</v>
       </c>
     </row>
@@ -25962,7 +25965,7 @@
       <c r="B249" s="0" t="s">
         <v>1077</v>
       </c>
-      <c r="C249" s="143" t="n">
+      <c r="C249" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -25978,7 +25981,7 @@
       <c r="B251" s="0" t="s">
         <v>1079</v>
       </c>
-      <c r="C251" s="143" t="n">
+      <c r="C251" s="144" t="n">
         <v>3.46956E-005</v>
       </c>
     </row>
@@ -26498,7 +26501,7 @@
       <c r="B316" s="0" t="s">
         <v>1144</v>
       </c>
-      <c r="C316" s="143" t="n">
+      <c r="C316" s="144" t="n">
         <v>5.45673E-012</v>
       </c>
     </row>
@@ -26546,7 +26549,7 @@
       <c r="B322" s="0" t="s">
         <v>1150</v>
       </c>
-      <c r="C322" s="143" t="n">
+      <c r="C322" s="144" t="n">
         <v>7.71713E-013</v>
       </c>
     </row>
@@ -26578,7 +26581,7 @@
       <c r="B326" s="0" t="s">
         <v>1154</v>
       </c>
-      <c r="C326" s="143" t="n">
+      <c r="C326" s="144" t="n">
         <v>-7.72781E-012</v>
       </c>
     </row>
@@ -26666,7 +26669,7 @@
       <c r="B337" s="0" t="s">
         <v>1165</v>
       </c>
-      <c r="C337" s="143" t="n">
+      <c r="C337" s="144" t="n">
         <v>5.61762E-010</v>
       </c>
     </row>
@@ -26842,7 +26845,7 @@
       <c r="B359" s="0" t="s">
         <v>1188</v>
       </c>
-      <c r="C359" s="143" t="n">
+      <c r="C359" s="144" t="n">
         <v>2.605E-012</v>
       </c>
     </row>
@@ -26906,7 +26909,7 @@
       <c r="B367" s="0" t="s">
         <v>1196</v>
       </c>
-      <c r="C367" s="143" t="n">
+      <c r="C367" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -26922,7 +26925,7 @@
       <c r="B369" s="0" t="s">
         <v>1198</v>
       </c>
-      <c r="C369" s="143" t="n">
+      <c r="C369" s="144" t="n">
         <v>9.64642E-011</v>
       </c>
     </row>
@@ -27442,7 +27445,7 @@
       <c r="B434" s="0" t="s">
         <v>1263</v>
       </c>
-      <c r="C434" s="143" t="n">
+      <c r="C434" s="144" t="n">
         <v>5.42202E-012</v>
       </c>
     </row>
@@ -27490,7 +27493,7 @@
       <c r="B440" s="0" t="s">
         <v>1269</v>
       </c>
-      <c r="C440" s="143" t="n">
+      <c r="C440" s="144" t="n">
         <v>5.83458E-013</v>
       </c>
     </row>
@@ -27522,7 +27525,7 @@
       <c r="B444" s="0" t="s">
         <v>1273</v>
       </c>
-      <c r="C444" s="143" t="n">
+      <c r="C444" s="144" t="n">
         <v>-5.09224E-012</v>
       </c>
     </row>
@@ -27610,7 +27613,7 @@
       <c r="B455" s="0" t="s">
         <v>1284</v>
       </c>
-      <c r="C455" s="143" t="n">
+      <c r="C455" s="144" t="n">
         <v>2.08783E-010</v>
       </c>
     </row>
@@ -27786,7 +27789,7 @@
       <c r="B477" s="0" t="s">
         <v>1307</v>
       </c>
-      <c r="C477" s="143" t="n">
+      <c r="C477" s="144" t="n">
         <v>2.32565E-012</v>
       </c>
     </row>
@@ -27850,7 +27853,7 @@
       <c r="B485" s="0" t="s">
         <v>1315</v>
       </c>
-      <c r="C485" s="143" t="n">
+      <c r="C485" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -27866,7 +27869,7 @@
       <c r="B487" s="0" t="s">
         <v>1317</v>
       </c>
-      <c r="C487" s="143" t="n">
+      <c r="C487" s="144" t="n">
         <v>7.29322E-011</v>
       </c>
     </row>
@@ -27954,7 +27957,7 @@
       <c r="B498" s="0" t="s">
         <v>1328</v>
       </c>
-      <c r="C498" s="143" t="n">
+      <c r="C498" s="144" t="n">
         <v>3.71179E-009</v>
       </c>
     </row>
@@ -27962,7 +27965,7 @@
       <c r="B499" s="0" t="s">
         <v>1329</v>
       </c>
-      <c r="C499" s="143" t="n">
+      <c r="C499" s="144" t="n">
         <v>3.71272E-009</v>
       </c>
     </row>
@@ -27970,7 +27973,7 @@
       <c r="B500" s="0" t="s">
         <v>1330</v>
       </c>
-      <c r="C500" s="143" t="n">
+      <c r="C500" s="144" t="n">
         <v>3.71425E-009</v>
       </c>
     </row>
@@ -27978,7 +27981,7 @@
       <c r="B501" s="0" t="s">
         <v>1331</v>
       </c>
-      <c r="C501" s="143" t="n">
+      <c r="C501" s="144" t="n">
         <v>3.71562E-009</v>
       </c>
     </row>
@@ -28546,7 +28549,7 @@
       <c r="B572" s="0" t="s">
         <v>1402</v>
       </c>
-      <c r="C572" s="143" t="n">
+      <c r="C572" s="144" t="n">
         <v>1.19678E-007</v>
       </c>
     </row>
@@ -28594,7 +28597,7 @@
       <c r="B578" s="0" t="s">
         <v>1408</v>
       </c>
-      <c r="C578" s="143" t="n">
+      <c r="C578" s="144" t="n">
         <v>1.19249E-007</v>
       </c>
     </row>
@@ -28626,7 +28629,7 @@
       <c r="B582" s="0" t="s">
         <v>1412</v>
       </c>
-      <c r="C582" s="143" t="n">
+      <c r="C582" s="144" t="n">
         <v>1.18808E-007</v>
       </c>
     </row>
@@ -28714,7 +28717,7 @@
       <c r="B593" s="0" t="s">
         <v>1423</v>
       </c>
-      <c r="C593" s="143" t="n">
+      <c r="C593" s="144" t="n">
         <v>3.58628E-009</v>
       </c>
     </row>
@@ -28890,7 +28893,7 @@
       <c r="B615" s="0" t="s">
         <v>1446</v>
       </c>
-      <c r="C615" s="143" t="n">
+      <c r="C615" s="144" t="n">
         <v>1.9029E-010</v>
       </c>
     </row>
@@ -28954,7 +28957,7 @@
       <c r="B623" s="0" t="s">
         <v>1454</v>
       </c>
-      <c r="C623" s="143" t="n">
+      <c r="C623" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -28970,7 +28973,7 @@
       <c r="B625" s="0" t="s">
         <v>1456</v>
       </c>
-      <c r="C625" s="143" t="n">
+      <c r="C625" s="144" t="n">
         <v>1.49062E-005</v>
       </c>
     </row>
@@ -29490,7 +29493,7 @@
       <c r="B690" s="0" t="s">
         <v>1521</v>
       </c>
-      <c r="C690" s="143" t="n">
+      <c r="C690" s="144" t="n">
         <v>5.80654E-012</v>
       </c>
     </row>
@@ -29538,7 +29541,7 @@
       <c r="B696" s="0" t="s">
         <v>1527</v>
       </c>
-      <c r="C696" s="143" t="n">
+      <c r="C696" s="144" t="n">
         <v>-1.88255E-013</v>
       </c>
     </row>
@@ -29570,7 +29573,7 @@
       <c r="B700" s="0" t="s">
         <v>1531</v>
       </c>
-      <c r="C700" s="143" t="n">
+      <c r="C700" s="144" t="n">
         <v>-6.71043E-012</v>
       </c>
     </row>
@@ -29658,7 +29661,7 @@
       <c r="B711" s="0" t="s">
         <v>1542</v>
       </c>
-      <c r="C711" s="143" t="n">
+      <c r="C711" s="144" t="n">
         <v>-3.52979E-010</v>
       </c>
     </row>
@@ -29834,7 +29837,7 @@
       <c r="B733" s="0" t="s">
         <v>1565</v>
       </c>
-      <c r="C733" s="143" t="n">
+      <c r="C733" s="144" t="n">
         <v>2.64443E-012</v>
       </c>
     </row>
@@ -29898,7 +29901,7 @@
       <c r="B741" s="0" t="s">
         <v>1573</v>
       </c>
-      <c r="C741" s="143" t="n">
+      <c r="C741" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -29914,7 +29917,7 @@
       <c r="B743" s="0" t="s">
         <v>1575</v>
       </c>
-      <c r="C743" s="143" t="n">
+      <c r="C743" s="144" t="n">
         <v>-2.35319E-011</v>
       </c>
     </row>
@@ -30470,7 +30473,7 @@
       <c r="B811" s="0" t="s">
         <v>1651</v>
       </c>
-      <c r="C811" s="143" t="n">
+      <c r="C811" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -30986,7 +30989,7 @@
       <c r="B874" s="0" t="s">
         <v>1716</v>
       </c>
-      <c r="C874" s="143" t="n">
+      <c r="C874" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -31502,7 +31505,7 @@
       <c r="B937" s="0" t="s">
         <v>1781</v>
       </c>
-      <c r="C937" s="143" t="n">
+      <c r="C937" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32018,7 +32021,7 @@
       <c r="B1000" s="0" t="s">
         <v>1846</v>
       </c>
-      <c r="C1000" s="143" t="n">
+      <c r="C1000" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -32534,7 +32537,7 @@
       <c r="B1063" s="0" t="s">
         <v>1911</v>
       </c>
-      <c r="C1063" s="143" t="n">
+      <c r="C1063" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33050,7 +33053,7 @@
       <c r="B1126" s="0" t="s">
         <v>1976</v>
       </c>
-      <c r="C1126" s="143" t="n">
+      <c r="C1126" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -33566,7 +33569,7 @@
       <c r="B1189" s="0" t="s">
         <v>2041</v>
       </c>
-      <c r="C1189" s="143" t="n">
+      <c r="C1189" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34082,7 +34085,7 @@
       <c r="B1252" s="0" t="s">
         <v>2106</v>
       </c>
-      <c r="C1252" s="143" t="n">
+      <c r="C1252" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -34598,7 +34601,7 @@
       <c r="B1315" s="0" t="s">
         <v>2171</v>
       </c>
-      <c r="C1315" s="143" t="n">
+      <c r="C1315" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35114,7 +35117,7 @@
       <c r="B1378" s="0" t="s">
         <v>2236</v>
       </c>
-      <c r="C1378" s="143" t="n">
+      <c r="C1378" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -35630,7 +35633,7 @@
       <c r="B1441" s="0" t="s">
         <v>2301</v>
       </c>
-      <c r="C1441" s="143" t="n">
+      <c r="C1441" s="144" t="n">
         <v>877877000</v>
       </c>
     </row>
@@ -36078,7 +36081,7 @@
       <c r="B1497" s="0" t="s">
         <v>2360</v>
       </c>
-      <c r="C1497" s="143" t="n">
+      <c r="C1497" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36704,7 +36707,7 @@
       <c r="B1576" s="0" t="s">
         <v>2444</v>
       </c>
-      <c r="C1576" s="143" t="n">
+      <c r="C1576" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -36873,7 +36876,7 @@
       <c r="B1596" s="0" t="s">
         <v>2466</v>
       </c>
-      <c r="C1596" s="143" t="n">
+      <c r="C1596" s="144" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -36881,7 +36884,7 @@
       <c r="B1597" s="0" t="s">
         <v>2467</v>
       </c>
-      <c r="C1597" s="143" t="n">
+      <c r="C1597" s="144" t="n">
         <v>1000000</v>
       </c>
     </row>
@@ -37761,7 +37764,7 @@
       <c r="B1707" s="0" t="s">
         <v>2578</v>
       </c>
-      <c r="C1707" s="143" t="n">
+      <c r="C1707" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -37777,7 +37780,7 @@
       <c r="B1709" s="0" t="s">
         <v>2580</v>
       </c>
-      <c r="C1709" s="143" t="n">
+      <c r="C1709" s="144" t="n">
         <v>34197800</v>
       </c>
     </row>
@@ -38297,7 +38300,7 @@
       <c r="B1774" s="0" t="s">
         <v>2645</v>
       </c>
-      <c r="C1774" s="143" t="n">
+      <c r="C1774" s="144" t="n">
         <v>12147700</v>
       </c>
     </row>
@@ -38377,7 +38380,7 @@
       <c r="B1784" s="0" t="s">
         <v>2655</v>
       </c>
-      <c r="C1784" s="143" t="n">
+      <c r="C1784" s="144" t="n">
         <v>-7098040</v>
       </c>
     </row>
@@ -38465,7 +38468,7 @@
       <c r="B1795" s="0" t="s">
         <v>2666</v>
       </c>
-      <c r="C1795" s="143" t="n">
+      <c r="C1795" s="144" t="n">
         <v>4465690</v>
       </c>
     </row>
@@ -38641,7 +38644,7 @@
       <c r="B1817" s="0" t="s">
         <v>2689</v>
       </c>
-      <c r="C1817" s="143" t="n">
+      <c r="C1817" s="144" t="n">
         <v>1999640</v>
       </c>
     </row>
@@ -38705,7 +38708,7 @@
       <c r="B1825" s="0" t="s">
         <v>2697</v>
       </c>
-      <c r="C1825" s="143" t="n">
+      <c r="C1825" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -38721,7 +38724,7 @@
       <c r="B1827" s="0" t="s">
         <v>2699</v>
       </c>
-      <c r="C1827" s="143" t="n">
+      <c r="C1827" s="144" t="n">
         <v>-13532400</v>
       </c>
     </row>
@@ -39324,7 +39327,7 @@
       <c r="B1902" s="0" t="s">
         <v>2776</v>
       </c>
-      <c r="C1902" s="143" t="n">
+      <c r="C1902" s="144" t="n">
         <v>4.37265E-007</v>
       </c>
     </row>
@@ -39372,7 +39375,7 @@
       <c r="B1908" s="0" t="s">
         <v>2782</v>
       </c>
-      <c r="C1908" s="143" t="n">
+      <c r="C1908" s="144" t="n">
         <v>4.35882E-007</v>
       </c>
     </row>
@@ -39404,7 +39407,7 @@
       <c r="B1912" s="0" t="s">
         <v>2786</v>
       </c>
-      <c r="C1912" s="143" t="n">
+      <c r="C1912" s="144" t="n">
         <v>4.34577E-007</v>
       </c>
     </row>
@@ -39492,7 +39495,7 @@
       <c r="B1923" s="0" t="s">
         <v>2797</v>
       </c>
-      <c r="C1923" s="143" t="n">
+      <c r="C1923" s="144" t="n">
         <v>9.15083E-009</v>
       </c>
     </row>
@@ -39668,7 +39671,7 @@
       <c r="B1945" s="0" t="s">
         <v>2820</v>
       </c>
-      <c r="C1945" s="143" t="n">
+      <c r="C1945" s="144" t="n">
         <v>6.45121E-010</v>
       </c>
     </row>
@@ -39732,7 +39735,7 @@
       <c r="B1953" s="0" t="s">
         <v>2828</v>
       </c>
-      <c r="C1953" s="143" t="n">
+      <c r="C1953" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -39748,7 +39751,7 @@
       <c r="B1955" s="0" t="s">
         <v>2830</v>
       </c>
-      <c r="C1955" s="143" t="n">
+      <c r="C1955" s="144" t="n">
         <v>5.44853E-005</v>
       </c>
     </row>
@@ -40268,7 +40271,7 @@
       <c r="B2020" s="0" t="s">
         <v>2895</v>
       </c>
-      <c r="C2020" s="143" t="n">
+      <c r="C2020" s="144" t="n">
         <v>4.37266E-007</v>
       </c>
     </row>
@@ -40316,7 +40319,7 @@
       <c r="B2026" s="0" t="s">
         <v>2901</v>
       </c>
-      <c r="C2026" s="143" t="n">
+      <c r="C2026" s="144" t="n">
         <v>4.35881E-007</v>
       </c>
     </row>
@@ -40348,7 +40351,7 @@
       <c r="B2030" s="0" t="s">
         <v>2905</v>
       </c>
-      <c r="C2030" s="143" t="n">
+      <c r="C2030" s="144" t="n">
         <v>4.34576E-007</v>
       </c>
     </row>
@@ -40436,7 +40439,7 @@
       <c r="B2041" s="0" t="s">
         <v>2916</v>
       </c>
-      <c r="C2041" s="143" t="n">
+      <c r="C2041" s="144" t="n">
         <v>8.38028E-009</v>
       </c>
     </row>
@@ -40612,7 +40615,7 @@
       <c r="B2063" s="0" t="s">
         <v>2939</v>
       </c>
-      <c r="C2063" s="143" t="n">
+      <c r="C2063" s="144" t="n">
         <v>6.44996E-010</v>
       </c>
     </row>
@@ -40676,7 +40679,7 @@
       <c r="B2071" s="0" t="s">
         <v>2947</v>
       </c>
-      <c r="C2071" s="143" t="n">
+      <c r="C2071" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -40692,7 +40695,7 @@
       <c r="B2073" s="0" t="s">
         <v>2949</v>
       </c>
-      <c r="C2073" s="143" t="n">
+      <c r="C2073" s="144" t="n">
         <v>5.44851E-005</v>
       </c>
     </row>
@@ -41212,7 +41215,7 @@
       <c r="B2138" s="0" t="s">
         <v>3014</v>
       </c>
-      <c r="C2138" s="143" t="n">
+      <c r="C2138" s="144" t="n">
         <v>1.0545E-011</v>
       </c>
     </row>
@@ -41260,7 +41263,7 @@
       <c r="B2144" s="0" t="s">
         <v>3020</v>
       </c>
-      <c r="C2144" s="143" t="n">
+      <c r="C2144" s="144" t="n">
         <v>1.35517E-012</v>
       </c>
     </row>
@@ -41292,7 +41295,7 @@
       <c r="B2148" s="0" t="s">
         <v>3024</v>
       </c>
-      <c r="C2148" s="143" t="n">
+      <c r="C2148" s="144" t="n">
         <v>-1.06504E-011</v>
       </c>
     </row>
@@ -41380,7 +41383,7 @@
       <c r="B2159" s="0" t="s">
         <v>3035</v>
       </c>
-      <c r="C2159" s="143" t="n">
+      <c r="C2159" s="144" t="n">
         <v>7.70545E-010</v>
       </c>
     </row>
@@ -41556,7 +41559,7 @@
       <c r="B2181" s="0" t="s">
         <v>3058</v>
       </c>
-      <c r="C2181" s="143" t="n">
+      <c r="C2181" s="144" t="n">
         <v>4.1709E-012</v>
       </c>
     </row>
@@ -41620,7 +41623,7 @@
       <c r="B2189" s="0" t="s">
         <v>3066</v>
       </c>
-      <c r="C2189" s="143" t="n">
+      <c r="C2189" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -41636,7 +41639,7 @@
       <c r="B2191" s="0" t="s">
         <v>3068</v>
       </c>
-      <c r="C2191" s="143" t="n">
+      <c r="C2191" s="144" t="n">
         <v>1.69396E-010</v>
       </c>
     </row>
@@ -42212,7 +42215,7 @@
       <c r="B2263" s="0" t="s">
         <v>3143</v>
       </c>
-      <c r="C2263" s="143" t="n">
+      <c r="C2263" s="144" t="n">
         <v>877987000</v>
       </c>
     </row>
@@ -42499,7 +42502,7 @@
       <c r="F2297" s="0" t="s">
         <v>3188</v>
       </c>
-      <c r="G2297" s="145" t="n">
+      <c r="G2297" s="146" t="n">
         <v>41244</v>
       </c>
     </row>
@@ -42591,7 +42594,7 @@
       <c r="B2307" s="0" t="s">
         <v>3202</v>
       </c>
-      <c r="C2307" s="143" t="n">
+      <c r="C2307" s="144" t="n">
         <v>878236000</v>
       </c>
     </row>
@@ -42677,7 +42680,7 @@
       <c r="B2317" s="0" t="s">
         <v>3218</v>
       </c>
-      <c r="C2317" s="143" t="n">
+      <c r="C2317" s="144" t="n">
         <v>32640100000</v>
       </c>
     </row>
@@ -42685,7 +42688,7 @@
       <c r="B2318" s="0" t="s">
         <v>3219</v>
       </c>
-      <c r="C2318" s="143" t="n">
+      <c r="C2318" s="144" t="n">
         <v>33683000000</v>
       </c>
     </row>
@@ -42701,7 +42704,7 @@
       <c r="B2320" s="0" t="s">
         <v>3221</v>
       </c>
-      <c r="C2320" s="143" t="n">
+      <c r="C2320" s="144" t="n">
         <v>30883800</v>
       </c>
     </row>
@@ -42749,7 +42752,7 @@
       <c r="C2326" s="0" t="s">
         <v>3229</v>
       </c>
-      <c r="D2326" s="146" t="n">
+      <c r="D2326" s="147" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>
@@ -42800,7 +42803,7 @@
       <c r="C2332" s="0" t="s">
         <v>3237</v>
       </c>
-      <c r="D2332" s="146" t="n">
+      <c r="D2332" s="147" t="n">
         <v>0.600474537037037</v>
       </c>
     </row>
@@ -42819,7 +42822,7 @@
       <c r="D2334" s="0" t="s">
         <v>3240</v>
       </c>
-      <c r="E2334" s="146" t="n">
+      <c r="E2334" s="147" t="n">
         <v>0.157314814814815</v>
       </c>
     </row>
@@ -42877,7 +42880,7 @@
       <c r="E2339" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="F2339" s="146" t="n">
+      <c r="F2339" s="147" t="n">
         <v>0.596990740740741</v>
       </c>
     </row>
@@ -43349,7 +43352,7 @@
       <c r="E2380" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="F2380" s="146" t="n">
+      <c r="F2380" s="147" t="n">
         <v>0.443159722222222</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cadashboard for maintenance time
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11787,14 +11787,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="F32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
-      <selection pane="bottomRight" activeCell="I58" activeCellId="0" sqref="I58"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
+      <selection pane="bottomRight" activeCell="I55" activeCellId="0" sqref="I55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -14763,7 +14763,7 @@
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="57" t="n">
-        <v>-22.758</v>
+        <v>-22.97</v>
       </c>
       <c r="J54" s="28" t="n">
         <v>-263394</v>
@@ -16998,7 +16998,7 @@
       </c>
       <c r="F26" s="104" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.758</v>
+        <v>-22.97</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="83" t="s">
@@ -17132,7 +17132,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17314,7 +17314,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17639,7 +17639,7 @@
       </c>
       <c r="F22" s="139" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.758</v>
+        <v>-22.97</v>
       </c>
       <c r="G22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
@@ -17888,7 +17888,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23959,7 +23959,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>

<commit_message>
cadashboard improvements, refine Modes lookup table
</commit_message>
<xml_diff>
--- a/Modes.xlsx
+++ b/Modes.xlsx
@@ -11787,14 +11787,14 @@
   <dimension ref="A1:AMJ66"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="4" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="E33" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
-      <selection pane="bottomRight" activeCell="I55" activeCellId="0" sqref="I55"/>
+      <selection pane="bottomLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="bottomRight" activeCell="K57" activeCellId="0" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.04"/>
@@ -13835,46 +13835,46 @@
         <v>135</v>
       </c>
       <c r="E40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="F40" s="0" t="n">
-        <v>-13926</v>
+        <v>2679</v>
       </c>
       <c r="G40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="H40" s="0" t="n">
-        <v>-13926</v>
+        <v>2679</v>
       </c>
       <c r="I40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>-13926</v>
+        <v>2679</v>
       </c>
       <c r="K40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="L40" s="0" t="n">
-        <v>-13926</v>
+        <v>2679</v>
       </c>
       <c r="M40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="N40" s="0" t="n">
-        <v>-13926</v>
+        <v>2679</v>
       </c>
       <c r="O40" s="33" t="n">
-        <v>-0.1735</v>
+        <v>0</v>
       </c>
       <c r="P40" s="0" t="n">
-        <v>-13926</v>
-      </c>
-      <c r="T40" s="30" t="n">
-        <v>-0.16105</v>
-      </c>
-      <c r="U40" s="32" t="n">
-        <v>-13803</v>
+        <v>2679</v>
+      </c>
+      <c r="T40" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" s="0" t="n">
+        <v>2679</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13889,46 +13889,46 @@
         <v>138</v>
       </c>
       <c r="E41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="F41" s="0" t="n">
-        <v>-25564</v>
+        <v>-10199</v>
       </c>
       <c r="G41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="H41" s="0" t="n">
-        <v>-25564</v>
+        <v>-10199</v>
       </c>
       <c r="I41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>-25564</v>
+        <v>-10199</v>
       </c>
       <c r="K41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="L41" s="0" t="n">
-        <v>-25564</v>
+        <v>-10199</v>
       </c>
       <c r="M41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="N41" s="0" t="n">
-        <v>-25564</v>
+        <v>-10199</v>
       </c>
       <c r="O41" s="33" t="n">
-        <v>0.1936</v>
+        <v>0</v>
       </c>
       <c r="P41" s="0" t="n">
-        <v>-25564</v>
-      </c>
-      <c r="T41" s="30" t="n">
-        <v>0.16105</v>
-      </c>
-      <c r="U41" s="32" t="n">
-        <v>-25895</v>
+        <v>-10199</v>
+      </c>
+      <c r="T41" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" s="0" t="n">
+        <v>-10199</v>
       </c>
     </row>
     <row r="42" s="35" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14753,38 +14753,38 @@
         <v>181</v>
       </c>
       <c r="E54" s="57" t="n">
-        <v>30.857</v>
+        <v>31.259</v>
       </c>
       <c r="F54" s="26" t="n">
-        <v>272755</v>
+        <v>276763</v>
       </c>
       <c r="G54" s="58" t="n">
         <v>-55.188</v>
       </c>
       <c r="H54" s="59"/>
       <c r="I54" s="57" t="n">
-        <v>-22.97</v>
+        <v>-22.744</v>
       </c>
       <c r="J54" s="28" t="n">
-        <v>-263394</v>
+        <v>-263256</v>
       </c>
       <c r="K54" s="60" t="n">
-        <v>43.326</v>
+        <v>43.506</v>
       </c>
       <c r="L54" s="28" t="n">
-        <v>397443</v>
+        <v>399229</v>
       </c>
       <c r="M54" s="60" t="n">
-        <v>43.326</v>
+        <v>43.749</v>
       </c>
       <c r="N54" s="28" t="n">
-        <v>397443</v>
+        <v>401650</v>
       </c>
       <c r="O54" s="57" t="n">
-        <v>17.437</v>
+        <v>17.735</v>
       </c>
       <c r="P54" s="28" t="n">
-        <v>138533</v>
+        <v>141529</v>
       </c>
       <c r="T54" s="58" t="n">
         <v>53.33</v>
@@ -14914,25 +14914,25 @@
         <v>4600216</v>
       </c>
       <c r="I56" s="61" t="n">
-        <v>54.22</v>
+        <v>54.559</v>
       </c>
       <c r="J56" s="23" t="n">
         <v>6151303</v>
       </c>
       <c r="K56" s="61" t="n">
-        <v>126.254</v>
+        <v>125.596</v>
       </c>
       <c r="L56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="M56" s="61" t="n">
-        <v>126.254</v>
+        <v>126.051</v>
       </c>
       <c r="N56" s="23" t="n">
         <v>9901395</v>
       </c>
       <c r="O56" s="61" t="n">
-        <v>97.298</v>
+        <v>97.709</v>
       </c>
       <c r="P56" s="23" t="n">
         <v>8392750</v>
@@ -14976,25 +14976,25 @@
         <v>1551088</v>
       </c>
       <c r="I57" s="64" t="n">
-        <v>47.419</v>
+        <v>47.758</v>
       </c>
       <c r="J57" s="32" t="n">
         <v>3351899</v>
       </c>
       <c r="K57" s="64" t="n">
-        <v>129.699</v>
+        <v>129.041</v>
       </c>
       <c r="L57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="M57" s="64" t="n">
-        <v>129.699</v>
+        <v>129.496</v>
       </c>
       <c r="N57" s="32" t="n">
         <v>7552437</v>
       </c>
       <c r="O57" s="64" t="n">
-        <v>95.993</v>
+        <v>96.404</v>
       </c>
       <c r="P57" s="32" t="n">
         <v>5879304</v>
@@ -15030,25 +15030,25 @@
         <v>354340</v>
       </c>
       <c r="I58" s="64" t="n">
-        <v>47.419</v>
+        <v>47.758</v>
       </c>
       <c r="J58" s="32" t="n">
         <v>1952224</v>
       </c>
       <c r="K58" s="64" t="n">
-        <v>129.699</v>
+        <v>129.041</v>
       </c>
       <c r="L58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="M58" s="64" t="n">
-        <v>129.699</v>
+        <v>129.496</v>
       </c>
       <c r="N58" s="32" t="n">
         <v>6355689</v>
       </c>
       <c r="O58" s="64" t="n">
-        <v>95.993</v>
+        <v>96.404</v>
       </c>
       <c r="P58" s="67" t="n">
         <v>4479629</v>
@@ -16952,7 +16952,7 @@
       </c>
       <c r="F24" s="104" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>30.857</v>
+        <v>31.259</v>
       </c>
       <c r="G24" s="0"/>
       <c r="H24" s="83" t="s">
@@ -16998,7 +16998,7 @@
       </c>
       <c r="F26" s="104" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.97</v>
+        <v>-22.744</v>
       </c>
       <c r="G26" s="0"/>
       <c r="H26" s="83" t="s">
@@ -17021,7 +17021,7 @@
       </c>
       <c r="F27" s="104" t="n">
         <f aca="false">'Modes A-F'!K54</f>
-        <v>43.326</v>
+        <v>43.506</v>
       </c>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
@@ -17040,7 +17040,7 @@
       </c>
       <c r="F28" s="104" t="n">
         <f aca="false">'Modes A-F'!M54</f>
-        <v>43.326</v>
+        <v>43.749</v>
       </c>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
@@ -17059,7 +17059,7 @@
       </c>
       <c r="F29" s="104" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>17.437</v>
+        <v>17.735</v>
       </c>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
@@ -17132,7 +17132,7 @@
       <selection pane="bottomRight" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33"/>
@@ -17314,7 +17314,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.36"/>
@@ -17373,11 +17373,11 @@
       </c>
       <c r="G3" s="122" t="n">
         <f aca="false">'Modes A-F'!O54</f>
-        <v>17.437</v>
+        <v>17.735</v>
       </c>
       <c r="H3" s="123" t="n">
         <f aca="false">G3-F3</f>
-        <v>-1.6661189817083</v>
+        <v>-1.3681189817083</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17393,19 +17393,19 @@
       </c>
       <c r="E4" s="104" t="n">
         <f aca="false">'Modes A-F'!K56</f>
-        <v>126.254</v>
+        <v>125.596</v>
       </c>
       <c r="F4" s="104" t="n">
         <f aca="false">E4-B4*TAN(2*(F2-E2)/1000)</f>
-        <v>97.3429132666878</v>
+        <v>96.6849132666878</v>
       </c>
       <c r="G4" s="122" t="n">
         <f aca="false">'Modes A-F'!O56</f>
-        <v>97.298</v>
+        <v>97.709</v>
       </c>
       <c r="H4" s="123" t="n">
         <f aca="false">G4-F4</f>
-        <v>-0.0449132666877574</v>
+        <v>1.02408673331225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17422,25 +17422,25 @@
       </c>
       <c r="E5" s="127" t="n">
         <f aca="false">'Modes A-F'!K57</f>
-        <v>129.699</v>
+        <v>129.041</v>
       </c>
       <c r="F5" s="127" t="n">
         <f aca="false">E5-B5*TAN(2*(F2-E2)/1000)</f>
-        <v>97.3229028716503</v>
+        <v>96.6649028716503</v>
       </c>
       <c r="G5" s="128" t="n">
         <f aca="false">'Modes A-F'!O57</f>
-        <v>95.993</v>
+        <v>96.404</v>
       </c>
       <c r="H5" s="123" t="n">
         <f aca="false">G5-F5</f>
-        <v>-1.32990287165035</v>
+        <v>-0.26090287165033</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="123" t="n">
         <f aca="false">AVERAGE(H3,H4,H5)</f>
-        <v>-1.01364504001547</v>
+        <v>-0.201645040015462</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>273</v>
@@ -17486,12 +17486,12 @@
       </c>
       <c r="E10" s="123" t="n">
         <f aca="false">'Modes A-F'!E54</f>
-        <v>30.857</v>
+        <v>31.259</v>
       </c>
       <c r="F10" s="123"/>
       <c r="G10" s="132" t="n">
         <f aca="false">E10-B10*TAN(2*(G9-E9)/1000)</f>
-        <v>33.0384000290853</v>
+        <v>33.4404000290853</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17635,15 +17635,15 @@
       </c>
       <c r="E22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(E19)/1000)+I17</f>
-        <v>-37.1093914229833</v>
+        <v>-36.7073914229833</v>
       </c>
       <c r="F22" s="139" t="n">
         <f aca="false">'Modes A-F'!I54</f>
-        <v>-22.97</v>
+        <v>-22.744</v>
       </c>
       <c r="G22" s="123" t="n">
         <f aca="false">E10-B22*TAN(2*(G19)/1000)+I17</f>
-        <v>-32.15802924884</v>
+        <v>-31.75602924884</v>
       </c>
       <c r="I22" s="119"/>
     </row>
@@ -17664,7 +17664,7 @@
       </c>
       <c r="F23" s="139" t="n">
         <f aca="false">'Modes A-F'!I56</f>
-        <v>54.22</v>
+        <v>54.559</v>
       </c>
       <c r="G23" s="123" t="n">
         <f aca="false">E11-B23*TAN(2*(G19)/1000)+I17</f>
@@ -17690,7 +17690,7 @@
       </c>
       <c r="F24" s="140" t="n">
         <f aca="false">'Modes A-F'!I57</f>
-        <v>47.419</v>
+        <v>47.758</v>
       </c>
       <c r="G24" s="141" t="n">
         <f aca="false">E12-B24*TAN(2*(G19)/1000)+I17</f>
@@ -17797,7 +17797,7 @@
       </c>
       <c r="E34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(E31)/1000)</f>
-        <v>-64.1176236638297</v>
+        <v>-63.7156236638297</v>
       </c>
       <c r="F34" s="139" t="n">
         <f aca="false">'Modes A-F'!G54</f>
@@ -17805,7 +17805,7 @@
       </c>
       <c r="G34" s="123" t="n">
         <f aca="false">E10-B34*TAN(2*(G31)/1000)+I29</f>
-        <v>-59.1660007866982</v>
+        <v>-58.7640007866982</v>
       </c>
       <c r="I34" s="119"/>
     </row>
@@ -17888,7 +17888,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.26"/>
   </cols>
@@ -23959,7 +23959,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.14"/>

</xml_diff>